<commit_message>
update dealer margin tax to 12 percent
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385AC0E8-2D7A-4EC0-9939-4A3D8B48A0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2421DB51-986A-404A-915F-8664C30FF97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -5491,8 +5491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05C9E0-A64E-40AC-B9F4-C919ED5906CC}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5568,16 +5568,16 @@
         <v>444200000</v>
       </c>
       <c r="D2" s="7">
-        <f>VLOOKUP(B2,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>31531531.531531528</v>
+        <f>VLOOKUP(B2,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>31219338.150031216</v>
       </c>
       <c r="E2" s="7">
         <f>D2*90%</f>
-        <v>28378378.378378376</v>
+        <v>28097404.335028097</v>
       </c>
       <c r="F2" s="7">
         <f>D2*70%</f>
-        <v>22072072.072072066</v>
+        <v>21853536.705021851</v>
       </c>
       <c r="G2" s="9">
         <v>228</v>
@@ -5598,16 +5598,16 @@
         <v>385500000</v>
       </c>
       <c r="D3" s="7">
-        <f>VLOOKUP(B3,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>29729729.729729727</v>
+        <f>VLOOKUP(B3,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>29435375.970029432</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" ref="E3:E32" si="0">D3*90%</f>
-        <v>26756756.756756756</v>
+        <v>26491838.37302649</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" ref="F3:F32" si="1">D3*70%</f>
-        <v>20810810.810810808</v>
+        <v>20604763.179020602</v>
       </c>
       <c r="G3" s="9">
         <v>227</v>
@@ -5628,16 +5628,16 @@
         <v>308500000</v>
       </c>
       <c r="D4" s="7">
-        <f>VLOOKUP(B4,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>20945945.945945945</v>
+        <f>VLOOKUP(B4,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>20738560.342520736</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="0"/>
-        <v>18851351.351351351</v>
+        <v>18664704.308268663</v>
       </c>
       <c r="F4" s="7">
         <f t="shared" si="1"/>
-        <v>14662162.162162161</v>
+        <v>14516992.239764515</v>
       </c>
       <c r="G4" s="9">
         <v>222</v>
@@ -5658,16 +5658,16 @@
         <v>326050000</v>
       </c>
       <c r="D5" s="7">
-        <f>VLOOKUP(B5,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>22252252.252252247</v>
+        <f>VLOOKUP(B5,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>22031932.923022028</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>20027027.027027022</v>
+        <v>19828739.630719826</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="1"/>
-        <v>15576576.576576572</v>
+        <v>15422353.046115419</v>
       </c>
       <c r="G5" s="9">
         <v>223</v>
@@ -5688,16 +5688,16 @@
         <v>402000000</v>
       </c>
       <c r="D6" s="7">
-        <f>VLOOKUP(B6,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>31531531.531531528</v>
+        <f>VLOOKUP(B6,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>31219338.150031216</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="0"/>
-        <v>28378378.378378376</v>
+        <v>28097404.335028097</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="1"/>
-        <v>22072072.072072066</v>
+        <v>21853536.705021851</v>
       </c>
       <c r="G6" s="9">
         <v>244</v>
@@ -5718,16 +5718,16 @@
         <v>442000000</v>
       </c>
       <c r="D7" s="7">
-        <f>VLOOKUP(B7,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>34234234.234234229</v>
+        <f>VLOOKUP(B7,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>33895281.420033887</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
-        <v>30810810.810810808</v>
+        <v>30505753.2780305</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="1"/>
-        <v>23963963.963963959</v>
+        <v>23726696.994023718</v>
       </c>
       <c r="G7" s="9">
         <v>245</v>
@@ -5749,16 +5749,16 @@
         <v>300000000</v>
       </c>
       <c r="D8" s="7">
-        <f>VLOOKUP(B8,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>20720720.720720716</v>
+        <f>VLOOKUP(B8,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>20515565.070020512</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
-        <v>18648648.648648646</v>
+        <v>18464008.56301846</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>14504504.5045045</v>
+        <v>14360895.549014358</v>
       </c>
       <c r="G8" s="4">
         <v>240</v>
@@ -5779,16 +5779,16 @@
         <v>260000000</v>
       </c>
       <c r="D9" s="7">
-        <f>VLOOKUP(B9,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>18018018.018018018</v>
+        <f>VLOOKUP(B9,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>17839621.800017841</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="0"/>
-        <v>16216216.216216218</v>
+        <v>16055659.620016057</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>12612612.612612613</v>
+        <v>12487735.260012489</v>
       </c>
       <c r="G9" s="4">
         <v>241</v>
@@ -5810,16 +5810,16 @@
         <v>214000000</v>
       </c>
       <c r="D10" s="7">
-        <f>VLOOKUP(B10,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>11711711.71171171</v>
+        <f>VLOOKUP(B10,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>11595754.170011595</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>10540540.540540539</v>
+        <v>10436178.753010435</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="1"/>
-        <v>8198198.1981981965</v>
+        <v>8117027.9190081162</v>
       </c>
       <c r="G10" s="4">
         <v>242</v>
@@ -5841,16 +5841,16 @@
         <v>185300000</v>
       </c>
       <c r="D11" s="7">
-        <f>VLOOKUP(B11,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>11441441.441441441</v>
+        <f>VLOOKUP(B11,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>11328159.843011327</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
-        <v>10297297.297297297</v>
+        <v>10195343.858710194</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="1"/>
-        <v>8009009.0090090083</v>
+        <v>7929711.8901079288</v>
       </c>
       <c r="G11" s="4">
         <v>202</v>
@@ -5872,16 +5872,16 @@
         <v>222850000</v>
       </c>
       <c r="D12" s="7">
-        <f>VLOOKUP(B12,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>14414414.414414413</v>
+        <f>VLOOKUP(B12,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>14271697.440014271</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
-        <v>12972972.972972972</v>
+        <v>12844527.696012843</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="1"/>
-        <v>10090090.090090089</v>
+        <v>9990188.2080099899</v>
       </c>
       <c r="G12" s="4">
         <v>204</v>
@@ -5903,16 +5903,16 @@
         <v>207700000</v>
       </c>
       <c r="D13" s="7">
-        <f>VLOOKUP(B13,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>13243243.243243242</v>
+        <f>VLOOKUP(B13,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>13112122.023013111</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="0"/>
-        <v>11918918.918918917</v>
+        <v>11800909.820711801</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="1"/>
-        <v>9270270.2702702694</v>
+        <v>9178485.4161091764</v>
       </c>
       <c r="G13" s="4">
         <v>205</v>
@@ -5933,16 +5933,16 @@
         <v>274200000</v>
       </c>
       <c r="D14" s="7">
-        <f>VLOOKUP(B14,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>18828828.828828827</v>
+        <f>VLOOKUP(B14,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>18642404.781018641</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
-        <v>16945945.945945945</v>
+        <v>16778164.302916776</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="1"/>
-        <v>13180180.180180177</v>
+        <v>13049683.346713047</v>
       </c>
       <c r="G14" s="4">
         <v>213</v>
@@ -5963,16 +5963,16 @@
         <v>288300000</v>
       </c>
       <c r="D15" s="7">
-        <f>VLOOKUP(B15,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>19819819.819819819</v>
+        <f>VLOOKUP(B15,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>19623583.980019622</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
-        <v>17837837.837837838</v>
+        <v>17661225.58201766</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
-        <v>13873873.873873873</v>
+        <v>13736508.786013734</v>
       </c>
       <c r="G15" s="4">
         <v>214</v>
@@ -5993,16 +5993,16 @@
         <v>259500000</v>
       </c>
       <c r="D16" s="7">
-        <f>VLOOKUP(B16,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>16486486.486486487</v>
+        <f>VLOOKUP(B16,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>16323253.947016323</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
-        <v>14837837.837837839</v>
+        <v>14690928.552314691</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="1"/>
-        <v>11540540.540540541</v>
+        <v>11426277.762911426</v>
       </c>
       <c r="G16" s="4">
         <v>209</v>
@@ -6023,16 +6023,16 @@
         <v>285200000</v>
       </c>
       <c r="D17" s="7">
-        <f>VLOOKUP(B17,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>18468468.468468465</v>
+        <f>VLOOKUP(B17,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>18285612.345018283</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
-        <v>16621621.621621618</v>
+        <v>16457051.110516455</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="1"/>
-        <v>12927927.927927924</v>
+        <v>12799928.641512796</v>
       </c>
       <c r="G17" s="4">
         <v>220</v>
@@ -6053,16 +6053,16 @@
         <v>209000000</v>
       </c>
       <c r="D18" s="7">
-        <f>VLOOKUP(B18,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>18918918.918918915</v>
+        <f>VLOOKUP(B18,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>18731602.890018728</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
-        <v>17027027.027027026</v>
+        <v>16858442.601016857</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>13243243.24324324</v>
+        <v>13112122.023013109</v>
       </c>
       <c r="G18" s="4">
         <v>221</v>
@@ -6083,16 +6083,16 @@
         <v>209000000</v>
       </c>
       <c r="D19" s="7">
-        <f>VLOOKUP(B19,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>18918918.918918915</v>
+        <f>VLOOKUP(B19,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>18731602.890018728</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" ref="E19" si="2">D19*90%</f>
-        <v>17027027.027027026</v>
+        <v>16858442.601016857</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" ref="F19" si="3">D19*70%</f>
-        <v>13243243.24324324</v>
+        <v>13112122.023013109</v>
       </c>
       <c r="G19" s="4">
         <v>221</v>
@@ -6112,16 +6112,16 @@
         <v>209000000</v>
       </c>
       <c r="D20" s="7">
-        <f>VLOOKUP(B20,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>18918918.918918915</v>
+        <f>VLOOKUP(B20,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>18731602.890018728</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
-        <v>17027027.027027026</v>
+        <v>16858442.601016857</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="1"/>
-        <v>13243243.24324324</v>
+        <v>13112122.023013109</v>
       </c>
       <c r="G20" s="4">
         <v>243</v>
@@ -6142,16 +6142,16 @@
         <v>246000000</v>
       </c>
       <c r="D21" s="7">
-        <f>VLOOKUP(B21,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>18918918.918918915</v>
+        <f>VLOOKUP(B21,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>18731602.890018728</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" si="0"/>
-        <v>17027027.027027026</v>
+        <v>16858442.601016857</v>
       </c>
       <c r="F21" s="7">
         <f t="shared" si="1"/>
-        <v>13243243.24324324</v>
+        <v>13112122.023013109</v>
       </c>
       <c r="G21" s="4">
         <v>250</v>
@@ -6172,16 +6172,16 @@
         <v>302500000</v>
       </c>
       <c r="D22" s="7">
-        <f>VLOOKUP(B22,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>22522522.522522524</v>
+        <f>VLOOKUP(B22,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>22299527.2500223</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
-        <v>20270270.270270273</v>
+        <v>20069574.52502007</v>
       </c>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>15765765.765765766</v>
+        <v>15609669.075015608</v>
       </c>
       <c r="G22" s="4">
         <v>235</v>
@@ -6202,16 +6202,16 @@
         <v>348000000</v>
       </c>
       <c r="D23" s="7">
-        <f>VLOOKUP(B23,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>26126126.126126125</v>
+        <f>VLOOKUP(B23,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>25867451.610025868</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>23513513.513513513</v>
+        <v>23280706.44902328</v>
       </c>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>18288288.288288288</v>
+        <v>18107216.127018105</v>
       </c>
       <c r="G23" s="4">
         <v>246</v>
@@ -6232,16 +6232,16 @@
         <v>358000000</v>
       </c>
       <c r="D24" s="7">
-        <f>VLOOKUP(B24,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>27027027.027027022</v>
+        <f>VLOOKUP(B24,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>26759432.700026754</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
-        <v>24324324.324324321</v>
+        <v>24083489.43002408</v>
       </c>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>18918918.918918915</v>
+        <v>18731602.890018728</v>
       </c>
       <c r="G24" s="4">
         <v>247</v>
@@ -6262,16 +6262,16 @@
         <v>408000000</v>
       </c>
       <c r="D25" s="7">
-        <f>VLOOKUP(B25,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>30630630.630630627</v>
+        <f>VLOOKUP(B25,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>30327357.060030323</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" si="0"/>
-        <v>27567567.567567565</v>
+        <v>27294621.35402729</v>
       </c>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>21441441.441441439</v>
+        <v>21229149.942021225</v>
       </c>
       <c r="G25" s="4">
         <v>248</v>
@@ -6292,16 +6292,16 @@
         <v>415000000</v>
       </c>
       <c r="D26" s="7">
-        <f>VLOOKUP(B26,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>33333333.333333328</v>
+        <f>VLOOKUP(B26,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>33003300.330032997</v>
       </c>
       <c r="E26" s="7">
         <f t="shared" si="0"/>
-        <v>29999999.999999996</v>
+        <v>29702970.297029696</v>
       </c>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>23333333.333333328</v>
+        <v>23102310.231023096</v>
       </c>
       <c r="G26" s="4">
         <v>251</v>
@@ -6322,16 +6322,16 @@
         <v>438000000</v>
       </c>
       <c r="D27" s="7">
-        <f>VLOOKUP(B27,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>33333333.333333328</v>
+        <f>VLOOKUP(B27,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>33003300.330032997</v>
       </c>
       <c r="E27" s="7">
         <f t="shared" ref="E27" si="4">D27*90%</f>
-        <v>29999999.999999996</v>
+        <v>29702970.297029696</v>
       </c>
       <c r="F27" s="7">
         <f t="shared" ref="F27" si="5">D27*70%</f>
-        <v>23333333.333333328</v>
+        <v>23102310.231023096</v>
       </c>
       <c r="G27" s="4">
         <v>249</v>
@@ -6352,16 +6352,16 @@
         <v>438000000</v>
       </c>
       <c r="D28" s="7">
-        <f>VLOOKUP(B28,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>33333333.333333328</v>
+        <f>VLOOKUP(B28,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>33003300.330032997</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>29999999.999999996</v>
+        <v>29702970.297029696</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>23333333.333333328</v>
+        <v>23102310.231023096</v>
       </c>
       <c r="G28" s="4">
         <v>249</v>
@@ -6382,16 +6382,16 @@
         <v>152700000</v>
       </c>
       <c r="D29" s="7">
-        <f>VLOOKUP(B29,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>10990990.990990989</v>
+        <f>VLOOKUP(B29,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>10882169.29801088</v>
       </c>
       <c r="E29" s="7">
         <f t="shared" si="0"/>
-        <v>9891891.8918918911</v>
+        <v>9793952.3682097923</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>7693693.6936936919</v>
+        <v>7617518.5086076157</v>
       </c>
       <c r="G29" s="4">
         <v>201</v>
@@ -6412,16 +6412,16 @@
         <v>169600000</v>
       </c>
       <c r="D30" s="7">
-        <f>VLOOKUP(B30,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>7207207.2072072066</v>
+        <f>VLOOKUP(B30,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>7135848.7200071355</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="0"/>
-        <v>6486486.4864864862</v>
+        <v>6422263.8480064217</v>
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>5045045.0450450443</v>
+        <v>4995094.104004995</v>
       </c>
       <c r="G30" s="4">
         <v>230</v>
@@ -6442,16 +6442,16 @@
         <v>173000000</v>
       </c>
       <c r="D31" s="7">
-        <f>VLOOKUP(B31,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>12162162.162162162</v>
+        <f>VLOOKUP(B31,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>12041744.715012042</v>
       </c>
       <c r="E31" s="7">
         <f t="shared" si="0"/>
-        <v>10945945.945945946</v>
+        <v>10837570.243510839</v>
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>8513513.5135135129</v>
+        <v>8429221.3005084284</v>
       </c>
       <c r="G31" s="4">
         <v>238</v>
@@ -6472,16 +6472,16 @@
         <v>165000000</v>
       </c>
       <c r="D32" s="7">
-        <f>VLOOKUP(B32,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>11261261.261261262</v>
+        <f>VLOOKUP(B32,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>11149763.62501115</v>
       </c>
       <c r="E32" s="7">
         <f t="shared" si="0"/>
-        <v>10135135.135135137</v>
+        <v>10034787.262510035</v>
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>7882882.8828828828</v>
+        <v>7804834.5375078041</v>
       </c>
       <c r="G32" s="4">
         <v>237</v>
@@ -6502,16 +6502,16 @@
         <v>185300000</v>
       </c>
       <c r="D33" s="7">
-        <f>VLOOKUP(B33,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>11441441.441441441</v>
+        <f>VLOOKUP(B33,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>11328159.843011327</v>
       </c>
       <c r="E33" s="7">
         <f t="shared" ref="E33:E34" si="6">D33*90%</f>
-        <v>10297297.297297297</v>
+        <v>10195343.858710194</v>
       </c>
       <c r="F33" s="7">
         <f t="shared" ref="F33:F34" si="7">D33*70%</f>
-        <v>8009009.0090090083</v>
+        <v>7929711.8901079288</v>
       </c>
       <c r="G33" s="4">
         <v>202</v>
@@ -6532,16 +6532,16 @@
         <v>438000000</v>
       </c>
       <c r="D34" s="7">
-        <f>VLOOKUP(B34,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>33333333.333333328</v>
+        <f>VLOOKUP(B34,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>33003300.330032997</v>
       </c>
       <c r="E34" s="7">
         <f t="shared" si="6"/>
-        <v>29999999.999999996</v>
+        <v>29702970.297029696</v>
       </c>
       <c r="F34" s="7">
         <f t="shared" si="7"/>
-        <v>23333333.333333328</v>
+        <v>23102310.231023096</v>
       </c>
       <c r="G34" s="4">
         <v>249</v>
@@ -6562,16 +6562,16 @@
         <v>342650000</v>
       </c>
       <c r="D35" s="7">
-        <f>VLOOKUP(B35,[2]pricelist!$B$3:$H$53,7,0)*1000</f>
-        <v>23063063.063063063</v>
+        <f>VLOOKUP(B35,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>22834715.904022835</v>
       </c>
       <c r="E35" s="7">
         <f t="shared" ref="E35" si="8">D35*90%</f>
-        <v>20756756.756756756</v>
+        <v>20551244.313620552</v>
       </c>
       <c r="F35" s="7">
         <f t="shared" ref="F35" si="9">D35*70%</f>
-        <v>16144144.144144142</v>
+        <v>15984301.132815983</v>
       </c>
       <c r="G35" s="4">
         <v>233</v>

</xml_diff>

<commit_message>
update data as of 3 July 2025
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2421DB51-986A-404A-915F-8664C30FF97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35DD9C8-04D4-407D-BE2F-398399ABDC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -28,7 +28,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="3" hidden="1">Confero!$A$1:$H$16</definedName>
@@ -491,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="583">
   <si>
     <t>Column1</t>
   </si>
@@ -2317,6 +2316,9 @@
   </si>
   <si>
     <t>CLOUD EV LITE</t>
+  </si>
+  <si>
+    <t>EQ100460LV1CCS2</t>
   </si>
 </sst>
 </file>
@@ -2889,455 +2891,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sales 2025"/>
-      <sheetName val="Sales Plan 2025"/>
-      <sheetName val="subsidi discount"/>
-      <sheetName val="pricelist"/>
-      <sheetName val="ASS"/>
-      <sheetName val="TOTAL"/>
-      <sheetName val="CIBUBUR"/>
-      <sheetName val="CIKUPA"/>
-      <sheetName val="DM"/>
-      <sheetName val="FTM"/>
-      <sheetName val="KBJ"/>
-      <sheetName val="HARMONI"/>
-      <sheetName val="SPG"/>
-      <sheetName val="TAJUR"/>
-      <sheetName val="KPG"/>
-      <sheetName val="GRESIK"/>
-      <sheetName val="MJKT"/>
-      <sheetName val="MADIUN"/>
-      <sheetName val="SBY"/>
-      <sheetName val="Fleet"/>
-      <sheetName val="HO"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Air Ev Lite</v>
-          </cell>
-          <cell r="C3">
-            <v>209000000</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v xml:space="preserve">Air Ev Lite 300 km </v>
-          </cell>
-          <cell r="C4">
-            <v>246000000</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Air Ev LV 1</v>
-          </cell>
-          <cell r="C5">
-            <v>246000000</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>Air Ev LV 2</v>
-          </cell>
-          <cell r="C6">
-            <v>302500000</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Almaz (1A RS EX 7 SEAT)</v>
-          </cell>
-          <cell r="C7">
-            <v>385500000</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>Almaz 1.5 S+ T CVT (Smart Enjoy CVT)</v>
-          </cell>
-          <cell r="C8">
-            <v>326050000</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>Almaz 1.5 S+ T MT (Smart Enjoy MT)</v>
-          </cell>
-          <cell r="C9">
-            <v>308500000</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Almaz 1.5L T Lux CVT (4x2) A/T</v>
-          </cell>
-          <cell r="C10">
-            <v>380100000</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Almaz 1.5LT LUX + SC CVT 2A(RS PRO)</v>
-          </cell>
-          <cell r="C11">
-            <v>444200000</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12" t="str">
-            <v>Almaz 1.5LT LUX CVT 1A 4x2 A/T Adas</v>
-          </cell>
-          <cell r="C12">
-            <v>373500000</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Almaz 1.5LT Lux+ SC CVT (4x2) A/T (Exclusive 7 SEAT)</v>
-          </cell>
-          <cell r="C13">
-            <v>390800000</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>Almaz RS 2.0 DHT LV3 7P2A 4X2 A/T (RS HYBRID)</v>
-          </cell>
-          <cell r="C14">
-            <v>476000000</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>Alvez (EX)- 5P2A</v>
-          </cell>
-          <cell r="C15">
-            <v>300000000</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>Alvez 1.5 CE 4X2 CVT</v>
-          </cell>
-          <cell r="C16">
-            <v>260000000</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>Alvez 1.5 SE 4X2 MT</v>
-          </cell>
-          <cell r="C17">
-            <v>214000000</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18" t="str">
-            <v>Binguo 330 km</v>
-          </cell>
-          <cell r="C18">
-            <v>348000000</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v>Binguo 410 km</v>
-          </cell>
-          <cell r="C19">
-            <v>358000000</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v>Binguo Premium Range AC+DC</v>
-          </cell>
-          <cell r="C20">
-            <v>408000000</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v>Cloud Ev</v>
-          </cell>
-          <cell r="C21">
-            <v>438000000</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>Confero DB</v>
-          </cell>
-          <cell r="C22">
-            <v>185300000</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v>Confero S (L LUX+MT)-1,5L 7P</v>
-          </cell>
-          <cell r="C23">
-            <v>222850000</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24" t="str">
-            <v>Confero S 1. 5C MY Lux+ (4x2) MT (*)</v>
-          </cell>
-          <cell r="C24">
-            <v>210800000</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v>Confero S 1.5C LUX MT</v>
-          </cell>
-          <cell r="C25">
-            <v>207700000</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v>Confero S 1.5L AC LUX+MT</v>
-          </cell>
-          <cell r="C26">
-            <v>232300000</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v>Confero S1.5L LUX MT*</v>
-          </cell>
-          <cell r="C27">
-            <v>220800000</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>Cortez (NEW CORTEZ EX LUX+CVT) LT +CVT</v>
-          </cell>
-          <cell r="C28">
-            <v>342650000</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29" t="str">
-            <v>Cortez 1.5 S T LUX + CVT (Leather Seat)</v>
-          </cell>
-          <cell r="C29">
-            <v>285200000</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v>Cortez 1.5 S T LUX CVT* (Leather Seat)</v>
-          </cell>
-          <cell r="C30">
-            <v>281100000</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31" t="str">
-            <v>Cortez 1.5 S T MT</v>
-          </cell>
-          <cell r="C31">
-            <v>259500000</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32" t="str">
-            <v>Cortez 1.5C T (4x2) 6 M/T</v>
-          </cell>
-          <cell r="C32">
-            <v>274200000</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33" t="str">
-            <v>Cortez 1.5C T (4x2) 6 M/T (*)</v>
-          </cell>
-          <cell r="C33">
-            <v>278300000</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>Cortez 1.5C T Lux CVT (4x2) A/T (*)</v>
-          </cell>
-          <cell r="C34">
-            <v>288300000</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35" t="str">
-            <v>Cortez 1.5C T Lux+ CVT (4x2) A/T</v>
-          </cell>
-          <cell r="C35">
-            <v>292300000</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36" t="str">
-            <v>Cortez 1.5L T Lux CVT</v>
-          </cell>
-          <cell r="C36">
-            <v>338650000</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37" t="str">
-            <v>Cortez 1.5L T Lux CVT (4x2) A/T</v>
-          </cell>
-          <cell r="C37">
-            <v>330650000</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38" t="str">
-            <v>Cortez 1.5L T Lux CVT (4x2) A/T (*)</v>
-          </cell>
-          <cell r="C38">
-            <v>326650000</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39" t="str">
-            <v>Cortez 1.5S T CVT (4x2) A/T (*)</v>
-          </cell>
-          <cell r="C39">
-            <v>277100000</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40" t="str">
-            <v>Cortez 1.5S+ T (4x2) 6 M/T (*)</v>
-          </cell>
-          <cell r="C40">
-            <v>263500000</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41" t="str">
-            <v>Formo Max PU 1.5MT NON AC</v>
-          </cell>
-          <cell r="C41">
-            <v>165000000</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42" t="str">
-            <v>Formo Max PU MT AC - LV0A MT</v>
-          </cell>
-          <cell r="C42">
-            <v>173000000</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43" t="str">
-            <v>Formo MB 1.2MT 5 Seat</v>
-          </cell>
-          <cell r="C43">
-            <v>164800000</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44" t="str">
-            <v>Formo MB 1.2MT 8 Seat</v>
-          </cell>
-          <cell r="C44">
-            <v>169600000</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45" t="str">
-            <v>Formo S / BV</v>
-          </cell>
-          <cell r="C45">
-            <v>152700000</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46" t="str">
-            <v>New Almaz RS 1.5T CVT (PRO)</v>
-          </cell>
-          <cell r="C46">
-            <v>402000000</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47" t="str">
-            <v>New Almaz RS 1.5T EX</v>
-          </cell>
-          <cell r="C47">
-            <v>364000000</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48" t="str">
-            <v>New Almaz RS 2.0 DHT 4X2 (RS HYBRID)</v>
-          </cell>
-          <cell r="C48">
-            <v>442000000</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49" t="str">
-            <v>New Almaz Smart Enjoy CVT</v>
-          </cell>
-          <cell r="C49">
-            <v>309000000</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50" t="str">
-            <v>New Cortez CE LUX + CVT</v>
-          </cell>
-          <cell r="C50">
-            <v>304300000</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51" t="str">
-            <v>New Cortez CE LUX CVT*</v>
-          </cell>
-          <cell r="C51">
-            <v>300300000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -5489,10 +5042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05C9E0-A64E-40AC-B9F4-C919ED5906CC}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5564,11 +5117,10 @@
         <v>541</v>
       </c>
       <c r="C2" s="7">
-        <f>VLOOKUP(B2,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>444200000</v>
+        <v>447200000</v>
       </c>
       <c r="D2" s="7">
-        <f>VLOOKUP(B2,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B2,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>31219338.150031216</v>
       </c>
       <c r="E2" s="7">
@@ -5594,11 +5146,10 @@
         <v>548</v>
       </c>
       <c r="C3" s="7">
-        <f>VLOOKUP(B3,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>385500000</v>
+        <v>388500000</v>
       </c>
       <c r="D3" s="7">
-        <f>VLOOKUP(B3,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B3,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>29435375.970029432</v>
       </c>
       <c r="E3" s="7">
@@ -5624,11 +5175,10 @@
         <v>542</v>
       </c>
       <c r="C4" s="7">
-        <f>VLOOKUP(B4,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>308500000</v>
+        <v>311500000</v>
       </c>
       <c r="D4" s="7">
-        <f>VLOOKUP(B4,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B4,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>20738560.342520736</v>
       </c>
       <c r="E4" s="7">
@@ -5654,11 +5204,10 @@
         <v>543</v>
       </c>
       <c r="C5" s="7">
-        <f>VLOOKUP(B5,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>326050000</v>
+        <v>329050000</v>
       </c>
       <c r="D5" s="7">
-        <f>VLOOKUP(B5,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B5,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>22031932.923022028</v>
       </c>
       <c r="E5" s="7">
@@ -5684,11 +5233,10 @@
         <v>530</v>
       </c>
       <c r="C6" s="7">
-        <f>VLOOKUP(B6,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>402000000</v>
+        <v>405000000</v>
       </c>
       <c r="D6" s="7">
-        <f>VLOOKUP(B6,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B6,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>31219338.150031216</v>
       </c>
       <c r="E6" s="7">
@@ -5714,11 +5262,10 @@
         <v>531</v>
       </c>
       <c r="C7" s="7">
-        <f>VLOOKUP(B7,[1]pricelist!$B$3:$C$51,2,0)</f>
         <v>442000000</v>
       </c>
       <c r="D7" s="7">
-        <f>VLOOKUP(B7,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B7,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>33895281.420033887</v>
       </c>
       <c r="E7" s="7">
@@ -5745,11 +5292,10 @@
         <v>532</v>
       </c>
       <c r="C8" s="7">
-        <f>VLOOKUP(B8,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>300000000</v>
+        <v>303000000</v>
       </c>
       <c r="D8" s="7">
-        <f>VLOOKUP(B8,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B8,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>20515565.070020512</v>
       </c>
       <c r="E8" s="7">
@@ -5775,11 +5321,10 @@
         <v>533</v>
       </c>
       <c r="C9" s="7">
-        <f>VLOOKUP(B9,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>260000000</v>
+        <v>263000000</v>
       </c>
       <c r="D9" s="7">
-        <f>VLOOKUP(B9,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B9,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>17839621.800017841</v>
       </c>
       <c r="E9" s="7">
@@ -5806,11 +5351,10 @@
         <v>534</v>
       </c>
       <c r="C10" s="7">
-        <f>VLOOKUP(B10,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>214000000</v>
+        <v>217000000</v>
       </c>
       <c r="D10" s="7">
-        <f>VLOOKUP(B10,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B10,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>11595754.170011595</v>
       </c>
       <c r="E10" s="7">
@@ -5837,11 +5381,10 @@
         <v>535</v>
       </c>
       <c r="C11" s="7">
-        <f>VLOOKUP(B11,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>185300000</v>
+        <v>188300000</v>
       </c>
       <c r="D11" s="7">
-        <f>VLOOKUP(B11,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B11,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>11328159.843011327</v>
       </c>
       <c r="E11" s="7">
@@ -5868,11 +5411,10 @@
         <v>536</v>
       </c>
       <c r="C12" s="7">
-        <f>VLOOKUP(B12,[1]pricelist!$B$3:$C$51,2,0)</f>
         <v>222850000</v>
       </c>
       <c r="D12" s="7">
-        <f>VLOOKUP(B12,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B12,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>14271697.440014271</v>
       </c>
       <c r="E12" s="7">
@@ -5899,11 +5441,10 @@
         <v>537</v>
       </c>
       <c r="C13" s="7">
-        <f>VLOOKUP(B13,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>207700000</v>
+        <v>210700000</v>
       </c>
       <c r="D13" s="7">
-        <f>VLOOKUP(B13,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B13,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>13112122.023013111</v>
       </c>
       <c r="E13" s="7">
@@ -5929,11 +5470,10 @@
         <v>490</v>
       </c>
       <c r="C14" s="7">
-        <f>VLOOKUP(B14,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>274200000</v>
+        <v>277200000</v>
       </c>
       <c r="D14" s="7">
-        <f>VLOOKUP(B14,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B14,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>18642404.781018641</v>
       </c>
       <c r="E14" s="7">
@@ -5959,11 +5499,10 @@
         <v>491</v>
       </c>
       <c r="C15" s="7">
-        <f>VLOOKUP(B15,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>288300000</v>
+        <v>291300000</v>
       </c>
       <c r="D15" s="7">
-        <f>VLOOKUP(B15,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B15,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>19623583.980019622</v>
       </c>
       <c r="E15" s="7">
@@ -5989,11 +5528,10 @@
         <v>544</v>
       </c>
       <c r="C16" s="7">
-        <f>VLOOKUP(B16,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>259500000</v>
+        <v>262500000</v>
       </c>
       <c r="D16" s="7">
-        <f>VLOOKUP(B16,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B16,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>16323253.947016323</v>
       </c>
       <c r="E16" s="7">
@@ -6019,11 +5557,10 @@
         <v>538</v>
       </c>
       <c r="C17" s="7">
-        <f>VLOOKUP(B17,[1]pricelist!$B$3:$C$51,2,0)</f>
         <v>285200000</v>
       </c>
       <c r="D17" s="7">
-        <f>VLOOKUP(B17,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B17,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>18285612.345018283</v>
       </c>
       <c r="E17" s="7">
@@ -6049,11 +5586,10 @@
         <v>507</v>
       </c>
       <c r="C18" s="7">
-        <f>VLOOKUP(B18,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>209000000</v>
+        <v>214000000</v>
       </c>
       <c r="D18" s="7">
-        <f>VLOOKUP(B18,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B18,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>18731602.890018728</v>
       </c>
       <c r="E18" s="7">
@@ -6079,11 +5615,10 @@
         <v>507</v>
       </c>
       <c r="C19" s="7">
-        <f>VLOOKUP(B19,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>209000000</v>
+        <v>251000000</v>
       </c>
       <c r="D19" s="7">
-        <f>VLOOKUP(B19,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B19,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>18731602.890018728</v>
       </c>
       <c r="E19" s="7">
@@ -6109,10 +5644,10 @@
         <v>556</v>
       </c>
       <c r="C20" s="7">
-        <v>209000000</v>
+        <v>251000000</v>
       </c>
       <c r="D20" s="7">
-        <f>VLOOKUP(B20,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B20,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>18731602.890018728</v>
       </c>
       <c r="E20" s="7">
@@ -6138,11 +5673,10 @@
         <v>508</v>
       </c>
       <c r="C21" s="7">
-        <f>VLOOKUP(B21,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>246000000</v>
+        <v>251000000</v>
       </c>
       <c r="D21" s="7">
-        <f>VLOOKUP(B21,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B21,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>18731602.890018728</v>
       </c>
       <c r="E21" s="7">
@@ -6168,11 +5702,10 @@
         <v>509</v>
       </c>
       <c r="C22" s="7">
-        <f>VLOOKUP(B22,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>302500000</v>
+        <v>307500000</v>
       </c>
       <c r="D22" s="7">
-        <f>VLOOKUP(B22,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B22,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>22299527.2500223</v>
       </c>
       <c r="E22" s="7">
@@ -6198,11 +5731,10 @@
         <v>549</v>
       </c>
       <c r="C23" s="7">
-        <f>VLOOKUP(B23,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>348000000</v>
+        <v>353000000</v>
       </c>
       <c r="D23" s="7">
-        <f>VLOOKUP(B23,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B23,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>25867451.610025868</v>
       </c>
       <c r="E23" s="7">
@@ -6228,11 +5760,10 @@
         <v>510</v>
       </c>
       <c r="C24" s="7">
-        <f>VLOOKUP(B24,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>358000000</v>
+        <v>363000000</v>
       </c>
       <c r="D24" s="7">
-        <f>VLOOKUP(B24,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B24,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>26759432.700026754</v>
       </c>
       <c r="E24" s="7">
@@ -6258,11 +5789,10 @@
         <v>511</v>
       </c>
       <c r="C25" s="7">
-        <f>VLOOKUP(B25,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>408000000</v>
+        <v>413000000</v>
       </c>
       <c r="D25" s="7">
-        <f>VLOOKUP(B25,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B25,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>30327357.060030323</v>
       </c>
       <c r="E25" s="7">
@@ -6288,11 +5818,10 @@
         <v>559</v>
       </c>
       <c r="C26" s="7">
-        <f>VLOOKUP(B26,[2]pricelist!$B$3:$C$53,2,0)</f>
         <v>415000000</v>
       </c>
       <c r="D26" s="7">
-        <f>VLOOKUP(B26,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B26,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>33003300.330032997</v>
       </c>
       <c r="E26" s="7">
@@ -6311,18 +5840,17 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
-        <v>558</v>
+      <c r="A27" t="s">
+        <v>582</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>512</v>
+        <v>559</v>
       </c>
       <c r="C27" s="7">
-        <f>VLOOKUP(B27,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>438000000</v>
+        <v>415000000</v>
       </c>
       <c r="D27" s="7">
-        <f>VLOOKUP(B27,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B27,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>33003300.330032997</v>
       </c>
       <c r="E27" s="7">
@@ -6334,33 +5862,32 @@
         <v>23102310.231023096</v>
       </c>
       <c r="G27" s="4">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>506</v>
+        <v>558</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>512</v>
       </c>
       <c r="C28" s="7">
-        <f>VLOOKUP(B28,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>438000000</v>
+        <v>443000000</v>
       </c>
       <c r="D28" s="7">
-        <f>VLOOKUP(B28,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <f>VLOOKUP(B28,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>33003300.330032997</v>
       </c>
       <c r="E28" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E28" si="6">D28*90%</f>
         <v>29702970.297029696</v>
       </c>
       <c r="F28" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F28" si="7">D28*70%</f>
         <v>23102310.231023096</v>
       </c>
       <c r="G28" s="4">
@@ -6372,59 +5899,57 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>529</v>
+        <v>506</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="C29" s="7">
-        <f>VLOOKUP(B29,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>152700000</v>
+        <v>443000000</v>
       </c>
       <c r="D29" s="7">
-        <f>VLOOKUP(B29,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>10882169.29801088</v>
+        <f>VLOOKUP(B29,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>33003300.330032997</v>
       </c>
       <c r="E29" s="7">
-        <f t="shared" si="0"/>
-        <v>9793952.3682097923</v>
+        <f>D29*90%</f>
+        <v>29702970.297029696</v>
       </c>
       <c r="F29" s="7">
-        <f t="shared" si="1"/>
-        <v>7617518.5086076157</v>
+        <f>D29*70%</f>
+        <v>23102310.231023096</v>
       </c>
       <c r="G29" s="4">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>513</v>
+        <v>539</v>
       </c>
       <c r="C30" s="7">
-        <f>VLOOKUP(B30,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>169600000</v>
+        <v>155700000</v>
       </c>
       <c r="D30" s="7">
-        <f>VLOOKUP(B30,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>7135848.7200071355</v>
+        <f>VLOOKUP(B30,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>10882169.29801088</v>
       </c>
       <c r="E30" s="7">
-        <f t="shared" si="0"/>
-        <v>6422263.8480064217</v>
+        <f>D30*90%</f>
+        <v>9793952.3682097923</v>
       </c>
       <c r="F30" s="7">
-        <f t="shared" si="1"/>
-        <v>4995094.104004995</v>
+        <f>D30*70%</f>
+        <v>7617518.5086076157</v>
       </c>
       <c r="G30" s="4">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>572</v>
@@ -6432,59 +5957,57 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>540</v>
+        <v>513</v>
       </c>
       <c r="C31" s="7">
-        <f>VLOOKUP(B31,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>173000000</v>
+        <v>172600000</v>
       </c>
       <c r="D31" s="7">
-        <f>VLOOKUP(B31,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>12041744.715012042</v>
+        <f>VLOOKUP(B31,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>7135848.7200071355</v>
       </c>
       <c r="E31" s="7">
-        <f t="shared" si="0"/>
-        <v>10837570.243510839</v>
+        <f>D31*90%</f>
+        <v>6422263.8480064217</v>
       </c>
       <c r="F31" s="7">
-        <f t="shared" si="1"/>
-        <v>8429221.3005084284</v>
+        <f>D31*70%</f>
+        <v>4995094.104004995</v>
       </c>
       <c r="G31" s="4">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="C32" s="7">
-        <f>VLOOKUP(B32,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>165000000</v>
+        <v>176000000</v>
       </c>
       <c r="D32" s="7">
-        <f>VLOOKUP(B32,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>11149763.62501115</v>
+        <f>VLOOKUP(B32,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>12041744.715012042</v>
       </c>
       <c r="E32" s="7">
-        <f t="shared" si="0"/>
-        <v>10034787.262510035</v>
+        <f>D32*90%</f>
+        <v>10837570.243510839</v>
       </c>
       <c r="F32" s="7">
-        <f t="shared" si="1"/>
-        <v>7804834.5375078041</v>
+        <f>D32*70%</f>
+        <v>8429221.3005084284</v>
       </c>
       <c r="G32" s="4">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>579</v>
@@ -6492,106 +6015,129 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>560</v>
+        <v>526</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>535</v>
+        <v>545</v>
       </c>
       <c r="C33" s="7">
-        <f>VLOOKUP(B33,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>185300000</v>
+        <v>168000000</v>
       </c>
       <c r="D33" s="7">
-        <f>VLOOKUP(B33,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>11328159.843011327</v>
+        <f>VLOOKUP(B33,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>11149763.62501115</v>
       </c>
       <c r="E33" s="7">
-        <f t="shared" ref="E33:E34" si="6">D33*90%</f>
-        <v>10195343.858710194</v>
+        <f>D33*90%</f>
+        <v>10034787.262510035</v>
       </c>
       <c r="F33" s="7">
-        <f t="shared" ref="F33:F34" si="7">D33*70%</f>
-        <v>7929711.8901079288</v>
+        <f>D33*70%</f>
+        <v>7804834.5375078041</v>
       </c>
       <c r="G33" s="4">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>568</v>
+        <v>579</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C34" s="7">
+        <v>188300000</v>
+      </c>
+      <c r="D34" s="7">
+        <f>VLOOKUP(B34,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>11328159.843011327</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" ref="E34:E35" si="8">D34*90%</f>
+        <v>10195343.858710194</v>
+      </c>
+      <c r="F34" s="7">
+        <f t="shared" ref="F34:F35" si="9">D34*70%</f>
+        <v>7929711.8901079288</v>
+      </c>
+      <c r="G34" s="4">
+        <v>202</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="C34" s="7">
-        <f>VLOOKUP(B34,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>438000000</v>
-      </c>
-      <c r="D34" s="7">
-        <f>VLOOKUP(B34,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+      <c r="C35" s="7">
+        <v>443000000</v>
+      </c>
+      <c r="D35" s="7">
+        <f>VLOOKUP(B35,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>33003300.330032997</v>
       </c>
-      <c r="E34" s="7">
-        <f t="shared" si="6"/>
+      <c r="E35" s="7">
+        <f t="shared" si="8"/>
         <v>29702970.297029696</v>
       </c>
-      <c r="F34" s="7">
-        <f t="shared" si="7"/>
+      <c r="F35" s="7">
+        <f t="shared" si="9"/>
         <v>23102310.231023096</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G35" s="4">
         <v>249</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="8" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
         <v>522</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="C35" s="7">
-        <f>VLOOKUP(B35,[1]pricelist!$B$3:$C$51,2,0)</f>
-        <v>342650000</v>
-      </c>
-      <c r="D35" s="7">
-        <f>VLOOKUP(B35,[2]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+      <c r="C36" s="7">
+        <v>345650000</v>
+      </c>
+      <c r="D36" s="7">
+        <f>VLOOKUP(B36,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>22834715.904022835</v>
       </c>
-      <c r="E35" s="7">
-        <f t="shared" ref="E35" si="8">D35*90%</f>
+      <c r="E36" s="7">
+        <f t="shared" ref="E36" si="10">D36*90%</f>
         <v>20551244.313620552</v>
       </c>
-      <c r="F35" s="7">
-        <f t="shared" ref="F35" si="9">D35*70%</f>
+      <c r="F36" s="7">
+        <f t="shared" ref="F36" si="11">D36*70%</f>
         <v>15984301.132815983</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G36" s="4">
         <v>233</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H36" s="6" t="s">
         <v>567</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A34">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  <conditionalFormatting sqref="A2:A26 A28:A35">
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A35">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  <conditionalFormatting sqref="A2:A26 A28:A36">
+    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C26" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -7571,7 +7117,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A24" sqref="A24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7619,11 +7165,11 @@
         <v>541</v>
       </c>
       <c r="C2" s="7">
-        <f>VLOOKUP(B2,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B2,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>447200000</v>
       </c>
       <c r="D2" s="7">
-        <f>VLOOKUP(B2,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B2,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>31531.531531531527</v>
       </c>
       <c r="E2" s="7">
@@ -7649,11 +7195,11 @@
         <v>548</v>
       </c>
       <c r="C3" s="7">
-        <f>VLOOKUP(B3,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B3,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>388500000</v>
       </c>
       <c r="D3" s="7">
-        <f>VLOOKUP(B3,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B3,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>29729.729729729726</v>
       </c>
       <c r="E3" s="7">
@@ -7679,11 +7225,11 @@
         <v>542</v>
       </c>
       <c r="C4" s="7">
-        <f>VLOOKUP(B4,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B4,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>311500000</v>
       </c>
       <c r="D4" s="7">
-        <f>VLOOKUP(B4,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B4,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>20945.945945945943</v>
       </c>
       <c r="E4" s="7">
@@ -7709,11 +7255,11 @@
         <v>543</v>
       </c>
       <c r="C5" s="7">
-        <f>VLOOKUP(B5,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B5,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>329050000</v>
       </c>
       <c r="D5" s="7">
-        <f>VLOOKUP(B5,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B5,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>22252.252252252249</v>
       </c>
       <c r="E5" s="7">
@@ -7739,11 +7285,11 @@
         <v>530</v>
       </c>
       <c r="C6" s="7">
-        <f>VLOOKUP(B6,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B6,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>405000000</v>
       </c>
       <c r="D6" s="7">
-        <f>VLOOKUP(B6,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B6,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>31531.531531531527</v>
       </c>
       <c r="E6" s="7">
@@ -7769,11 +7315,11 @@
         <v>531</v>
       </c>
       <c r="C7" s="7">
-        <f>VLOOKUP(B7,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B7,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>442000000</v>
       </c>
       <c r="D7" s="7">
-        <f>VLOOKUP(B7,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B7,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>34234.234234234231</v>
       </c>
       <c r="E7" s="7">
@@ -7799,11 +7345,11 @@
         <v>532</v>
       </c>
       <c r="C8" s="7">
-        <f>VLOOKUP(B8,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B8,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>303000000</v>
       </c>
       <c r="D8" s="7">
-        <f>VLOOKUP(B8,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B8,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>20720.720720720718</v>
       </c>
       <c r="E8" s="7">
@@ -7829,11 +7375,11 @@
         <v>533</v>
       </c>
       <c r="C9" s="7">
-        <f>VLOOKUP(B9,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B9,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>263000000</v>
       </c>
       <c r="D9" s="7">
-        <f>VLOOKUP(B9,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B9,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18018.018018018018</v>
       </c>
       <c r="E9" s="7">
@@ -7859,11 +7405,11 @@
         <v>534</v>
       </c>
       <c r="C10" s="7">
-        <f>VLOOKUP(B10,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B10,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>217000000</v>
       </c>
       <c r="D10" s="7">
-        <f>VLOOKUP(B10,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B10,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>11711.71171171171</v>
       </c>
       <c r="E10" s="7">
@@ -7889,11 +7435,11 @@
         <v>535</v>
       </c>
       <c r="C11" s="7">
-        <f>VLOOKUP(B11,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B11,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>188300000</v>
       </c>
       <c r="D11" s="7">
-        <f>VLOOKUP(B11,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B11,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>11441.44144144144</v>
       </c>
       <c r="E11" s="7">
@@ -7919,11 +7465,11 @@
         <v>536</v>
       </c>
       <c r="C12" s="7">
-        <f>VLOOKUP(B12,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B12,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>222850000</v>
       </c>
       <c r="D12" s="7">
-        <f>VLOOKUP(B12,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B12,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>14414.414414414414</v>
       </c>
       <c r="E12" s="7">
@@ -7949,11 +7495,11 @@
         <v>537</v>
       </c>
       <c r="C13" s="7">
-        <f>VLOOKUP(B13,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B13,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>210700000</v>
       </c>
       <c r="D13" s="7">
-        <f>VLOOKUP(B13,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B13,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>13243.243243243242</v>
       </c>
       <c r="E13" s="7">
@@ -7979,11 +7525,11 @@
         <v>490</v>
       </c>
       <c r="C14" s="7">
-        <f>VLOOKUP(B14,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B14,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>277200000</v>
       </c>
       <c r="D14" s="7">
-        <f>VLOOKUP(B14,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B14,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18828.828828828828</v>
       </c>
       <c r="E14" s="7">
@@ -8009,11 +7555,11 @@
         <v>491</v>
       </c>
       <c r="C15" s="7">
-        <f>VLOOKUP(B15,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B15,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>291300000</v>
       </c>
       <c r="D15" s="7">
-        <f>VLOOKUP(B15,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B15,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>19819.819819819819</v>
       </c>
       <c r="E15" s="7">
@@ -8039,11 +7585,11 @@
         <v>544</v>
       </c>
       <c r="C16" s="7">
-        <f>VLOOKUP(B16,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B16,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>262500000</v>
       </c>
       <c r="D16" s="7">
-        <f>VLOOKUP(B16,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B16,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>16486.486486486487</v>
       </c>
       <c r="E16" s="7">
@@ -8069,11 +7615,11 @@
         <v>538</v>
       </c>
       <c r="C17" s="7">
-        <f>VLOOKUP(B17,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B17,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>285200000</v>
       </c>
       <c r="D17" s="7">
-        <f>VLOOKUP(B17,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B17,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18468.468468468465</v>
       </c>
       <c r="E17" s="7">
@@ -8099,11 +7645,11 @@
         <v>507</v>
       </c>
       <c r="C18" s="7">
-        <f>VLOOKUP(B18,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B18,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>214000000</v>
       </c>
       <c r="D18" s="7">
-        <f>VLOOKUP(B18,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B18,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18918.918918918916</v>
       </c>
       <c r="E18" s="7">
@@ -8129,11 +7675,11 @@
         <v>556</v>
       </c>
       <c r="C19" s="7">
-        <f>VLOOKUP(B19,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B19,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>251000000</v>
       </c>
       <c r="D19" s="7">
-        <f>VLOOKUP(B19,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B19,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18918.918918918916</v>
       </c>
       <c r="E19" s="7">
@@ -8159,11 +7705,11 @@
         <v>508</v>
       </c>
       <c r="C20" s="7">
-        <f>VLOOKUP(B20,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B20,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>251000000</v>
       </c>
       <c r="D20" s="7">
-        <f>VLOOKUP(B20,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B20,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18918.918918918916</v>
       </c>
       <c r="E20" s="7">
@@ -8189,11 +7735,11 @@
         <v>509</v>
       </c>
       <c r="C21" s="7">
-        <f>VLOOKUP(B21,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B21,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>307500000</v>
       </c>
       <c r="D21" s="7">
-        <f>VLOOKUP(B21,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B21,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>22522.522522522522</v>
       </c>
       <c r="E21" s="7">
@@ -8219,11 +7765,11 @@
         <v>549</v>
       </c>
       <c r="C22" s="7">
-        <f>VLOOKUP(B22,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B22,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>353000000</v>
       </c>
       <c r="D22" s="7">
-        <f>VLOOKUP(B22,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B22,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>26126.126126126124</v>
       </c>
       <c r="E22" s="7">
@@ -8249,11 +7795,11 @@
         <v>510</v>
       </c>
       <c r="C23" s="7">
-        <f>VLOOKUP(B23,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B23,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>363000000</v>
       </c>
       <c r="D23" s="7">
-        <f>VLOOKUP(B23,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B23,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>27027.027027027023</v>
       </c>
       <c r="E23" s="7">
@@ -8279,11 +7825,11 @@
         <v>511</v>
       </c>
       <c r="C24" s="7">
-        <f>VLOOKUP(B24,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B24,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>413000000</v>
       </c>
       <c r="D24" s="7">
-        <f>VLOOKUP(B24,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B24,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>30630.630630630629</v>
       </c>
       <c r="E24" s="7">
@@ -8309,11 +7855,11 @@
         <v>559</v>
       </c>
       <c r="C25" s="7">
-        <f>VLOOKUP(B25,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B25,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>415000000</v>
       </c>
       <c r="D25" s="7">
-        <f>VLOOKUP(B25,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B25,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33333.333333333328</v>
       </c>
       <c r="E25" s="7">
@@ -8339,11 +7885,11 @@
         <v>512</v>
       </c>
       <c r="C26" s="7">
-        <f>VLOOKUP(B26,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B26,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>443000000</v>
       </c>
       <c r="D26" s="7">
-        <f>VLOOKUP(B26,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B26,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33333.333333333328</v>
       </c>
       <c r="E26" s="7">
@@ -8369,11 +7915,11 @@
         <v>512</v>
       </c>
       <c r="C27" s="7">
-        <f>VLOOKUP(B27,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B27,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>443000000</v>
       </c>
       <c r="D27" s="7">
-        <f>VLOOKUP(B27,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B27,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33333.333333333328</v>
       </c>
       <c r="E27" s="7">
@@ -8399,11 +7945,11 @@
         <v>539</v>
       </c>
       <c r="C28" s="7">
-        <f>VLOOKUP(B28,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B28,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>155700000</v>
       </c>
       <c r="D28" s="7">
-        <f>VLOOKUP(B28,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B28,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>10990.990990990989</v>
       </c>
       <c r="E28" s="7">
@@ -8429,11 +7975,11 @@
         <v>513</v>
       </c>
       <c r="C29" s="7">
-        <f>VLOOKUP(B29,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B29,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>172600000</v>
       </c>
       <c r="D29" s="7">
-        <f>VLOOKUP(B29,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B29,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>7207.2072072072069</v>
       </c>
       <c r="E29" s="7">
@@ -8459,11 +8005,11 @@
         <v>540</v>
       </c>
       <c r="C30" s="7">
-        <f>VLOOKUP(B30,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B30,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>176000000</v>
       </c>
       <c r="D30" s="7">
-        <f>VLOOKUP(B30,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B30,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>12162.162162162162</v>
       </c>
       <c r="E30" s="7">
@@ -8489,11 +8035,11 @@
         <v>545</v>
       </c>
       <c r="C31" s="7">
-        <f>VLOOKUP(B31,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B31,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>168000000</v>
       </c>
       <c r="D31" s="7">
-        <f>VLOOKUP(B31,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B31,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>11261.261261261261</v>
       </c>
       <c r="E31" s="7">
@@ -8519,11 +8065,11 @@
         <v>535</v>
       </c>
       <c r="C32" s="7">
-        <f>VLOOKUP(B32,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B32,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>188300000</v>
       </c>
       <c r="D32" s="7">
-        <f>VLOOKUP(B32,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B32,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>11441.44144144144</v>
       </c>
       <c r="E32" s="7">
@@ -8549,11 +8095,11 @@
         <v>512</v>
       </c>
       <c r="C33" s="7">
-        <f>VLOOKUP(B33,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B33,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>443000000</v>
       </c>
       <c r="D33" s="7">
-        <f>VLOOKUP(B33,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B33,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33333.333333333328</v>
       </c>
       <c r="E33" s="7">
@@ -8579,11 +8125,11 @@
         <v>550</v>
       </c>
       <c r="C34" s="7">
-        <f>VLOOKUP(B34,[2]pricelist!$B$3:$C$53,2,0)</f>
+        <f>VLOOKUP(B34,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>345650000</v>
       </c>
       <c r="D34" s="7">
-        <f>VLOOKUP(B34,[2]pricelist!$B$3:$H$53,7,0)</f>
+        <f>VLOOKUP(B34,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>23063.063063063062</v>
       </c>
       <c r="E34" s="7">
@@ -8603,10 +8149,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A33">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A34">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UPDATE: DF and Pricelist - 1st August 2025
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35DD9C8-04D4-407D-BE2F-398399ABDC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B66198-2087-4301-B497-B4EF0EC17762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="587">
   <si>
     <t>Column1</t>
   </si>
@@ -2319,6 +2319,18 @@
   </si>
   <si>
     <t>EQ100460LV1CCS2</t>
+  </si>
+  <si>
+    <t>New Binguo EV Lite</t>
+  </si>
+  <si>
+    <t>New Binguo EV Pro</t>
+  </si>
+  <si>
+    <t>E260R EV 50ZW333LV0Y2A</t>
+  </si>
+  <si>
+    <t>E260R EV 50ZW333LV1Y2A</t>
   </si>
 </sst>
 </file>
@@ -5042,17 +5054,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05C9E0-A64E-40AC-B9F4-C919ED5906CC}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="51.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
@@ -5153,11 +5165,11 @@
         <v>29435375.970029432</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E32" si="0">D3*90%</f>
+        <f t="shared" ref="E3:E28" si="0">D3*90%</f>
         <v>26491838.37302649</v>
       </c>
       <c r="F3" s="7">
-        <f t="shared" ref="F3:F32" si="1">D3*70%</f>
+        <f t="shared" ref="F3:F28" si="1">D3*70%</f>
         <v>20604763.179020602</v>
       </c>
       <c r="G3" s="9">
@@ -5812,329 +5824,387 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>557</v>
+        <v>585</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>559</v>
+        <v>583</v>
       </c>
       <c r="C26" s="7">
-        <v>415000000</v>
+        <v>318000000</v>
       </c>
       <c r="D26" s="7">
-        <f>VLOOKUP(B26,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33003300.330032997</v>
+        <f>26000000/1.12</f>
+        <v>23214285.714285713</v>
       </c>
       <c r="E26" s="7">
-        <f t="shared" si="0"/>
-        <v>29702970.297029696</v>
+        <f t="shared" ref="E26:E27" si="4">D26*90%</f>
+        <v>20892857.142857142</v>
       </c>
       <c r="F26" s="7">
-        <f t="shared" si="1"/>
-        <v>23102310.231023096</v>
+        <f t="shared" ref="F26:F27" si="5">D26*70%</f>
+        <v>16249999.999999998</v>
       </c>
       <c r="G26" s="4">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>582</v>
+      <c r="A27" s="6" t="s">
+        <v>586</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>559</v>
+        <v>584</v>
       </c>
       <c r="C27" s="7">
-        <v>415000000</v>
+        <v>363000000</v>
       </c>
       <c r="D27" s="7">
-        <f>VLOOKUP(B27,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33003300.330032997</v>
+        <f>29000000/1.12</f>
+        <v>25892857.142857142</v>
       </c>
       <c r="E27" s="7">
-        <f t="shared" ref="E27" si="4">D27*90%</f>
-        <v>29702970.297029696</v>
+        <f t="shared" si="4"/>
+        <v>23303571.428571429</v>
       </c>
       <c r="F27" s="7">
-        <f t="shared" ref="F27" si="5">D27*70%</f>
-        <v>23102310.231023096</v>
+        <f t="shared" si="5"/>
+        <v>18124999.999999996</v>
       </c>
       <c r="G27" s="4">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>512</v>
+        <v>559</v>
       </c>
       <c r="C28" s="7">
-        <v>443000000</v>
+        <v>415000000</v>
       </c>
       <c r="D28" s="7">
         <f>VLOOKUP(B28,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>33003300.330032997</v>
       </c>
       <c r="E28" s="7">
-        <f t="shared" ref="E28" si="6">D28*90%</f>
+        <f t="shared" si="0"/>
         <v>29702970.297029696</v>
       </c>
       <c r="F28" s="7">
-        <f t="shared" ref="F28" si="7">D28*70%</f>
+        <f t="shared" si="1"/>
         <v>23102310.231023096</v>
       </c>
       <c r="G28" s="4">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>506</v>
+      <c r="A29" t="s">
+        <v>582</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>512</v>
+        <v>559</v>
       </c>
       <c r="C29" s="7">
-        <v>443000000</v>
+        <v>415000000</v>
       </c>
       <c r="D29" s="7">
         <f>VLOOKUP(B29,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>33003300.330032997</v>
       </c>
       <c r="E29" s="7">
-        <f>D29*90%</f>
+        <f t="shared" ref="E29" si="6">D29*90%</f>
         <v>29702970.297029696</v>
       </c>
       <c r="F29" s="7">
-        <f>D29*70%</f>
+        <f t="shared" ref="F29" si="7">D29*70%</f>
         <v>23102310.231023096</v>
       </c>
       <c r="G29" s="4">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
-        <v>529</v>
+        <v>558</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="C30" s="7">
-        <v>155700000</v>
+        <v>443000000</v>
       </c>
       <c r="D30" s="7">
         <f>VLOOKUP(B30,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>10882169.29801088</v>
+        <v>33003300.330032997</v>
       </c>
       <c r="E30" s="7">
-        <f>D30*90%</f>
-        <v>9793952.3682097923</v>
+        <f t="shared" ref="E30" si="8">D30*90%</f>
+        <v>29702970.297029696</v>
       </c>
       <c r="F30" s="7">
-        <f>D30*70%</f>
-        <v>7617518.5086076157</v>
+        <f t="shared" ref="F30" si="9">D30*70%</f>
+        <v>23102310.231023096</v>
       </c>
       <c r="G30" s="4">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C31" s="7">
-        <v>172600000</v>
+        <v>443000000</v>
       </c>
       <c r="D31" s="7">
         <f>VLOOKUP(B31,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>7135848.7200071355</v>
+        <v>33003300.330032997</v>
       </c>
       <c r="E31" s="7">
         <f>D31*90%</f>
-        <v>6422263.8480064217</v>
+        <v>29702970.297029696</v>
       </c>
       <c r="F31" s="7">
         <f>D31*70%</f>
-        <v>4995094.104004995</v>
+        <v>23102310.231023096</v>
       </c>
       <c r="G31" s="4">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C32" s="7">
-        <v>176000000</v>
+        <v>155700000</v>
       </c>
       <c r="D32" s="7">
         <f>VLOOKUP(B32,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>12041744.715012042</v>
+        <v>10882169.29801088</v>
       </c>
       <c r="E32" s="7">
         <f>D32*90%</f>
-        <v>10837570.243510839</v>
+        <v>9793952.3682097923</v>
       </c>
       <c r="F32" s="7">
         <f>D32*70%</f>
-        <v>8429221.3005084284</v>
+        <v>7617518.5086076157</v>
       </c>
       <c r="G32" s="4">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>545</v>
+        <v>513</v>
       </c>
       <c r="C33" s="7">
-        <v>168000000</v>
+        <v>172600000</v>
       </c>
       <c r="D33" s="7">
         <f>VLOOKUP(B33,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>11149763.62501115</v>
+        <v>7135848.7200071355</v>
       </c>
       <c r="E33" s="7">
         <f>D33*90%</f>
-        <v>10034787.262510035</v>
+        <v>6422263.8480064217</v>
       </c>
       <c r="F33" s="7">
         <f>D33*70%</f>
-        <v>7804834.5375078041</v>
+        <v>4995094.104004995</v>
       </c>
       <c r="G33" s="4">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>560</v>
+        <v>521</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="C34" s="7">
-        <v>188300000</v>
+        <v>176000000</v>
       </c>
       <c r="D34" s="7">
         <f>VLOOKUP(B34,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>11328159.843011327</v>
+        <v>12041744.715012042</v>
       </c>
       <c r="E34" s="7">
-        <f t="shared" ref="E34:E35" si="8">D34*90%</f>
-        <v>10195343.858710194</v>
+        <f>D34*90%</f>
+        <v>10837570.243510839</v>
       </c>
       <c r="F34" s="7">
-        <f t="shared" ref="F34:F35" si="9">D34*70%</f>
-        <v>7929711.8901079288</v>
+        <f>D34*70%</f>
+        <v>8429221.3005084284</v>
       </c>
       <c r="G34" s="4">
-        <v>202</v>
+        <v>238</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>568</v>
+        <v>579</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>561</v>
+        <v>526</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>512</v>
+        <v>545</v>
       </c>
       <c r="C35" s="7">
-        <v>443000000</v>
+        <v>168000000</v>
       </c>
       <c r="D35" s="7">
         <f>VLOOKUP(B35,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33003300.330032997</v>
+        <v>11149763.62501115</v>
       </c>
       <c r="E35" s="7">
-        <f t="shared" si="8"/>
-        <v>29702970.297029696</v>
+        <f>D35*90%</f>
+        <v>10034787.262510035</v>
       </c>
       <c r="F35" s="7">
-        <f t="shared" si="9"/>
-        <v>23102310.231023096</v>
+        <f>D35*70%</f>
+        <v>7804834.5375078041</v>
       </c>
       <c r="G35" s="4">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>571</v>
+        <v>579</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
-        <v>522</v>
+      <c r="A36" s="6" t="s">
+        <v>560</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
       <c r="C36" s="7">
-        <v>345650000</v>
+        <v>188300000</v>
       </c>
       <c r="D36" s="7">
         <f>VLOOKUP(B36,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>11328159.843011327</v>
+      </c>
+      <c r="E36" s="7">
+        <f t="shared" ref="E36:E37" si="10">D36*90%</f>
+        <v>10195343.858710194</v>
+      </c>
+      <c r="F36" s="7">
+        <f t="shared" ref="F36:F37" si="11">D36*70%</f>
+        <v>7929711.8901079288</v>
+      </c>
+      <c r="G36" s="4">
+        <v>202</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="C37" s="7">
+        <v>443000000</v>
+      </c>
+      <c r="D37" s="7">
+        <f>VLOOKUP(B37,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
+        <v>33003300.330032997</v>
+      </c>
+      <c r="E37" s="7">
+        <f t="shared" si="10"/>
+        <v>29702970.297029696</v>
+      </c>
+      <c r="F37" s="7">
+        <f t="shared" si="11"/>
+        <v>23102310.231023096</v>
+      </c>
+      <c r="G37" s="4">
+        <v>249</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="C38" s="7">
+        <v>345650000</v>
+      </c>
+      <c r="D38" s="7">
+        <f>VLOOKUP(B38,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
         <v>22834715.904022835</v>
       </c>
-      <c r="E36" s="7">
-        <f t="shared" ref="E36" si="10">D36*90%</f>
+      <c r="E38" s="7">
+        <f t="shared" ref="E38" si="12">D38*90%</f>
         <v>20551244.313620552</v>
       </c>
-      <c r="F36" s="7">
-        <f t="shared" ref="F36" si="11">D36*70%</f>
+      <c r="F38" s="7">
+        <f t="shared" ref="F38" si="13">D38*70%</f>
         <v>15984301.132815983</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G38" s="4">
         <v>233</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>567</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A26 A28:A35">
+  <conditionalFormatting sqref="A30:A37 A2:A28">
     <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A26 A28:A36">
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+  <conditionalFormatting sqref="A30:A38 A2:A28">
+    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8149,10 +8219,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A33">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A34">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UPDATE: RS and Pricelist as of 04/08/2025
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B66198-2087-4301-B497-B4EF0EC17762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F554F98E-42E8-4DBA-8F4A-D988EED529AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="588">
   <si>
     <t>Column1</t>
   </si>
@@ -2331,6 +2331,9 @@
   </si>
   <si>
     <t>E260R EV 50ZW333LV1Y2A</t>
+  </si>
+  <si>
+    <t>Full Margin</t>
   </si>
 </sst>
 </file>
@@ -2426,7 +2429,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2445,6 +2448,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2953,7 +2958,7 @@
             <v>187264138.16</v>
           </cell>
           <cell r="H3">
-            <v>18918.918918918916</v>
+            <v>18750</v>
           </cell>
         </row>
         <row r="4">
@@ -2974,7 +2979,7 @@
             <v>220202148.16</v>
           </cell>
           <cell r="H4">
-            <v>18918.918918918916</v>
+            <v>18750</v>
           </cell>
         </row>
         <row r="5">
@@ -2995,7 +3000,7 @@
             <v>220194138.16</v>
           </cell>
           <cell r="H5">
-            <v>18918.918918918916</v>
+            <v>18750</v>
           </cell>
         </row>
         <row r="6">
@@ -3016,7 +3021,7 @@
             <v>270444428.16000003</v>
           </cell>
           <cell r="H6">
-            <v>22522.522522522522</v>
+            <v>22321.428571428569</v>
           </cell>
         </row>
         <row r="7">
@@ -3037,7 +3042,7 @@
             <v>300132158.16000003</v>
           </cell>
           <cell r="H7">
-            <v>29729.729729729726</v>
+            <v>29464.28571428571</v>
           </cell>
         </row>
         <row r="8">
@@ -3058,7 +3063,7 @@
             <v>254888118.16</v>
           </cell>
           <cell r="H8">
-            <v>22252.252252252249</v>
+            <v>22053.571428571428</v>
           </cell>
         </row>
         <row r="9">
@@ -3079,7 +3084,7 @@
             <v>240957838.16</v>
           </cell>
           <cell r="H9">
-            <v>20945.945945945943</v>
+            <v>20758.928571428569</v>
           </cell>
         </row>
         <row r="10">
@@ -3100,7 +3105,7 @@
             <v>297015378.16000003</v>
           </cell>
           <cell r="H10">
-            <v>26126.126126126124</v>
+            <v>25892.857142857141</v>
           </cell>
         </row>
         <row r="11">
@@ -3121,7 +3126,7 @@
             <v>352375158.16000003</v>
           </cell>
           <cell r="H11">
-            <v>31531.531531531527</v>
+            <v>31249.999999999996</v>
           </cell>
         </row>
         <row r="12">
@@ -3142,7 +3147,7 @@
             <v>291141378.16000003</v>
           </cell>
           <cell r="H12">
-            <v>28918.918918918916</v>
+            <v>28660.714285714283</v>
           </cell>
         </row>
         <row r="13">
@@ -3163,7 +3168,7 @@
             <v>304849158.16000003</v>
           </cell>
           <cell r="H13">
-            <v>27027.027027027023</v>
+            <v>26785.714285714283</v>
           </cell>
         </row>
         <row r="14">
@@ -3184,7 +3189,7 @@
             <v>377944858.16000003</v>
           </cell>
           <cell r="H14">
-            <v>34234.234234234231</v>
+            <v>33928.571428571428</v>
           </cell>
         </row>
         <row r="15">
@@ -3205,7 +3210,7 @@
             <v>237657718.16</v>
           </cell>
           <cell r="H15">
-            <v>20720.720720720718</v>
+            <v>20535.714285714283</v>
           </cell>
         </row>
         <row r="16">
@@ -3226,7 +3231,7 @@
             <v>206085858.16</v>
           </cell>
           <cell r="H16">
-            <v>18018.018018018018</v>
+            <v>17857.142857142855</v>
           </cell>
         </row>
         <row r="17">
@@ -3247,7 +3252,7 @@
             <v>169433878.16</v>
           </cell>
           <cell r="H17">
-            <v>11711.71171171171</v>
+            <v>11607.142857142857</v>
           </cell>
         </row>
         <row r="18">
@@ -3268,7 +3273,7 @@
             <v>310961678.16000003</v>
           </cell>
           <cell r="H18">
-            <v>26126.126126126124</v>
+            <v>25892.857142857141</v>
           </cell>
         </row>
         <row r="19">
@@ -3289,7 +3294,7 @@
             <v>319855448.16000003</v>
           </cell>
           <cell r="H19">
-            <v>27027.027027027023</v>
+            <v>26785.714285714283</v>
           </cell>
         </row>
         <row r="20">
@@ -3310,7 +3315,7 @@
             <v>364323408.16000003</v>
           </cell>
           <cell r="H20">
-            <v>30630.630630630629</v>
+            <v>30357.142857142855</v>
           </cell>
         </row>
         <row r="21">
@@ -3331,7 +3336,7 @@
             <v>366060688.16000003</v>
           </cell>
           <cell r="H21">
-            <v>33333.333333333328</v>
+            <v>33035.714285714283</v>
           </cell>
         </row>
         <row r="22">
@@ -3352,7 +3357,7 @@
             <v>439275144</v>
           </cell>
           <cell r="H22">
-            <v>33333.333333333328</v>
+            <v>33035.714285714283</v>
           </cell>
         </row>
         <row r="23">
@@ -3373,7 +3378,7 @@
             <v>143819678.16</v>
           </cell>
           <cell r="H23">
-            <v>11441.44144144144</v>
+            <v>11339.285714285714</v>
           </cell>
         </row>
         <row r="24">
@@ -3394,7 +3399,7 @@
             <v>173990678.16</v>
           </cell>
           <cell r="H24">
-            <v>14414.414414414414</v>
+            <v>14285.714285714284</v>
           </cell>
         </row>
         <row r="25">
@@ -3415,7 +3420,7 @@
             <v>164695518.16</v>
           </cell>
           <cell r="H25">
-            <v>13513.513513513511</v>
+            <v>13392.857142857141</v>
           </cell>
         </row>
         <row r="26">
@@ -3436,7 +3441,7 @@
             <v>161936518.16</v>
           </cell>
           <cell r="H26">
-            <v>13243.243243243242</v>
+            <v>13124.999999999998</v>
           </cell>
         </row>
         <row r="27">
@@ -3457,7 +3462,7 @@
             <v>184870038.16</v>
           </cell>
           <cell r="H27">
-            <v>15045.045045045044</v>
+            <v>14910.714285714284</v>
           </cell>
         </row>
         <row r="28">
@@ -3478,7 +3483,7 @@
             <v>172166178.16</v>
           </cell>
           <cell r="H28">
-            <v>14144.144144144142</v>
+            <v>14017.857142857141</v>
           </cell>
         </row>
         <row r="29">
@@ -3499,7 +3504,7 @@
             <v>268855778.16000003</v>
           </cell>
           <cell r="H29">
-            <v>23063.063063063062</v>
+            <v>22857.142857142855</v>
           </cell>
         </row>
         <row r="30">
@@ -3520,7 +3525,7 @@
             <v>224165976.75999999</v>
           </cell>
           <cell r="H30">
-            <v>18468.468468468465</v>
+            <v>18303.571428571428</v>
           </cell>
         </row>
         <row r="31">
@@ -3558,7 +3563,7 @@
             <v>202388798.16</v>
           </cell>
           <cell r="H32">
-            <v>16486.486486486487</v>
+            <v>16339.285714285712</v>
           </cell>
         </row>
         <row r="33">
@@ -3579,7 +3584,7 @@
             <v>213392758.16</v>
           </cell>
           <cell r="H33">
-            <v>18828.828828828828</v>
+            <v>18660.714285714283</v>
           </cell>
         </row>
         <row r="34">
@@ -3600,7 +3605,7 @@
             <v>217041758.16</v>
           </cell>
           <cell r="H34">
-            <v>19189.189189189186</v>
+            <v>19017.857142857141</v>
           </cell>
         </row>
         <row r="35">
@@ -3621,7 +3626,7 @@
             <v>224512418.16</v>
           </cell>
           <cell r="H35">
-            <v>19819.819819819819</v>
+            <v>19642.857142857141</v>
           </cell>
         </row>
         <row r="36">
@@ -3642,7 +3647,7 @@
             <v>228072418.16</v>
           </cell>
           <cell r="H36">
-            <v>20180.180180180178</v>
+            <v>19999.999999999996</v>
           </cell>
         </row>
         <row r="37">
@@ -3663,7 +3668,7 @@
             <v>265295778.16</v>
           </cell>
           <cell r="H37">
-            <v>22702.7027027027</v>
+            <v>22499.999999999996</v>
           </cell>
         </row>
         <row r="38">
@@ -3684,7 +3689,7 @@
             <v>258175778.16</v>
           </cell>
           <cell r="H38">
-            <v>23063.063063063062</v>
+            <v>22857.142857142855</v>
           </cell>
         </row>
         <row r="39">
@@ -3705,7 +3710,7 @@
             <v>254615778.16</v>
           </cell>
           <cell r="H39">
-            <v>22702.7027027027</v>
+            <v>22499.999999999996</v>
           </cell>
         </row>
         <row r="40">
@@ -3726,7 +3731,7 @@
             <v>216233638.16</v>
           </cell>
           <cell r="H40">
-            <v>17747.747747747748</v>
+            <v>17589.285714285714</v>
           </cell>
         </row>
         <row r="41">
@@ -3747,7 +3752,7 @@
             <v>223442638.16</v>
           </cell>
           <cell r="H41">
-            <v>18468.468468468465</v>
+            <v>18303.571428571428</v>
           </cell>
         </row>
         <row r="42">
@@ -3768,7 +3773,7 @@
             <v>205948798.16</v>
           </cell>
           <cell r="H42">
-            <v>16846.846846846845</v>
+            <v>16696.428571428569</v>
           </cell>
         </row>
         <row r="43">
@@ -3789,7 +3794,7 @@
             <v>127594978.16</v>
           </cell>
           <cell r="H43">
-            <v>11261.261261261261</v>
+            <v>11160.714285714284</v>
           </cell>
         </row>
         <row r="44">
@@ -3810,7 +3815,7 @@
             <v>134714978.16</v>
           </cell>
           <cell r="H44">
-            <v>12162.162162162162</v>
+            <v>12053.571428571428</v>
           </cell>
         </row>
         <row r="45">
@@ -3831,7 +3836,7 @@
             <v>129323358.16</v>
           </cell>
           <cell r="H45">
-            <v>7207.2072072072069</v>
+            <v>7142.8571428571422</v>
           </cell>
         </row>
         <row r="46">
@@ -3852,7 +3857,7 @@
             <v>132815718.16</v>
           </cell>
           <cell r="H46">
-            <v>7207.2072072072069</v>
+            <v>7142.8571428571422</v>
           </cell>
         </row>
         <row r="47">
@@ -3873,7 +3878,7 @@
             <v>123770648.16</v>
           </cell>
           <cell r="H47">
-            <v>10990.990990990989</v>
+            <v>10892.857142857141</v>
           </cell>
         </row>
         <row r="48">
@@ -3894,7 +3899,7 @@
             <v>320959938.16000003</v>
           </cell>
           <cell r="H48">
-            <v>31531.531531531527</v>
+            <v>31249.999999999996</v>
           </cell>
         </row>
         <row r="49">
@@ -3915,7 +3920,7 @@
             <v>290258498.16000003</v>
           </cell>
           <cell r="H49">
-            <v>29729.729729729726</v>
+            <v>29464.28571428571</v>
           </cell>
         </row>
         <row r="50">
@@ -3936,7 +3941,7 @@
             <v>350283230.95999998</v>
           </cell>
           <cell r="H50">
-            <v>34234.234234234231</v>
+            <v>33928.571428571428</v>
           </cell>
         </row>
         <row r="51">
@@ -3957,7 +3962,7 @@
             <v>245986338.16</v>
           </cell>
           <cell r="H51">
-            <v>19819.819819819819</v>
+            <v>19642.857142857141</v>
           </cell>
         </row>
         <row r="52">
@@ -3978,7 +3983,7 @@
             <v>235192418.16</v>
           </cell>
           <cell r="H52">
-            <v>20180.180180180178</v>
+            <v>19999.999999999996</v>
           </cell>
         </row>
         <row r="53">
@@ -3999,7 +4004,7 @@
             <v>238752418.16</v>
           </cell>
           <cell r="H53">
-            <v>19819.819819819819</v>
+            <v>19642.857142857141</v>
           </cell>
         </row>
       </sheetData>
@@ -5056,8 +5061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05C9E0-A64E-40AC-B9F4-C919ED5906CC}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:H27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5120,6 +5125,9 @@
       <c r="H1" s="11" t="s">
         <v>564</v>
       </c>
+      <c r="I1" s="13" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -5132,22 +5140,25 @@
         <v>447200000</v>
       </c>
       <c r="D2" s="7">
-        <f>VLOOKUP(B2,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>31219338.150031216</v>
+        <f>I2/1.12</f>
+        <v>31249999.999999996</v>
       </c>
       <c r="E2" s="7">
         <f>D2*90%</f>
-        <v>28097404.335028097</v>
+        <v>28124999.999999996</v>
       </c>
       <c r="F2" s="7">
         <f>D2*70%</f>
-        <v>21853536.705021851</v>
+        <v>21874999.999999996</v>
       </c>
       <c r="G2" s="9">
         <v>228</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>565</v>
+      </c>
+      <c r="I2" s="12">
+        <v>35000000</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -5161,22 +5172,25 @@
         <v>388500000</v>
       </c>
       <c r="D3" s="7">
-        <f>VLOOKUP(B3,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>29435375.970029432</v>
+        <f t="shared" ref="D3:D38" si="0">I3/1.12</f>
+        <v>29464285.714285709</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E28" si="0">D3*90%</f>
-        <v>26491838.37302649</v>
+        <f t="shared" ref="E3:E28" si="1">D3*90%</f>
+        <v>26517857.142857138</v>
       </c>
       <c r="F3" s="7">
-        <f t="shared" ref="F3:F28" si="1">D3*70%</f>
-        <v>20604763.179020602</v>
+        <f t="shared" ref="F3:F28" si="2">D3*70%</f>
+        <v>20624999.999999996</v>
       </c>
       <c r="G3" s="9">
         <v>227</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>565</v>
+      </c>
+      <c r="I3" s="12">
+        <v>32999999.999999996</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -5190,22 +5204,25 @@
         <v>311500000</v>
       </c>
       <c r="D4" s="7">
-        <f>VLOOKUP(B4,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>20738560.342520736</v>
+        <f t="shared" si="0"/>
+        <v>20758928.571428567</v>
       </c>
       <c r="E4" s="7">
-        <f t="shared" si="0"/>
-        <v>18664704.308268663</v>
+        <f t="shared" si="1"/>
+        <v>18683035.714285713</v>
       </c>
       <c r="F4" s="7">
-        <f t="shared" si="1"/>
-        <v>14516992.239764515</v>
+        <f t="shared" si="2"/>
+        <v>14531249.999999996</v>
       </c>
       <c r="G4" s="9">
         <v>222</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>565</v>
+      </c>
+      <c r="I4" s="12">
+        <v>23249999.999999996</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -5219,22 +5236,25 @@
         <v>329050000</v>
       </c>
       <c r="D5" s="7">
-        <f>VLOOKUP(B5,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>22031932.923022028</v>
+        <f t="shared" si="0"/>
+        <v>22053571.428571429</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" si="0"/>
-        <v>19828739.630719826</v>
+        <f t="shared" si="1"/>
+        <v>19848214.285714287</v>
       </c>
       <c r="F5" s="7">
-        <f t="shared" si="1"/>
-        <v>15422353.046115419</v>
+        <f t="shared" si="2"/>
+        <v>15437500</v>
       </c>
       <c r="G5" s="9">
         <v>223</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>565</v>
+      </c>
+      <c r="I5" s="12">
+        <v>24700000.000000004</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -5248,22 +5268,25 @@
         <v>405000000</v>
       </c>
       <c r="D6" s="7">
-        <f>VLOOKUP(B6,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>31219338.150031216</v>
+        <f t="shared" si="0"/>
+        <v>31249999.999999996</v>
       </c>
       <c r="E6" s="7">
-        <f t="shared" si="0"/>
-        <v>28097404.335028097</v>
+        <f t="shared" si="1"/>
+        <v>28124999.999999996</v>
       </c>
       <c r="F6" s="7">
-        <f t="shared" si="1"/>
-        <v>21853536.705021851</v>
+        <f t="shared" si="2"/>
+        <v>21874999.999999996</v>
       </c>
       <c r="G6" s="9">
         <v>244</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>565</v>
+      </c>
+      <c r="I6" s="12">
+        <v>35000000</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -5277,22 +5300,25 @@
         <v>442000000</v>
       </c>
       <c r="D7" s="7">
-        <f>VLOOKUP(B7,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33895281.420033887</v>
+        <f t="shared" si="0"/>
+        <v>33928571.428571425</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" si="0"/>
-        <v>30505753.2780305</v>
+        <f t="shared" si="1"/>
+        <v>30535714.285714284</v>
       </c>
       <c r="F7" s="7">
-        <f t="shared" si="1"/>
-        <v>23726696.994023718</v>
+        <f t="shared" si="2"/>
+        <v>23749999.999999996</v>
       </c>
       <c r="G7" s="9">
         <v>245</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>565</v>
+      </c>
+      <c r="I7" s="12">
+        <v>38000000</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -5307,22 +5333,25 @@
         <v>303000000</v>
       </c>
       <c r="D8" s="7">
-        <f>VLOOKUP(B8,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>20515565.070020512</v>
+        <f t="shared" si="0"/>
+        <v>20535714.285714284</v>
       </c>
       <c r="E8" s="7">
-        <f t="shared" si="0"/>
-        <v>18464008.56301846</v>
+        <f t="shared" si="1"/>
+        <v>18482142.857142854</v>
       </c>
       <c r="F8" s="7">
-        <f t="shared" si="1"/>
-        <v>14360895.549014358</v>
+        <f t="shared" si="2"/>
+        <v>14374999.999999998</v>
       </c>
       <c r="G8" s="4">
         <v>240</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>566</v>
+      </c>
+      <c r="I8" s="12">
+        <v>23000000</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -5336,22 +5365,25 @@
         <v>263000000</v>
       </c>
       <c r="D9" s="7">
-        <f>VLOOKUP(B9,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>17839621.800017841</v>
+        <f t="shared" si="0"/>
+        <v>17857142.857142854</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" si="0"/>
-        <v>16055659.620016057</v>
+        <f t="shared" si="1"/>
+        <v>16071428.571428569</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="1"/>
-        <v>12487735.260012489</v>
+        <f t="shared" si="2"/>
+        <v>12499999.999999998</v>
       </c>
       <c r="G9" s="4">
         <v>241</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>566</v>
+      </c>
+      <c r="I9" s="12">
+        <v>20000000</v>
       </c>
       <c r="J9" s="3"/>
     </row>
@@ -5366,22 +5398,25 @@
         <v>217000000</v>
       </c>
       <c r="D10" s="7">
-        <f>VLOOKUP(B10,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>11595754.170011595</v>
+        <f t="shared" si="0"/>
+        <v>11607142.857142856</v>
       </c>
       <c r="E10" s="7">
-        <f t="shared" si="0"/>
-        <v>10436178.753010435</v>
+        <f t="shared" si="1"/>
+        <v>10446428.571428571</v>
       </c>
       <c r="F10" s="7">
-        <f t="shared" si="1"/>
-        <v>8117027.9190081162</v>
+        <f t="shared" si="2"/>
+        <v>8124999.9999999991</v>
       </c>
       <c r="G10" s="4">
         <v>242</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>566</v>
+      </c>
+      <c r="I10" s="12">
+        <v>13000000</v>
       </c>
       <c r="J10" s="3"/>
     </row>
@@ -5396,22 +5431,25 @@
         <v>188300000</v>
       </c>
       <c r="D11" s="7">
-        <f>VLOOKUP(B11,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>11328159.843011327</v>
+        <f t="shared" si="0"/>
+        <v>11339285.714285715</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" si="0"/>
-        <v>10195343.858710194</v>
+        <f t="shared" si="1"/>
+        <v>10205357.142857144</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" si="1"/>
-        <v>7929711.8901079288</v>
+        <f t="shared" si="2"/>
+        <v>7937500</v>
       </c>
       <c r="G11" s="4">
         <v>202</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>568</v>
+      </c>
+      <c r="I11" s="12">
+        <v>12700000.000000002</v>
       </c>
       <c r="J11" s="3"/>
     </row>
@@ -5426,22 +5464,25 @@
         <v>222850000</v>
       </c>
       <c r="D12" s="7">
-        <f>VLOOKUP(B12,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>14271697.440014271</v>
+        <f t="shared" si="0"/>
+        <v>14285714.285714284</v>
       </c>
       <c r="E12" s="7">
-        <f t="shared" si="0"/>
-        <v>12844527.696012843</v>
+        <f t="shared" si="1"/>
+        <v>12857142.857142856</v>
       </c>
       <c r="F12" s="7">
-        <f t="shared" si="1"/>
-        <v>9990188.2080099899</v>
+        <f t="shared" si="2"/>
+        <v>9999999.9999999981</v>
       </c>
       <c r="G12" s="4">
         <v>204</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>573</v>
+      </c>
+      <c r="I12" s="12">
+        <v>16000000</v>
       </c>
       <c r="J12" s="3"/>
     </row>
@@ -5456,22 +5497,25 @@
         <v>210700000</v>
       </c>
       <c r="D13" s="7">
-        <f>VLOOKUP(B13,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>13112122.023013111</v>
+        <f t="shared" si="0"/>
+        <v>13124999.999999998</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="0"/>
-        <v>11800909.820711801</v>
+        <f t="shared" si="1"/>
+        <v>11812499.999999998</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="1"/>
-        <v>9178485.4161091764</v>
+        <f t="shared" si="2"/>
+        <v>9187499.9999999981</v>
       </c>
       <c r="G13" s="4">
         <v>205</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>573</v>
+      </c>
+      <c r="I13" s="12">
+        <v>14700000</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -5485,22 +5529,25 @@
         <v>277200000</v>
       </c>
       <c r="D14" s="7">
-        <f>VLOOKUP(B14,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>18642404.781018641</v>
+        <f t="shared" si="0"/>
+        <v>18660714.285714284</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" si="0"/>
-        <v>16778164.302916776</v>
+        <f t="shared" si="1"/>
+        <v>16794642.857142854</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" si="1"/>
-        <v>13049683.346713047</v>
+        <f t="shared" si="2"/>
+        <v>13062499.999999998</v>
       </c>
       <c r="G14" s="4">
         <v>213</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>567</v>
+      </c>
+      <c r="I14" s="12">
+        <v>20900000</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -5514,22 +5561,25 @@
         <v>291300000</v>
       </c>
       <c r="D15" s="7">
-        <f>VLOOKUP(B15,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>19623583.980019622</v>
+        <f t="shared" si="0"/>
+        <v>19642857.142857142</v>
       </c>
       <c r="E15" s="7">
-        <f t="shared" si="0"/>
-        <v>17661225.58201766</v>
+        <f t="shared" si="1"/>
+        <v>17678571.428571429</v>
       </c>
       <c r="F15" s="7">
-        <f t="shared" si="1"/>
-        <v>13736508.786013734</v>
+        <f t="shared" si="2"/>
+        <v>13749999.999999998</v>
       </c>
       <c r="G15" s="4">
         <v>214</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>567</v>
+      </c>
+      <c r="I15" s="12">
+        <v>22000000</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -5543,16 +5593,16 @@
         <v>262500000</v>
       </c>
       <c r="D16" s="7">
-        <f>VLOOKUP(B16,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>16323253.947016323</v>
+        <f t="shared" si="0"/>
+        <v>16339285.714285713</v>
       </c>
       <c r="E16" s="7">
-        <f t="shared" si="0"/>
-        <v>14690928.552314691</v>
+        <f t="shared" si="1"/>
+        <v>14705357.142857142</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" si="1"/>
-        <v>11426277.762911426</v>
+        <f t="shared" si="2"/>
+        <v>11437499.999999998</v>
       </c>
       <c r="G16" s="4">
         <v>209</v>
@@ -5560,8 +5610,11 @@
       <c r="H16" s="6" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="12">
+        <v>18300000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>499</v>
       </c>
@@ -5572,16 +5625,16 @@
         <v>285200000</v>
       </c>
       <c r="D17" s="7">
-        <f>VLOOKUP(B17,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>18285612.345018283</v>
+        <f t="shared" si="0"/>
+        <v>18303571.428571429</v>
       </c>
       <c r="E17" s="7">
-        <f t="shared" si="0"/>
-        <v>16457051.110516455</v>
+        <f t="shared" si="1"/>
+        <v>16473214.285714287</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" si="1"/>
-        <v>12799928.641512796</v>
+        <f t="shared" si="2"/>
+        <v>12812500</v>
       </c>
       <c r="G17" s="4">
         <v>220</v>
@@ -5589,8 +5642,11 @@
       <c r="H17" s="6" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="12">
+        <v>20500000.000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>580</v>
       </c>
@@ -5601,16 +5657,16 @@
         <v>214000000</v>
       </c>
       <c r="D18" s="7">
-        <f>VLOOKUP(B18,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>18731602.890018728</v>
+        <f t="shared" si="0"/>
+        <v>18750000</v>
       </c>
       <c r="E18" s="7">
-        <f t="shared" si="0"/>
-        <v>16858442.601016857</v>
+        <f t="shared" si="1"/>
+        <v>16875000</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" si="1"/>
-        <v>13112122.023013109</v>
+        <f t="shared" si="2"/>
+        <v>13125000</v>
       </c>
       <c r="G18" s="4">
         <v>221</v>
@@ -5618,8 +5674,11 @@
       <c r="H18" s="6" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" s="12">
+        <v>21000000.000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>555</v>
       </c>
@@ -5630,16 +5689,16 @@
         <v>251000000</v>
       </c>
       <c r="D19" s="7">
-        <f>VLOOKUP(B19,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>18731602.890018728</v>
+        <f t="shared" si="0"/>
+        <v>18750000</v>
       </c>
       <c r="E19" s="7">
-        <f t="shared" ref="E19" si="2">D19*90%</f>
-        <v>16858442.601016857</v>
+        <f t="shared" ref="E19" si="3">D19*90%</f>
+        <v>16875000</v>
       </c>
       <c r="F19" s="7">
-        <f t="shared" ref="F19" si="3">D19*70%</f>
-        <v>13112122.023013109</v>
+        <f t="shared" ref="F19" si="4">D19*70%</f>
+        <v>13125000</v>
       </c>
       <c r="G19" s="4">
         <v>221</v>
@@ -5647,8 +5706,11 @@
       <c r="H19" s="6" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" s="12">
+        <v>21000000.000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>500</v>
       </c>
@@ -5659,16 +5721,16 @@
         <v>251000000</v>
       </c>
       <c r="D20" s="7">
-        <f>VLOOKUP(B20,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>18731602.890018728</v>
+        <f t="shared" si="0"/>
+        <v>18750000</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="0"/>
-        <v>16858442.601016857</v>
+        <f t="shared" si="1"/>
+        <v>16875000</v>
       </c>
       <c r="F20" s="7">
-        <f t="shared" si="1"/>
-        <v>13112122.023013109</v>
+        <f t="shared" si="2"/>
+        <v>13125000</v>
       </c>
       <c r="G20" s="4">
         <v>243</v>
@@ -5676,8 +5738,11 @@
       <c r="H20" s="6" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="12">
+        <v>21000000.000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>501</v>
       </c>
@@ -5688,16 +5753,16 @@
         <v>251000000</v>
       </c>
       <c r="D21" s="7">
-        <f>VLOOKUP(B21,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>18731602.890018728</v>
+        <f t="shared" si="0"/>
+        <v>18750000</v>
       </c>
       <c r="E21" s="7">
-        <f t="shared" si="0"/>
-        <v>16858442.601016857</v>
+        <f t="shared" si="1"/>
+        <v>16875000</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" si="1"/>
-        <v>13112122.023013109</v>
+        <f t="shared" si="2"/>
+        <v>13125000</v>
       </c>
       <c r="G21" s="4">
         <v>250</v>
@@ -5705,8 +5770,11 @@
       <c r="H21" s="6" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" s="12">
+        <v>21000000.000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>502</v>
       </c>
@@ -5717,16 +5785,16 @@
         <v>307500000</v>
       </c>
       <c r="D22" s="7">
-        <f>VLOOKUP(B22,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>22299527.2500223</v>
+        <f t="shared" si="0"/>
+        <v>22321428.571428567</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" si="0"/>
-        <v>20069574.52502007</v>
+        <f t="shared" si="1"/>
+        <v>20089285.714285713</v>
       </c>
       <c r="F22" s="7">
-        <f t="shared" si="1"/>
-        <v>15609669.075015608</v>
+        <f t="shared" si="2"/>
+        <v>15624999.999999996</v>
       </c>
       <c r="G22" s="4">
         <v>235</v>
@@ -5734,8 +5802,11 @@
       <c r="H22" s="6" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22" s="12">
+        <v>24999999.999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>503</v>
       </c>
@@ -5746,16 +5817,16 @@
         <v>353000000</v>
       </c>
       <c r="D23" s="7">
-        <f>VLOOKUP(B23,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>25867451.610025868</v>
+        <f t="shared" si="0"/>
+        <v>25892857.142857142</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" si="0"/>
-        <v>23280706.44902328</v>
+        <f t="shared" si="1"/>
+        <v>23303571.428571429</v>
       </c>
       <c r="F23" s="7">
-        <f t="shared" si="1"/>
-        <v>18107216.127018105</v>
+        <f t="shared" si="2"/>
+        <v>18124999.999999996</v>
       </c>
       <c r="G23" s="4">
         <v>246</v>
@@ -5763,8 +5834,11 @@
       <c r="H23" s="6" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23" s="12">
+        <v>29000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>504</v>
       </c>
@@ -5775,16 +5849,16 @@
         <v>363000000</v>
       </c>
       <c r="D24" s="7">
-        <f>VLOOKUP(B24,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>26759432.700026754</v>
+        <f t="shared" si="0"/>
+        <v>26785714.285714284</v>
       </c>
       <c r="E24" s="7">
-        <f t="shared" si="0"/>
-        <v>24083489.43002408</v>
+        <f t="shared" si="1"/>
+        <v>24107142.857142854</v>
       </c>
       <c r="F24" s="7">
-        <f t="shared" si="1"/>
-        <v>18731602.890018728</v>
+        <f t="shared" si="2"/>
+        <v>18749999.999999996</v>
       </c>
       <c r="G24" s="4">
         <v>247</v>
@@ -5792,8 +5866,11 @@
       <c r="H24" s="6" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" s="12">
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>505</v>
       </c>
@@ -5804,16 +5881,16 @@
         <v>413000000</v>
       </c>
       <c r="D25" s="7">
-        <f>VLOOKUP(B25,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>30327357.060030323</v>
+        <f t="shared" si="0"/>
+        <v>30357142.857142854</v>
       </c>
       <c r="E25" s="7">
-        <f t="shared" si="0"/>
-        <v>27294621.35402729</v>
+        <f t="shared" si="1"/>
+        <v>27321428.571428571</v>
       </c>
       <c r="F25" s="7">
-        <f t="shared" si="1"/>
-        <v>21229149.942021225</v>
+        <f t="shared" si="2"/>
+        <v>21249999.999999996</v>
       </c>
       <c r="G25" s="4">
         <v>248</v>
@@ -5821,8 +5898,11 @@
       <c r="H25" s="6" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" s="12">
+        <v>34000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>585</v>
       </c>
@@ -5833,15 +5913,15 @@
         <v>318000000</v>
       </c>
       <c r="D26" s="7">
-        <f>26000000/1.12</f>
+        <f t="shared" si="0"/>
         <v>23214285.714285713</v>
       </c>
       <c r="E26" s="7">
-        <f t="shared" ref="E26:E27" si="4">D26*90%</f>
+        <f t="shared" ref="E26:E27" si="5">D26*90%</f>
         <v>20892857.142857142</v>
       </c>
       <c r="F26" s="7">
-        <f t="shared" ref="F26:F27" si="5">D26*70%</f>
+        <f t="shared" ref="F26:F27" si="6">D26*70%</f>
         <v>16249999.999999998</v>
       </c>
       <c r="G26" s="4">
@@ -5850,8 +5930,11 @@
       <c r="H26" s="6" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26" s="12">
+        <v>26000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>586</v>
       </c>
@@ -5862,15 +5945,15 @@
         <v>363000000</v>
       </c>
       <c r="D27" s="7">
-        <f>29000000/1.12</f>
+        <f t="shared" si="0"/>
         <v>25892857.142857142</v>
       </c>
       <c r="E27" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23303571.428571429</v>
       </c>
       <c r="F27" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18124999.999999996</v>
       </c>
       <c r="G27" s="4">
@@ -5879,8 +5962,11 @@
       <c r="H27" s="6" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27" s="12">
+        <v>29000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>557</v>
       </c>
@@ -5891,16 +5977,16 @@
         <v>415000000</v>
       </c>
       <c r="D28" s="7">
-        <f>VLOOKUP(B28,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33003300.330032997</v>
+        <f t="shared" si="0"/>
+        <v>33035714.285714284</v>
       </c>
       <c r="E28" s="7">
-        <f t="shared" si="0"/>
-        <v>29702970.297029696</v>
+        <f t="shared" si="1"/>
+        <v>29732142.857142854</v>
       </c>
       <c r="F28" s="7">
-        <f t="shared" si="1"/>
-        <v>23102310.231023096</v>
+        <f t="shared" si="2"/>
+        <v>23124999.999999996</v>
       </c>
       <c r="G28" s="4">
         <v>251</v>
@@ -5908,8 +5994,11 @@
       <c r="H28" s="6" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28" s="12">
+        <v>37000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>582</v>
       </c>
@@ -5920,16 +6009,16 @@
         <v>415000000</v>
       </c>
       <c r="D29" s="7">
-        <f>VLOOKUP(B29,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33003300.330032997</v>
+        <f t="shared" si="0"/>
+        <v>33035714.285714284</v>
       </c>
       <c r="E29" s="7">
-        <f t="shared" ref="E29" si="6">D29*90%</f>
-        <v>29702970.297029696</v>
+        <f t="shared" ref="E29" si="7">D29*90%</f>
+        <v>29732142.857142854</v>
       </c>
       <c r="F29" s="7">
-        <f t="shared" ref="F29" si="7">D29*70%</f>
-        <v>23102310.231023096</v>
+        <f t="shared" ref="F29" si="8">D29*70%</f>
+        <v>23124999.999999996</v>
       </c>
       <c r="G29" s="4">
         <v>251</v>
@@ -5937,8 +6026,11 @@
       <c r="H29" s="6" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29" s="12">
+        <v>37000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>558</v>
       </c>
@@ -5949,16 +6041,16 @@
         <v>443000000</v>
       </c>
       <c r="D30" s="7">
-        <f>VLOOKUP(B30,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33003300.330032997</v>
+        <f t="shared" si="0"/>
+        <v>33035714.285714284</v>
       </c>
       <c r="E30" s="7">
-        <f t="shared" ref="E30" si="8">D30*90%</f>
-        <v>29702970.297029696</v>
+        <f t="shared" ref="E30" si="9">D30*90%</f>
+        <v>29732142.857142854</v>
       </c>
       <c r="F30" s="7">
-        <f t="shared" ref="F30" si="9">D30*70%</f>
-        <v>23102310.231023096</v>
+        <f t="shared" ref="F30" si="10">D30*70%</f>
+        <v>23124999.999999996</v>
       </c>
       <c r="G30" s="4">
         <v>249</v>
@@ -5966,8 +6058,11 @@
       <c r="H30" s="6" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30" s="12">
+        <v>37000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>506</v>
       </c>
@@ -5978,16 +6073,16 @@
         <v>443000000</v>
       </c>
       <c r="D31" s="7">
-        <f>VLOOKUP(B31,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33003300.330032997</v>
+        <f t="shared" si="0"/>
+        <v>33035714.285714284</v>
       </c>
       <c r="E31" s="7">
         <f>D31*90%</f>
-        <v>29702970.297029696</v>
+        <v>29732142.857142854</v>
       </c>
       <c r="F31" s="7">
         <f>D31*70%</f>
-        <v>23102310.231023096</v>
+        <v>23124999.999999996</v>
       </c>
       <c r="G31" s="4">
         <v>249</v>
@@ -5995,8 +6090,11 @@
       <c r="H31" s="6" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31" s="12">
+        <v>37000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>529</v>
       </c>
@@ -6007,16 +6105,16 @@
         <v>155700000</v>
       </c>
       <c r="D32" s="7">
-        <f>VLOOKUP(B32,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>10882169.29801088</v>
+        <f t="shared" si="0"/>
+        <v>10892857.142857142</v>
       </c>
       <c r="E32" s="7">
         <f>D32*90%</f>
-        <v>9793952.3682097923</v>
+        <v>9803571.4285714272</v>
       </c>
       <c r="F32" s="7">
         <f>D32*70%</f>
-        <v>7617518.5086076157</v>
+        <v>7624999.9999999991</v>
       </c>
       <c r="G32" s="4">
         <v>201</v>
@@ -6024,8 +6122,11 @@
       <c r="H32" s="6" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32" s="12">
+        <v>12200000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>520</v>
       </c>
@@ -6036,16 +6137,16 @@
         <v>172600000</v>
       </c>
       <c r="D33" s="7">
-        <f>VLOOKUP(B33,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>7135848.7200071355</v>
+        <f t="shared" si="0"/>
+        <v>7142857.1428571418</v>
       </c>
       <c r="E33" s="7">
         <f>D33*90%</f>
-        <v>6422263.8480064217</v>
+        <v>6428571.4285714282</v>
       </c>
       <c r="F33" s="7">
         <f>D33*70%</f>
-        <v>4995094.104004995</v>
+        <v>4999999.9999999991</v>
       </c>
       <c r="G33" s="4">
         <v>230</v>
@@ -6053,8 +6154,11 @@
       <c r="H33" s="6" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33" s="12">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>521</v>
       </c>
@@ -6065,16 +6169,16 @@
         <v>176000000</v>
       </c>
       <c r="D34" s="7">
-        <f>VLOOKUP(B34,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>12041744.715012042</v>
+        <f t="shared" si="0"/>
+        <v>12053571.428571427</v>
       </c>
       <c r="E34" s="7">
         <f>D34*90%</f>
-        <v>10837570.243510839</v>
+        <v>10848214.285714285</v>
       </c>
       <c r="F34" s="7">
         <f>D34*70%</f>
-        <v>8429221.3005084284</v>
+        <v>8437499.9999999981</v>
       </c>
       <c r="G34" s="4">
         <v>238</v>
@@ -6082,8 +6186,11 @@
       <c r="H34" s="6" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34" s="12">
+        <v>13500000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>526</v>
       </c>
@@ -6094,16 +6201,16 @@
         <v>168000000</v>
       </c>
       <c r="D35" s="7">
-        <f>VLOOKUP(B35,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>11149763.62501115</v>
+        <f t="shared" si="0"/>
+        <v>11160714.285714284</v>
       </c>
       <c r="E35" s="7">
         <f>D35*90%</f>
-        <v>10034787.262510035</v>
+        <v>10044642.857142856</v>
       </c>
       <c r="F35" s="7">
         <f>D35*70%</f>
-        <v>7804834.5375078041</v>
+        <v>7812499.9999999981</v>
       </c>
       <c r="G35" s="4">
         <v>237</v>
@@ -6111,8 +6218,11 @@
       <c r="H35" s="6" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35" s="12">
+        <v>12499999.999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>560</v>
       </c>
@@ -6123,16 +6233,16 @@
         <v>188300000</v>
       </c>
       <c r="D36" s="7">
-        <f>VLOOKUP(B36,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>11328159.843011327</v>
+        <f t="shared" si="0"/>
+        <v>11339285.714285715</v>
       </c>
       <c r="E36" s="7">
-        <f t="shared" ref="E36:E37" si="10">D36*90%</f>
-        <v>10195343.858710194</v>
+        <f t="shared" ref="E36:E37" si="11">D36*90%</f>
+        <v>10205357.142857144</v>
       </c>
       <c r="F36" s="7">
-        <f t="shared" ref="F36:F37" si="11">D36*70%</f>
-        <v>7929711.8901079288</v>
+        <f t="shared" ref="F36:F37" si="12">D36*70%</f>
+        <v>7937500</v>
       </c>
       <c r="G36" s="4">
         <v>202</v>
@@ -6140,8 +6250,11 @@
       <c r="H36" s="6" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36" s="12">
+        <v>12700000.000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>561</v>
       </c>
@@ -6152,16 +6265,16 @@
         <v>443000000</v>
       </c>
       <c r="D37" s="7">
-        <f>VLOOKUP(B37,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>33003300.330032997</v>
+        <f t="shared" si="0"/>
+        <v>33035714.285714284</v>
       </c>
       <c r="E37" s="7">
-        <f t="shared" si="10"/>
-        <v>29702970.297029696</v>
+        <f t="shared" si="11"/>
+        <v>29732142.857142854</v>
       </c>
       <c r="F37" s="7">
-        <f t="shared" si="11"/>
-        <v>23102310.231023096</v>
+        <f t="shared" si="12"/>
+        <v>23124999.999999996</v>
       </c>
       <c r="G37" s="4">
         <v>249</v>
@@ -6169,8 +6282,11 @@
       <c r="H37" s="6" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37" s="12">
+        <v>37000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>522</v>
       </c>
@@ -6181,22 +6297,25 @@
         <v>345650000</v>
       </c>
       <c r="D38" s="7">
-        <f>VLOOKUP(B38,[1]pricelist!$B$3:$H$53,7,0)*1000/1.01</f>
-        <v>22834715.904022835</v>
+        <f t="shared" si="0"/>
+        <v>22857142.857142854</v>
       </c>
       <c r="E38" s="7">
-        <f t="shared" ref="E38" si="12">D38*90%</f>
-        <v>20551244.313620552</v>
+        <f t="shared" ref="E38" si="13">D38*90%</f>
+        <v>20571428.571428571</v>
       </c>
       <c r="F38" s="7">
-        <f t="shared" ref="F38" si="13">D38*70%</f>
-        <v>15984301.132815983</v>
+        <f t="shared" ref="F38" si="14">D38*70%</f>
+        <v>15999999.999999996</v>
       </c>
       <c r="G38" s="4">
         <v>233</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>567</v>
+      </c>
+      <c r="I38" s="12">
+        <v>25600000</v>
       </c>
     </row>
   </sheetData>
@@ -7240,15 +7359,15 @@
       </c>
       <c r="D2" s="7">
         <f>VLOOKUP(B2,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>31531.531531531527</v>
+        <v>31249.999999999996</v>
       </c>
       <c r="E2" s="7">
         <f>D2*90%</f>
-        <v>28378.378378378377</v>
+        <v>28124.999999999996</v>
       </c>
       <c r="F2" s="7">
         <f>D2*70%</f>
-        <v>22072.072072072067</v>
+        <v>21874.999999999996</v>
       </c>
       <c r="G2" s="9">
         <v>228</v>
@@ -7270,15 +7389,15 @@
       </c>
       <c r="D3" s="7">
         <f>VLOOKUP(B3,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>29729.729729729726</v>
+        <v>29464.28571428571</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" ref="E3:E34" si="0">D3*90%</f>
-        <v>26756.756756756753</v>
+        <v>26517.857142857141</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" ref="F3:F34" si="1">D3*70%</f>
-        <v>20810.810810810806</v>
+        <v>20624.999999999996</v>
       </c>
       <c r="G3" s="9">
         <v>227</v>
@@ -7300,15 +7419,15 @@
       </c>
       <c r="D4" s="7">
         <f>VLOOKUP(B4,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>20945.945945945943</v>
+        <v>20758.928571428569</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="0"/>
-        <v>18851.35135135135</v>
+        <v>18683.035714285714</v>
       </c>
       <c r="F4" s="7">
         <f t="shared" si="1"/>
-        <v>14662.16216216216</v>
+        <v>14531.249999999996</v>
       </c>
       <c r="G4" s="9">
         <v>222</v>
@@ -7330,15 +7449,15 @@
       </c>
       <c r="D5" s="7">
         <f>VLOOKUP(B5,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>22252.252252252249</v>
+        <v>22053.571428571428</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>20027.027027027023</v>
+        <v>19848.214285714286</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="1"/>
-        <v>15576.576576576574</v>
+        <v>15437.499999999998</v>
       </c>
       <c r="G5" s="9">
         <v>223</v>
@@ -7360,15 +7479,15 @@
       </c>
       <c r="D6" s="7">
         <f>VLOOKUP(B6,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>31531.531531531527</v>
+        <v>31249.999999999996</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="0"/>
-        <v>28378.378378378377</v>
+        <v>28124.999999999996</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="1"/>
-        <v>22072.072072072067</v>
+        <v>21874.999999999996</v>
       </c>
       <c r="G6" s="9">
         <v>244</v>
@@ -7390,15 +7509,15 @@
       </c>
       <c r="D7" s="7">
         <f>VLOOKUP(B7,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>34234.234234234231</v>
+        <v>33928.571428571428</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
-        <v>30810.81081081081</v>
+        <v>30535.714285714286</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="1"/>
-        <v>23963.963963963961</v>
+        <v>23749.999999999996</v>
       </c>
       <c r="G7" s="9">
         <v>245</v>
@@ -7420,15 +7539,15 @@
       </c>
       <c r="D8" s="7">
         <f>VLOOKUP(B8,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>20720.720720720718</v>
+        <v>20535.714285714283</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
-        <v>18648.648648648646</v>
+        <v>18482.142857142855</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>14504.504504504501</v>
+        <v>14374.999999999996</v>
       </c>
       <c r="G8" s="4">
         <v>240</v>
@@ -7450,15 +7569,15 @@
       </c>
       <c r="D9" s="7">
         <f>VLOOKUP(B9,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>18018.018018018018</v>
+        <v>17857.142857142855</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="0"/>
-        <v>16216.216216216217</v>
+        <v>16071.428571428571</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>12612.612612612611</v>
+        <v>12499.999999999998</v>
       </c>
       <c r="G9" s="4">
         <v>241</v>
@@ -7480,15 +7599,15 @@
       </c>
       <c r="D10" s="7">
         <f>VLOOKUP(B10,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>11711.71171171171</v>
+        <v>11607.142857142857</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>10540.54054054054</v>
+        <v>10446.428571428571</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="1"/>
-        <v>8198.1981981981971</v>
+        <v>8124.9999999999991</v>
       </c>
       <c r="G10" s="4">
         <v>242</v>
@@ -7510,15 +7629,15 @@
       </c>
       <c r="D11" s="7">
         <f>VLOOKUP(B11,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>11441.44144144144</v>
+        <v>11339.285714285714</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
-        <v>10297.297297297297</v>
+        <v>10205.357142857143</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="1"/>
-        <v>8009.009009009008</v>
+        <v>7937.4999999999991</v>
       </c>
       <c r="G11" s="4">
         <v>202</v>
@@ -7540,15 +7659,15 @@
       </c>
       <c r="D12" s="7">
         <f>VLOOKUP(B12,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>14414.414414414414</v>
+        <v>14285.714285714284</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
-        <v>12972.972972972973</v>
+        <v>12857.142857142857</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="1"/>
-        <v>10090.090090090089</v>
+        <v>9999.9999999999982</v>
       </c>
       <c r="G12" s="4">
         <v>204</v>
@@ -7570,15 +7689,15 @@
       </c>
       <c r="D13" s="7">
         <f>VLOOKUP(B13,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>13243.243243243242</v>
+        <v>13124.999999999998</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="0"/>
-        <v>11918.918918918918</v>
+        <v>11812.499999999998</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="1"/>
-        <v>9270.2702702702682</v>
+        <v>9187.4999999999982</v>
       </c>
       <c r="G13" s="4">
         <v>205</v>
@@ -7600,15 +7719,15 @@
       </c>
       <c r="D14" s="7">
         <f>VLOOKUP(B14,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>18828.828828828828</v>
+        <v>18660.714285714283</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
-        <v>16945.945945945947</v>
+        <v>16794.642857142855</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="1"/>
-        <v>13180.180180180179</v>
+        <v>13062.499999999996</v>
       </c>
       <c r="G14" s="4">
         <v>213</v>
@@ -7630,15 +7749,15 @@
       </c>
       <c r="D15" s="7">
         <f>VLOOKUP(B15,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>19819.819819819819</v>
+        <v>19642.857142857141</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
-        <v>17837.837837837837</v>
+        <v>17678.571428571428</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
-        <v>13873.873873873872</v>
+        <v>13749.999999999998</v>
       </c>
       <c r="G15" s="4">
         <v>214</v>
@@ -7660,15 +7779,15 @@
       </c>
       <c r="D16" s="7">
         <f>VLOOKUP(B16,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>16486.486486486487</v>
+        <v>16339.285714285712</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
-        <v>14837.837837837838</v>
+        <v>14705.357142857141</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="1"/>
-        <v>11540.54054054054</v>
+        <v>11437.499999999998</v>
       </c>
       <c r="G16" s="4">
         <v>209</v>
@@ -7690,15 +7809,15 @@
       </c>
       <c r="D17" s="7">
         <f>VLOOKUP(B17,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>18468.468468468465</v>
+        <v>18303.571428571428</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
-        <v>16621.62162162162</v>
+        <v>16473.214285714286</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="1"/>
-        <v>12927.927927927925</v>
+        <v>12812.499999999998</v>
       </c>
       <c r="G17" s="4">
         <v>220</v>
@@ -7720,15 +7839,15 @@
       </c>
       <c r="D18" s="7">
         <f>VLOOKUP(B18,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>18918.918918918916</v>
+        <v>18750</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
-        <v>17027.027027027027</v>
+        <v>16875</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>13243.243243243242</v>
+        <v>13125</v>
       </c>
       <c r="G18" s="4">
         <v>221</v>
@@ -7750,15 +7869,15 @@
       </c>
       <c r="D19" s="7">
         <f>VLOOKUP(B19,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>18918.918918918916</v>
+        <v>18750</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="0"/>
-        <v>17027.027027027027</v>
+        <v>16875</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="1"/>
-        <v>13243.243243243242</v>
+        <v>13125</v>
       </c>
       <c r="G19" s="4">
         <v>243</v>
@@ -7780,15 +7899,15 @@
       </c>
       <c r="D20" s="7">
         <f>VLOOKUP(B20,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>18918.918918918916</v>
+        <v>18750</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
-        <v>17027.027027027027</v>
+        <v>16875</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="1"/>
-        <v>13243.243243243242</v>
+        <v>13125</v>
       </c>
       <c r="G20" s="4">
         <v>250</v>
@@ -7810,15 +7929,15 @@
       </c>
       <c r="D21" s="7">
         <f>VLOOKUP(B21,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>22522.522522522522</v>
+        <v>22321.428571428569</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" si="0"/>
-        <v>20270.27027027027</v>
+        <v>20089.285714285714</v>
       </c>
       <c r="F21" s="7">
         <f t="shared" si="1"/>
-        <v>15765.765765765764</v>
+        <v>15624.999999999996</v>
       </c>
       <c r="G21" s="4">
         <v>235</v>
@@ -7840,15 +7959,15 @@
       </c>
       <c r="D22" s="7">
         <f>VLOOKUP(B22,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>26126.126126126124</v>
+        <v>25892.857142857141</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
-        <v>23513.513513513513</v>
+        <v>23303.571428571428</v>
       </c>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>18288.288288288284</v>
+        <v>18124.999999999996</v>
       </c>
       <c r="G22" s="4">
         <v>246</v>
@@ -7870,15 +7989,15 @@
       </c>
       <c r="D23" s="7">
         <f>VLOOKUP(B23,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>27027.027027027023</v>
+        <v>26785.714285714283</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>24324.32432432432</v>
+        <v>24107.142857142855</v>
       </c>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>18918.918918918916</v>
+        <v>18749.999999999996</v>
       </c>
       <c r="G23" s="4">
         <v>247</v>
@@ -7900,15 +8019,15 @@
       </c>
       <c r="D24" s="7">
         <f>VLOOKUP(B24,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>30630.630630630629</v>
+        <v>30357.142857142855</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
-        <v>27567.567567567567</v>
+        <v>27321.428571428569</v>
       </c>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>21441.441441441439</v>
+        <v>21249.999999999996</v>
       </c>
       <c r="G24" s="4">
         <v>248</v>
@@ -7930,15 +8049,15 @@
       </c>
       <c r="D25" s="7">
         <f>VLOOKUP(B25,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>33333.333333333328</v>
+        <v>33035.714285714283</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" si="0"/>
-        <v>29999.999999999996</v>
+        <v>29732.142857142855</v>
       </c>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>23333.333333333328</v>
+        <v>23124.999999999996</v>
       </c>
       <c r="G25" s="4">
         <v>251</v>
@@ -7960,15 +8079,15 @@
       </c>
       <c r="D26" s="7">
         <f>VLOOKUP(B26,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>33333.333333333328</v>
+        <v>33035.714285714283</v>
       </c>
       <c r="E26" s="7">
         <f t="shared" si="0"/>
-        <v>29999.999999999996</v>
+        <v>29732.142857142855</v>
       </c>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>23333.333333333328</v>
+        <v>23124.999999999996</v>
       </c>
       <c r="G26" s="4">
         <v>249</v>
@@ -7990,15 +8109,15 @@
       </c>
       <c r="D27" s="7">
         <f>VLOOKUP(B27,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>33333.333333333328</v>
+        <v>33035.714285714283</v>
       </c>
       <c r="E27" s="7">
         <f t="shared" si="0"/>
-        <v>29999.999999999996</v>
+        <v>29732.142857142855</v>
       </c>
       <c r="F27" s="7">
         <f t="shared" si="1"/>
-        <v>23333.333333333328</v>
+        <v>23124.999999999996</v>
       </c>
       <c r="G27" s="4">
         <v>249</v>
@@ -8020,15 +8139,15 @@
       </c>
       <c r="D28" s="7">
         <f>VLOOKUP(B28,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>10990.990990990989</v>
+        <v>10892.857142857141</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>9891.8918918918898</v>
+        <v>9803.5714285714275</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>7693.6936936936918</v>
+        <v>7624.9999999999982</v>
       </c>
       <c r="G28" s="4">
         <v>201</v>
@@ -8050,15 +8169,15 @@
       </c>
       <c r="D29" s="7">
         <f>VLOOKUP(B29,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>7207.2072072072069</v>
+        <v>7142.8571428571422</v>
       </c>
       <c r="E29" s="7">
         <f t="shared" si="0"/>
-        <v>6486.4864864864867</v>
+        <v>6428.5714285714284</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>5045.0450450450444</v>
+        <v>4999.9999999999991</v>
       </c>
       <c r="G29" s="4">
         <v>230</v>
@@ -8080,15 +8199,15 @@
       </c>
       <c r="D30" s="7">
         <f>VLOOKUP(B30,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>12162.162162162162</v>
+        <v>12053.571428571428</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="0"/>
-        <v>10945.945945945945</v>
+        <v>10848.214285714284</v>
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>8513.5135135135133</v>
+        <v>8437.4999999999982</v>
       </c>
       <c r="G30" s="4">
         <v>238</v>
@@ -8110,15 +8229,15 @@
       </c>
       <c r="D31" s="7">
         <f>VLOOKUP(B31,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>11261.261261261261</v>
+        <v>11160.714285714284</v>
       </c>
       <c r="E31" s="7">
         <f t="shared" si="0"/>
-        <v>10135.135135135135</v>
+        <v>10044.642857142857</v>
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>7882.8828828828819</v>
+        <v>7812.4999999999982</v>
       </c>
       <c r="G31" s="4">
         <v>237</v>
@@ -8140,15 +8259,15 @@
       </c>
       <c r="D32" s="7">
         <f>VLOOKUP(B32,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>11441.44144144144</v>
+        <v>11339.285714285714</v>
       </c>
       <c r="E32" s="7">
         <f t="shared" si="0"/>
-        <v>10297.297297297297</v>
+        <v>10205.357142857143</v>
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>8009.009009009008</v>
+        <v>7937.4999999999991</v>
       </c>
       <c r="G32" s="4">
         <v>202</v>
@@ -8170,15 +8289,15 @@
       </c>
       <c r="D33" s="7">
         <f>VLOOKUP(B33,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>33333.333333333328</v>
+        <v>33035.714285714283</v>
       </c>
       <c r="E33" s="7">
         <f t="shared" si="0"/>
-        <v>29999.999999999996</v>
+        <v>29732.142857142855</v>
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>23333.333333333328</v>
+        <v>23124.999999999996</v>
       </c>
       <c r="G33" s="4">
         <v>249</v>
@@ -8200,15 +8319,15 @@
       </c>
       <c r="D34" s="7">
         <f>VLOOKUP(B34,[1]pricelist!$B$3:$H$53,7,0)</f>
-        <v>23063.063063063062</v>
+        <v>22857.142857142855</v>
       </c>
       <c r="E34" s="7">
         <f t="shared" si="0"/>
-        <v>20756.756756756757</v>
+        <v>20571.428571428569</v>
       </c>
       <c r="F34" s="7">
         <f t="shared" si="1"/>
-        <v>16144.144144144142</v>
+        <v>15999.999999999998</v>
       </c>
       <c r="G34" s="4">
         <v>233</v>

</xml_diff>

<commit_message>
UPDATE: Changed name in pricelist
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F554F98E-42E8-4DBA-8F4A-D988EED529AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B0C069-3BEA-42CF-BEFE-825C639BCFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -2327,13 +2327,13 @@
     <t>New Binguo EV Pro</t>
   </si>
   <si>
-    <t>E260R EV 50ZW333LV0Y2A</t>
-  </si>
-  <si>
-    <t>E260R EV 50ZW333LV1Y2A</t>
-  </si>
-  <si>
     <t>Full Margin</t>
+  </si>
+  <si>
+    <t>E260R EV 50ZW333LV0YID (4X2) A/T</t>
+  </si>
+  <si>
+    <t>E260R EV 50ZW333LV1YID (4X2) A/T</t>
   </si>
 </sst>
 </file>
@@ -5061,8 +5061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05C9E0-A64E-40AC-B9F4-C919ED5906CC}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5126,7 +5126,7 @@
         <v>564</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -5904,7 +5904,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>583</v>
@@ -5936,7 +5936,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>584</v>

</xml_diff>

<commit_message>
UPDATE: Added New Binguo Pro Price
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gp-app\gp-app-1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B0C069-3BEA-42CF-BEFE-825C639BCFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7B096C-A0CE-4824-964F-64EA1F07D5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="589">
   <si>
     <t>Column1</t>
   </si>
@@ -2334,6 +2334,9 @@
   </si>
   <si>
     <t>E260R EV 50ZW333LV1YID (4X2) A/T</t>
+  </si>
+  <si>
+    <t>E260R EV 50KW333LV1YID (4X2) A/T</t>
   </si>
 </sst>
 </file>
@@ -5059,10 +5062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05C9E0-A64E-40AC-B9F4-C919ED5906CC}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5172,15 +5175,15 @@
         <v>388500000</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" ref="D3:D38" si="0">I3/1.12</f>
+        <f t="shared" ref="D3:D39" si="0">I3/1.12</f>
         <v>29464285.714285709</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E28" si="1">D3*90%</f>
+        <f t="shared" ref="E3:E29" si="1">D3*90%</f>
         <v>26517857.142857138</v>
       </c>
       <c r="F3" s="7">
-        <f t="shared" ref="F3:F28" si="2">D3*70%</f>
+        <f t="shared" ref="F3:F29" si="2">D3*70%</f>
         <v>20624999.999999996</v>
       </c>
       <c r="G3" s="9">
@@ -5872,135 +5875,135 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="C25" s="7">
+        <v>363000000</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" ref="D25" si="5">I25/1.12</f>
+        <v>25892857.142857142</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="1"/>
+        <v>23303571.428571429</v>
+      </c>
+      <c r="F25" s="7">
+        <f t="shared" si="2"/>
+        <v>18124999.999999996</v>
+      </c>
+      <c r="G25" s="4">
+        <v>253</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="I25" s="12">
+        <v>29000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C26" s="7">
         <v>413000000</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D26" s="7">
         <f t="shared" si="0"/>
         <v>30357142.857142854</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E26" s="7">
         <f t="shared" si="1"/>
         <v>27321428.571428571</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F26" s="7">
         <f t="shared" si="2"/>
         <v>21249999.999999996</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G26" s="4">
         <v>248</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>578</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I26" s="12">
         <v>34000000</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
         <v>586</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C27" s="7">
         <v>318000000</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D27" s="7">
         <f t="shared" si="0"/>
         <v>23214285.714285713</v>
       </c>
-      <c r="E26" s="7">
-        <f t="shared" ref="E26:E27" si="5">D26*90%</f>
+      <c r="E27" s="7">
+        <f t="shared" ref="E27:E28" si="6">D27*90%</f>
         <v>20892857.142857142</v>
       </c>
-      <c r="F26" s="7">
-        <f t="shared" ref="F26:F27" si="6">D26*70%</f>
+      <c r="F27" s="7">
+        <f t="shared" ref="F27:F28" si="7">D27*70%</f>
         <v>16249999.999999998</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G27" s="4">
         <v>252</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>576</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I27" s="12">
         <v>26000000</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
         <v>587</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>584</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C28" s="7">
         <v>363000000</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D28" s="7">
         <f t="shared" si="0"/>
         <v>25892857.142857142</v>
       </c>
-      <c r="E27" s="7">
-        <f t="shared" si="5"/>
+      <c r="E28" s="7">
+        <f t="shared" si="6"/>
         <v>23303571.428571429</v>
       </c>
-      <c r="F27" s="7">
-        <f t="shared" si="6"/>
+      <c r="F28" s="7">
+        <f t="shared" si="7"/>
         <v>18124999.999999996</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G28" s="4">
         <v>253</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>577</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I28" s="12">
         <v>29000000</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
         <v>557</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="C28" s="7">
-        <v>415000000</v>
-      </c>
-      <c r="D28" s="7">
-        <f t="shared" si="0"/>
-        <v>33035714.285714284</v>
-      </c>
-      <c r="E28" s="7">
-        <f t="shared" si="1"/>
-        <v>29732142.857142854</v>
-      </c>
-      <c r="F28" s="7">
-        <f t="shared" si="2"/>
-        <v>23124999.999999996</v>
-      </c>
-      <c r="G28" s="4">
-        <v>251</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>581</v>
-      </c>
-      <c r="I28" s="12">
-        <v>37000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>582</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>559</v>
@@ -6013,11 +6016,11 @@
         <v>33035714.285714284</v>
       </c>
       <c r="E29" s="7">
-        <f t="shared" ref="E29" si="7">D29*90%</f>
+        <f t="shared" si="1"/>
         <v>29732142.857142854</v>
       </c>
       <c r="F29" s="7">
-        <f t="shared" ref="F29" si="8">D29*70%</f>
+        <f t="shared" si="2"/>
         <v>23124999.999999996</v>
       </c>
       <c r="G29" s="4">
@@ -6031,32 +6034,32 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>558</v>
+      <c r="A30" t="s">
+        <v>582</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>512</v>
+        <v>559</v>
       </c>
       <c r="C30" s="7">
-        <v>443000000</v>
+        <v>415000000</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" si="0"/>
         <v>33035714.285714284</v>
       </c>
       <c r="E30" s="7">
-        <f t="shared" ref="E30" si="9">D30*90%</f>
+        <f t="shared" ref="E30" si="8">D30*90%</f>
         <v>29732142.857142854</v>
       </c>
       <c r="F30" s="7">
-        <f t="shared" ref="F30" si="10">D30*70%</f>
+        <f t="shared" ref="F30" si="9">D30*70%</f>
         <v>23124999.999999996</v>
       </c>
       <c r="G30" s="4">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
       <c r="I30" s="12">
         <v>37000000</v>
@@ -6064,7 +6067,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>506</v>
+        <v>558</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>512</v>
@@ -6077,11 +6080,11 @@
         <v>33035714.285714284</v>
       </c>
       <c r="E31" s="7">
-        <f>D31*90%</f>
+        <f t="shared" ref="E31" si="10">D31*90%</f>
         <v>29732142.857142854</v>
       </c>
       <c r="F31" s="7">
-        <f>D31*70%</f>
+        <f t="shared" ref="F31" si="11">D31*70%</f>
         <v>23124999.999999996</v>
       </c>
       <c r="G31" s="4">
@@ -6096,233 +6099,265 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>529</v>
+        <v>506</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
       <c r="C32" s="7">
-        <v>155700000</v>
+        <v>443000000</v>
       </c>
       <c r="D32" s="7">
         <f t="shared" si="0"/>
-        <v>10892857.142857142</v>
+        <v>33035714.285714284</v>
       </c>
       <c r="E32" s="7">
         <f>D32*90%</f>
-        <v>9803571.4285714272</v>
+        <v>29732142.857142854</v>
       </c>
       <c r="F32" s="7">
         <f>D32*70%</f>
-        <v>7624999.9999999991</v>
+        <v>23124999.999999996</v>
       </c>
       <c r="G32" s="4">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I32" s="12">
-        <v>12200000</v>
+        <v>37000000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>513</v>
+        <v>539</v>
       </c>
       <c r="C33" s="7">
-        <v>172600000</v>
+        <v>155700000</v>
       </c>
       <c r="D33" s="7">
         <f t="shared" si="0"/>
-        <v>7142857.1428571418</v>
+        <v>10892857.142857142</v>
       </c>
       <c r="E33" s="7">
         <f>D33*90%</f>
-        <v>6428571.4285714282</v>
+        <v>9803571.4285714272</v>
       </c>
       <c r="F33" s="7">
         <f>D33*70%</f>
-        <v>4999999.9999999991</v>
+        <v>7624999.9999999991</v>
       </c>
       <c r="G33" s="4">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>572</v>
       </c>
       <c r="I33" s="12">
-        <v>8000000</v>
+        <v>12200000</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>540</v>
+        <v>513</v>
       </c>
       <c r="C34" s="7">
-        <v>176000000</v>
+        <v>172600000</v>
       </c>
       <c r="D34" s="7">
         <f t="shared" si="0"/>
-        <v>12053571.428571427</v>
+        <v>7142857.1428571418</v>
       </c>
       <c r="E34" s="7">
         <f>D34*90%</f>
-        <v>10848214.285714285</v>
+        <v>6428571.4285714282</v>
       </c>
       <c r="F34" s="7">
         <f>D34*70%</f>
-        <v>8437499.9999999981</v>
+        <v>4999999.9999999991</v>
       </c>
       <c r="G34" s="4">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="I34" s="12">
-        <v>13500000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="C35" s="7">
-        <v>168000000</v>
+        <v>176000000</v>
       </c>
       <c r="D35" s="7">
         <f t="shared" si="0"/>
-        <v>11160714.285714284</v>
+        <v>12053571.428571427</v>
       </c>
       <c r="E35" s="7">
         <f>D35*90%</f>
-        <v>10044642.857142856</v>
+        <v>10848214.285714285</v>
       </c>
       <c r="F35" s="7">
         <f>D35*70%</f>
-        <v>7812499.9999999981</v>
+        <v>8437499.9999999981</v>
       </c>
       <c r="G35" s="4">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>579</v>
       </c>
       <c r="I35" s="12">
-        <v>12499999.999999998</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>560</v>
+        <v>526</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>535</v>
+        <v>545</v>
       </c>
       <c r="C36" s="7">
-        <v>188300000</v>
+        <v>168000000</v>
       </c>
       <c r="D36" s="7">
         <f t="shared" si="0"/>
-        <v>11339285.714285715</v>
+        <v>11160714.285714284</v>
       </c>
       <c r="E36" s="7">
-        <f t="shared" ref="E36:E37" si="11">D36*90%</f>
-        <v>10205357.142857144</v>
+        <f>D36*90%</f>
+        <v>10044642.857142856</v>
       </c>
       <c r="F36" s="7">
-        <f t="shared" ref="F36:F37" si="12">D36*70%</f>
-        <v>7937500</v>
+        <f>D36*70%</f>
+        <v>7812499.9999999981</v>
       </c>
       <c r="G36" s="4">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>568</v>
+        <v>579</v>
       </c>
       <c r="I36" s="12">
-        <v>12700000.000000002</v>
+        <v>12499999.999999998</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>512</v>
+        <v>535</v>
       </c>
       <c r="C37" s="7">
-        <v>443000000</v>
+        <v>188300000</v>
       </c>
       <c r="D37" s="7">
         <f t="shared" si="0"/>
-        <v>33035714.285714284</v>
+        <v>11339285.714285715</v>
       </c>
       <c r="E37" s="7">
-        <f t="shared" si="11"/>
-        <v>29732142.857142854</v>
+        <f t="shared" ref="E37:E38" si="12">D37*90%</f>
+        <v>10205357.142857144</v>
       </c>
       <c r="F37" s="7">
-        <f t="shared" si="12"/>
-        <v>23124999.999999996</v>
+        <f t="shared" ref="F37:F38" si="13">D37*70%</f>
+        <v>7937500</v>
       </c>
       <c r="G37" s="4">
-        <v>249</v>
+        <v>202</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="I37" s="12">
-        <v>37000000</v>
+        <v>12700000.000000002</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="8" t="s">
-        <v>522</v>
+      <c r="A38" s="6" t="s">
+        <v>561</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>550</v>
+        <v>512</v>
       </c>
       <c r="C38" s="7">
-        <v>345650000</v>
+        <v>443000000</v>
       </c>
       <c r="D38" s="7">
         <f t="shared" si="0"/>
+        <v>33035714.285714284</v>
+      </c>
+      <c r="E38" s="7">
+        <f t="shared" si="12"/>
+        <v>29732142.857142854</v>
+      </c>
+      <c r="F38" s="7">
+        <f t="shared" si="13"/>
+        <v>23124999.999999996</v>
+      </c>
+      <c r="G38" s="4">
+        <v>249</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="I38" s="12">
+        <v>37000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="C39" s="7">
+        <v>345650000</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="0"/>
         <v>22857142.857142854</v>
       </c>
-      <c r="E38" s="7">
-        <f t="shared" ref="E38" si="13">D38*90%</f>
+      <c r="E39" s="7">
+        <f t="shared" ref="E39" si="14">D39*90%</f>
         <v>20571428.571428571</v>
       </c>
-      <c r="F38" s="7">
-        <f t="shared" ref="F38" si="14">D38*70%</f>
+      <c r="F39" s="7">
+        <f t="shared" ref="F39" si="15">D39*70%</f>
         <v>15999999.999999996</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G39" s="4">
         <v>233</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H39" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="I38" s="12">
+      <c r="I39" s="12">
         <v>25600000</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A30:A37 A2:A28">
+  <conditionalFormatting sqref="A31:A38 A2:A29">
     <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30:A38 A2:A28">
+  <conditionalFormatting sqref="A31:A39 A2:A29">
     <cfRule type="duplicateValues" dxfId="2" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UPDATE: Pricelist added mini van and blind van EV (Mitra EV)
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7B096C-A0CE-4824-964F-64EA1F07D5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01E09BF-8E46-444D-A9D9-9201054E1B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="599">
   <si>
     <t>Column1</t>
   </si>
@@ -2337,6 +2337,36 @@
   </si>
   <si>
     <t>E260R EV 50KW333LV1YID (4X2) A/T</t>
+  </si>
+  <si>
+    <t>350VB E1C (4X2) A/T</t>
+  </si>
+  <si>
+    <t>350V E1C (4X2) A/T</t>
+  </si>
+  <si>
+    <t>350VB E2C (4X2) A/T</t>
+  </si>
+  <si>
+    <t>350V E2C (4X2) A/T</t>
+  </si>
+  <si>
+    <t>Mitra EV BV 300</t>
+  </si>
+  <si>
+    <t>Mitra EV MB 300</t>
+  </si>
+  <si>
+    <t>Mitra EV BV 400</t>
+  </si>
+  <si>
+    <t>Mitra EV MB 400</t>
+  </si>
+  <si>
+    <t>MITRA EV BV</t>
+  </si>
+  <si>
+    <t>MITRA EV MB</t>
   </si>
 </sst>
 </file>
@@ -2391,7 +2421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2425,6 +2455,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2432,15 +2558,13 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2450,9 +2574,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2460,7 +2604,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DA2601EE-1999-4BF8-AF5E-538A4398209C}"/>
     <cellStyle name="Normal 2 2" xfId="3" xr:uid="{8C240942-BC33-4996-847D-14CFBB46F4A3}"/>
   </cellStyles>
-  <dxfs count="136">
+  <dxfs count="149">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2500,6 +2644,329 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -4454,312 +4921,330 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}" name="Table001__Page_2" displayName="Table001__Page_2" ref="A1:G16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G16" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A26CE965-72B2-472B-B9FF-D68F7847F3C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="135"/>
-    <tableColumn id="2" xr3:uid="{375BF78E-5806-424A-B7BD-C63C40843BE9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="134"/>
-    <tableColumn id="3" xr3:uid="{CD1FFC74-B097-42B5-B1FA-08D3BD4531B9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="133"/>
-    <tableColumn id="4" xr3:uid="{EA6F5C08-47B3-4BE3-8F9B-3167F2B34338}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="132"/>
-    <tableColumn id="5" xr3:uid="{67D1B145-6151-4A54-9C79-A6B0381CDA09}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="131"/>
-    <tableColumn id="6" xr3:uid="{E8D8899E-ED32-4A2F-B13D-18F4C289A59B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="130"/>
-    <tableColumn id="7" xr3:uid="{CD1BCBB0-10DE-4DDA-903D-C14D16829749}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I43" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:I43" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0E6335F2-6B6A-436C-92FA-B48E61551308}" name="Merek/Type" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{5A4965DA-398A-4134-90BD-9CE4D8355880}" name="Tipe" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{010303D1-E0A2-4DE6-8E87-64ACC3102E09}" name="Harga OTR Awal" dataDxfId="10" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{91C798B0-7964-436A-84A5-7687993F376F}" name="Dealer Margin" dataDxfId="9" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{CD936623-36F3-4BAA-A615-AF79A61C51E8}" name="Dealer Margin 9 %" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{A36173E8-D9B2-4F38-A572-F5D32CDADEB8}" name="Dealer Margin 7 %" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{7A11B7F5-7683-492A-A8B5-D96984323DDD}" name="Code Unit" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{AF243BB3-2044-4D1E-9F0D-A1EC0D2C15CF}" name="Merk/Type" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{9E0E2E6A-108F-4ACE-959D-9EB0F753BD73}" name="Full Margin" dataDxfId="4"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}" name="Table010__Page_6" displayName="Table010__Page_6" ref="A18:I20" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A18:I20" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}" name="Table009__Page_6" displayName="Table009__Page_6" ref="A1:I16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D02866AC-7C8C-4041-B0D6-297717EA2BCA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{F9BA0334-AC0F-4599-91DD-1D3B53530BA2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{2E40CB08-FF90-4211-A5F6-3255AA5CEAED}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{951E49DE-3DB8-41C0-8F36-6E5A1649659D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{D7FC7D23-AA29-4FAE-8DF4-B23A11020D8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{85DA6C7C-BC56-4316-BB56-3D2CA86DF4B0}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{47F39228-8CCC-4319-9964-568280350AF4}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{781188CD-5AC0-41B9-8575-2EACD4BA90A4}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{A2DFBEC8-960F-4613-A8B8-821CF42818AC}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{5980B244-73E4-43AF-B863-305E8B039C33}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{549208EE-7E07-4F0F-ACFD-9606CC8F6B50}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{086F7B88-A201-47FD-B9A0-0C976108E144}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="80"/>
+    <tableColumn id="4" xr3:uid="{CC912184-CE02-4DC9-8815-71C4295C86DF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="79"/>
+    <tableColumn id="5" xr3:uid="{8F3F2202-7C07-4D43-B483-871C9E242208}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{6D2190D6-B434-4BB9-95B1-A29148C453AF}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="77"/>
+    <tableColumn id="7" xr3:uid="{A33DE0AF-7DA7-4623-87E7-DBA2BF4E404A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="76"/>
+    <tableColumn id="8" xr3:uid="{CD689B59-BA44-4F67-9FF9-E08337BE66FD}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="75"/>
+    <tableColumn id="9" xr3:uid="{744F224A-BA1E-4758-B291-8D5C8D341610}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}" name="Table011__Page_7" displayName="Table011__Page_7" ref="A1:C15" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C15" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{384F6B08-E7B1-4ECD-BC7E-1F8C8FC9CD11}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{BD116665-54B3-487B-82AD-7E260403FB1A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{A0C72322-3C63-446F-A7B0-E45538411191}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}" name="Table010__Page_6" displayName="Table010__Page_6" ref="A18:I20" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A18:I20" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{D02866AC-7C8C-4041-B0D6-297717EA2BCA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{F9BA0334-AC0F-4599-91DD-1D3B53530BA2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{2E40CB08-FF90-4211-A5F6-3255AA5CEAED}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{951E49DE-3DB8-41C0-8F36-6E5A1649659D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{D7FC7D23-AA29-4FAE-8DF4-B23A11020D8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{85DA6C7C-BC56-4316-BB56-3D2CA86DF4B0}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{47F39228-8CCC-4319-9964-568280350AF4}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{781188CD-5AC0-41B9-8575-2EACD4BA90A4}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{A2DFBEC8-960F-4613-A8B8-821CF42818AC}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}" name="Table012__Page_7" displayName="Table012__Page_7" ref="A17:C19" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A17:C19" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}" name="Table011__Page_7" displayName="Table011__Page_7" ref="A1:C15" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C15" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{92B56AD9-FE6F-4702-B777-811CB1B6E64F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{C37743D7-7886-43A1-BB26-C0F3914426C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{DFF6BFBF-623A-4318-86AF-C5448FC821A5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{384F6B08-E7B1-4ECD-BC7E-1F8C8FC9CD11}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{BD116665-54B3-487B-82AD-7E260403FB1A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{A0C72322-3C63-446F-A7B0-E45538411191}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}" name="Table013__Page_8" displayName="Table013__Page_8" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E16" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{811DEB23-A3B8-4E1E-AF98-CBD4FE9515C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{D1233A63-9D37-45F3-9DC7-52977AC06ADC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{400191B1-4CF8-4D78-82E7-FED7CD6730E6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{3D829CC4-4292-4CD0-80B8-3490D4014AC9}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{9BC50CF1-EF44-42B4-9129-E887F74428C9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}" name="Table012__Page_7" displayName="Table012__Page_7" ref="A17:C19" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A17:C19" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{92B56AD9-FE6F-4702-B777-811CB1B6E64F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{C37743D7-7886-43A1-BB26-C0F3914426C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{DFF6BFBF-623A-4318-86AF-C5448FC821A5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}" name="Table014__Page_8" displayName="Table014__Page_8" ref="A18:E21" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A18:E21" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}" name="Table013__Page_8" displayName="Table013__Page_8" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E16" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{98A6121C-2EC1-48CA-8A40-28DAFD66423E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{6B521FB3-E639-4556-B8C5-473A63201BC1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{3D07F9E9-4DA3-41C6-98A7-BC28F0C8BFB5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{89F1E0D5-9B1D-4170-BB1D-3FBA7855FC27}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{68E29A0D-4E20-4E2A-A030-157EF3C69E97}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{811DEB23-A3B8-4E1E-AF98-CBD4FE9515C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{D1233A63-9D37-45F3-9DC7-52977AC06ADC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{400191B1-4CF8-4D78-82E7-FED7CD6730E6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{3D829CC4-4292-4CD0-80B8-3490D4014AC9}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{9BC50CF1-EF44-42B4-9129-E887F74428C9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}" name="Table015__Page_9" displayName="Table015__Page_9" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F16" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B9D47F1B-922B-4B02-855C-93AF62167342}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{9915D8BD-1C99-4D36-BE7E-9EBEAD6D7B12}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{D353D58B-6A1D-4079-A9EC-77376B67A375}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{ACF53426-7425-4D38-9673-B3197A3F9292}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{673A9374-D6DA-46D7-AAD2-6F2220F4ED8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{37C428F9-0692-44D1-B8CF-2CBC7901020B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}" name="Table014__Page_8" displayName="Table014__Page_8" ref="A18:E21" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A18:E21" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{98A6121C-2EC1-48CA-8A40-28DAFD66423E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{6B521FB3-E639-4556-B8C5-473A63201BC1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{3D07F9E9-4DA3-41C6-98A7-BC28F0C8BFB5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{89F1E0D5-9B1D-4170-BB1D-3FBA7855FC27}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{68E29A0D-4E20-4E2A-A030-157EF3C69E97}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}" name="Table016__Page_9" displayName="Table016__Page_9" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A18:F20" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}" name="Table015__Page_9" displayName="Table015__Page_9" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F16" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{48EBD4D1-26EB-449F-8D09-DF1A8D9D96A3}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{671AE648-452F-44F1-9A65-8468F7B19950}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{C3287937-E8A8-4D80-A27C-D2A5C0E44D68}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{49CAB777-0355-40CC-9F2D-C41408ED9E98}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{A19C49CB-F2CF-4D60-B082-761FE4F0ABC5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{801427E9-2562-451E-AE45-ACF6DAAAFFFB}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{B9D47F1B-922B-4B02-855C-93AF62167342}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{9915D8BD-1C99-4D36-BE7E-9EBEAD6D7B12}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{D353D58B-6A1D-4079-A9EC-77376B67A375}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{ACF53426-7425-4D38-9673-B3197A3F9292}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{673A9374-D6DA-46D7-AAD2-6F2220F4ED8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{37C428F9-0692-44D1-B8CF-2CBC7901020B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}" name="Table017__Page_10" displayName="Table017__Page_10" ref="A1:E15" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E15" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{626476ED-551C-48ED-A0F5-9CB680097EF0}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{9215A7DD-9718-48E5-BA20-B6B9989DD0D2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{AE2AC56F-3587-4342-A60B-0B4A30905DD3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{F7BE237D-2C3F-4C27-92EF-2601ABCBA887}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{7950C4F9-8FA4-4C6E-B03A-A0235ECC51FF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}" name="Table016__Page_9" displayName="Table016__Page_9" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A18:F20" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{48EBD4D1-26EB-449F-8D09-DF1A8D9D96A3}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{671AE648-452F-44F1-9A65-8468F7B19950}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{C3287937-E8A8-4D80-A27C-D2A5C0E44D68}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{49CAB777-0355-40CC-9F2D-C41408ED9E98}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{A19C49CB-F2CF-4D60-B082-761FE4F0ABC5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{801427E9-2562-451E-AE45-ACF6DAAAFFFB}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}" name="Table018__Page_10" displayName="Table018__Page_10" ref="A17:E19" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A17:E19" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}" name="Table017__Page_10" displayName="Table017__Page_10" ref="A1:E15" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E15" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{210B1486-2DC9-4D94-98AC-6BEB874B7545}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{BB67F395-3AAE-4514-BCCE-DE32693EB37D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{230B22CA-5CA3-4E2D-92CC-C75BC5831FF2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{42788CA6-A70D-442A-9072-79E0D19F0B28}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{E37C1038-7442-4E7D-BB43-162AD6FA4195}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{626476ED-551C-48ED-A0F5-9CB680097EF0}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{9215A7DD-9718-48E5-BA20-B6B9989DD0D2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{AE2AC56F-3587-4342-A60B-0B4A30905DD3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{F7BE237D-2C3F-4C27-92EF-2601ABCBA887}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{7950C4F9-8FA4-4C6E-B03A-A0235ECC51FF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}" name="Table019__Page_11" displayName="Table019__Page_11" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E16" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}" name="Table018__Page_10" displayName="Table018__Page_10" ref="A17:E19" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A17:E19" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{60EAA1C9-E43C-458C-A33C-365CF023541D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{BF4ECEAF-8998-4833-A444-7DD2840947AB}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{A77E13C5-CB25-43C0-9678-51A378FA64FC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{46713ABC-AA6E-45DD-9BBE-03C863D6B1D1}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{85365AB6-280F-40C4-AB42-3455547D61F1}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{210B1486-2DC9-4D94-98AC-6BEB874B7545}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{BB67F395-3AAE-4514-BCCE-DE32693EB37D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{230B22CA-5CA3-4E2D-92CC-C75BC5831FF2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{42788CA6-A70D-442A-9072-79E0D19F0B28}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{E37C1038-7442-4E7D-BB43-162AD6FA4195}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}" name="Table002__Page_2" displayName="Table002__Page_2" ref="A19:G21" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A19:G21" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}" name="Table001__Page_2" displayName="Table001__Page_2" ref="A1:G16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G16" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8A3681DA-5FE9-4564-BCAB-75CCDF2C3A51}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="128"/>
-    <tableColumn id="2" xr3:uid="{44D6563C-A88C-4FEE-9427-B5252DF8FA5D}" uniqueName="2" name="Column6" queryTableFieldId="2" dataDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{2514D758-49E4-4E3E-A628-2B2D894F398E}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{062470EA-CB73-435C-8DF3-28DE262C8D69}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="125"/>
-    <tableColumn id="5" xr3:uid="{CDE500EE-B268-43D9-A30D-9E6CC1608CD0}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="124"/>
-    <tableColumn id="6" xr3:uid="{699F51E2-9A1B-4953-91BE-8D6434D76B20}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="123"/>
-    <tableColumn id="7" xr3:uid="{C62D0670-E212-49FF-BA61-22C41F21B60E}" uniqueName="7" name="Column62" queryTableFieldId="7" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{A26CE965-72B2-472B-B9FF-D68F7847F3C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{375BF78E-5806-424A-B7BD-C63C40843BE9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{CD1FFC74-B097-42B5-B1FA-08D3BD4531B9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{EA6F5C08-47B3-4BE3-8F9B-3167F2B34338}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{67D1B145-6151-4A54-9C79-A6B0381CDA09}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{E8D8899E-ED32-4A2F-B13D-18F4C289A59B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{CD1BCBB0-10DE-4DDA-903D-C14D16829749}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="142"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}" name="Table019__Page_11" displayName="Table019__Page_11" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E16" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{60EAA1C9-E43C-458C-A33C-365CF023541D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{BF4ECEAF-8998-4833-A444-7DD2840947AB}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{A77E13C5-CB25-43C0-9678-51A378FA64FC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{46713ABC-AA6E-45DD-9BBE-03C863D6B1D1}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{85365AB6-280F-40C4-AB42-3455547D61F1}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0B4290D5-7CEE-4DDC-B997-690EEF6D9589}" name="Table020__Page_11" displayName="Table020__Page_11" ref="A18:E20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:E20" xr:uid="{0B4290D5-7CEE-4DDC-B997-690EEF6D9589}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{344C3D84-8C5A-4C60-ADD3-4EE73F83858B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{3470DF86-5A38-429A-95CF-F5FF5E59449C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{BC1BD851-46F6-4634-95EE-ED117E75EBB6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{FF5D3D34-BBDB-4113-8340-C737255ED1BD}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{F05FA152-C9D6-4773-B0A5-5B18B60C7102}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{344C3D84-8C5A-4C60-ADD3-4EE73F83858B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{3470DF86-5A38-429A-95CF-F5FF5E59449C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{BC1BD851-46F6-4634-95EE-ED117E75EBB6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{FF5D3D34-BBDB-4113-8340-C737255ED1BD}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{F05FA152-C9D6-4773-B0A5-5B18B60C7102}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}" name="Table003__Page_3" displayName="Table003__Page_3" ref="A1:H16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H16" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5E78ED26-3040-4033-A95F-3AC09118D17C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{52F60F93-88D4-4F60-A15A-4B2113E53BE2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{2A66B2A9-165C-4995-937F-8E0D8B01B3D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{937ED0C3-8277-4EC6-BFD2-C6699696538D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="118"/>
-    <tableColumn id="5" xr3:uid="{37EAAABA-4FEF-4D28-B237-360AD0A7194A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="117"/>
-    <tableColumn id="6" xr3:uid="{6E7D50A0-6329-4797-9F9A-628D251C7CA5}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="116"/>
-    <tableColumn id="7" xr3:uid="{F8F31C01-9522-488B-915F-110987168D09}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="115"/>
-    <tableColumn id="8" xr3:uid="{FFD35FDD-AAE7-4F54-8AF3-197380BC0AEB}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}" name="Table002__Page_2" displayName="Table002__Page_2" ref="A19:G21" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A19:G21" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8A3681DA-5FE9-4564-BCAB-75CCDF2C3A51}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{44D6563C-A88C-4FEE-9427-B5252DF8FA5D}" uniqueName="2" name="Column6" queryTableFieldId="2" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{2514D758-49E4-4E3E-A628-2B2D894F398E}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{062470EA-CB73-435C-8DF3-28DE262C8D69}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="138"/>
+    <tableColumn id="5" xr3:uid="{CDE500EE-B268-43D9-A30D-9E6CC1608CD0}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="137"/>
+    <tableColumn id="6" xr3:uid="{699F51E2-9A1B-4953-91BE-8D6434D76B20}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{C62D0670-E212-49FF-BA61-22C41F21B60E}" uniqueName="7" name="Column62" queryTableFieldId="7" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}" name="Table004__Page_3" displayName="Table004__Page_3" ref="A18:H20" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A18:H20" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}" name="Table003__Page_3" displayName="Table003__Page_3" ref="A1:H16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H16" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A8A6FCCE-AE43-4EDA-82DC-831809E03401}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{0231594E-DA9E-47DE-A01C-22488210A4CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="112"/>
-    <tableColumn id="3" xr3:uid="{7A06306A-69AF-482D-910F-86D0EF88F740}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="111"/>
-    <tableColumn id="4" xr3:uid="{E96F3603-E9D2-4710-BDE5-6FE3E6A378D8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="110"/>
-    <tableColumn id="5" xr3:uid="{37151140-CC9F-4EBB-B58D-F87E1081314A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="109"/>
-    <tableColumn id="6" xr3:uid="{F0AAEEC2-014D-412A-B58D-24C71FEC9A66}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="108"/>
-    <tableColumn id="7" xr3:uid="{A4B4F3F0-B14D-498F-B185-AA3E2BAE729A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="107"/>
-    <tableColumn id="8" xr3:uid="{0C517BB9-44A4-4BBA-AA88-B86BB679F208}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="106"/>
+    <tableColumn id="1" xr3:uid="{5E78ED26-3040-4033-A95F-3AC09118D17C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="134"/>
+    <tableColumn id="2" xr3:uid="{52F60F93-88D4-4F60-A15A-4B2113E53BE2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="133"/>
+    <tableColumn id="3" xr3:uid="{2A66B2A9-165C-4995-937F-8E0D8B01B3D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="132"/>
+    <tableColumn id="4" xr3:uid="{937ED0C3-8277-4EC6-BFD2-C6699696538D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="131"/>
+    <tableColumn id="5" xr3:uid="{37EAAABA-4FEF-4D28-B237-360AD0A7194A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="130"/>
+    <tableColumn id="6" xr3:uid="{6E7D50A0-6329-4797-9F9A-628D251C7CA5}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="129"/>
+    <tableColumn id="7" xr3:uid="{F8F31C01-9522-488B-915F-110987168D09}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="128"/>
+    <tableColumn id="8" xr3:uid="{FFD35FDD-AAE7-4F54-8AF3-197380BC0AEB}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="127"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}" name="Table005__Page_4" displayName="Table005__Page_4" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F16" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AB42FEA9-5A85-4A69-B46D-444C53C4B4EF}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{0D7919B1-FB5E-4192-8675-3D57B39D9AB0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{94F12F3D-88BF-4BEB-85E7-FF6313F6B88E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{2B04EEA3-DC55-4C69-860F-9571D35E352D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{461C5084-182B-40CC-B479-24798E48D0F4}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{258F7EB6-7345-43CA-BF8A-5E088D06FF8F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}" name="Table004__Page_3" displayName="Table004__Page_3" ref="A18:H20" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A18:H20" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{A8A6FCCE-AE43-4EDA-82DC-831809E03401}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{0231594E-DA9E-47DE-A01C-22488210A4CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{7A06306A-69AF-482D-910F-86D0EF88F740}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{E96F3603-E9D2-4710-BDE5-6FE3E6A378D8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{37151140-CC9F-4EBB-B58D-F87E1081314A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="122"/>
+    <tableColumn id="6" xr3:uid="{F0AAEEC2-014D-412A-B58D-24C71FEC9A66}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="121"/>
+    <tableColumn id="7" xr3:uid="{A4B4F3F0-B14D-498F-B185-AA3E2BAE729A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="120"/>
+    <tableColumn id="8" xr3:uid="{0C517BB9-44A4-4BBA-AA88-B86BB679F208}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}" name="Table006__Page_4" displayName="Table006__Page_4" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A18:F20" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}" name="Table005__Page_4" displayName="Table005__Page_4" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F16" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{55987721-40E8-4E11-9B6F-67EE503D78F4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{15260D47-39CC-4501-9656-F8DBE6AD3AB1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{06C8B30C-3DD3-49E6-8BE6-C8A9D39F2FC4}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{40A070F6-4BDB-49A7-9394-4D63F3A9E318}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{C5E0BAEF-796C-4C71-ACA7-889E63543C2D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{1BA75280-A961-41F1-B113-5935891BA00A}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{AB42FEA9-5A85-4A69-B46D-444C53C4B4EF}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="118"/>
+    <tableColumn id="2" xr3:uid="{0D7919B1-FB5E-4192-8675-3D57B39D9AB0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="117"/>
+    <tableColumn id="3" xr3:uid="{94F12F3D-88BF-4BEB-85E7-FF6313F6B88E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="116"/>
+    <tableColumn id="4" xr3:uid="{2B04EEA3-DC55-4C69-860F-9571D35E352D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="115"/>
+    <tableColumn id="5" xr3:uid="{461C5084-182B-40CC-B479-24798E48D0F4}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="114"/>
+    <tableColumn id="6" xr3:uid="{258F7EB6-7345-43CA-BF8A-5E088D06FF8F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}" name="Table007__Page_5" displayName="Table007__Page_5" ref="A1:L16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:L16" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9561388E-64AE-4A76-863E-A0B2091E2F9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{151810A9-7DD3-4FD0-91D6-6608DF85A8CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{94D629BF-F745-493D-8F74-FA7EEFDEAA84}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{AE87299A-170F-4661-BD08-B108394E2F7C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{708CB468-5E3F-4D0C-B6BD-C2C44C7191EC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{5D4BD3CB-C344-4155-B3C1-ECC49F86CED1}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{61DF1122-5C54-47A3-98F9-27CA1B50CA9D}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="87"/>
-    <tableColumn id="8" xr3:uid="{130590EE-DDCB-43DB-A020-385B521DA018}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="86"/>
-    <tableColumn id="9" xr3:uid="{06B903F7-5E22-476D-A116-655599D2C518}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="85"/>
-    <tableColumn id="10" xr3:uid="{CED96D55-8B0D-492D-B0EC-F3E56EFB2649}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="84"/>
-    <tableColumn id="11" xr3:uid="{346823E9-F305-4F11-941F-1C42A8AB0C99}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="83"/>
-    <tableColumn id="12" xr3:uid="{7B421AA8-C9DB-4E35-A456-DF0F56050B79}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="82"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}" name="Table006__Page_4" displayName="Table006__Page_4" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A18:F20" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{55987721-40E8-4E11-9B6F-67EE503D78F4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{15260D47-39CC-4501-9656-F8DBE6AD3AB1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{06C8B30C-3DD3-49E6-8BE6-C8A9D39F2FC4}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{40A070F6-4BDB-49A7-9394-4D63F3A9E318}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{C5E0BAEF-796C-4C71-ACA7-889E63543C2D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="108"/>
+    <tableColumn id="6" xr3:uid="{1BA75280-A961-41F1-B113-5935891BA00A}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}" name="Table008__Page_5" displayName="Table008__Page_5" ref="A18:L20" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A18:L20" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}" name="Table007__Page_5" displayName="Table007__Page_5" ref="A1:L16" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:L16" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{01D3C90B-BA67-46B4-BD1D-5C53486CAE57}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{166854EB-0B50-4420-BB3F-7A5A2C9FB7F7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{638857E5-1EB4-4FBE-9FFE-2951F2F4ABD0}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{F4EFE2EF-AC84-40F8-BE68-0B6B520F8EA8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{38D026D2-A47E-46EA-BA10-AF890A55BF2B}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{025C6DA2-37A6-491F-904E-DDE12948D35B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{AC28B573-67B7-4468-A6A2-F648D17079B6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{F6F06554-210B-472F-95F2-8E89D931E4C1}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="74"/>
-    <tableColumn id="9" xr3:uid="{F0A8F323-36C1-4290-980B-8F6F5DC6A41E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="73"/>
-    <tableColumn id="10" xr3:uid="{25D60007-5007-4174-85F5-572E3C29FE33}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="72"/>
-    <tableColumn id="11" xr3:uid="{2071EB9B-B14E-4EF0-9B86-0D5FDA96828D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="71"/>
-    <tableColumn id="12" xr3:uid="{1660C180-EE6B-48E8-9880-55F02CC623C4}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{9561388E-64AE-4A76-863E-A0B2091E2F9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{151810A9-7DD3-4FD0-91D6-6608DF85A8CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{94D629BF-F745-493D-8F74-FA7EEFDEAA84}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{AE87299A-170F-4661-BD08-B108394E2F7C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{708CB468-5E3F-4D0C-B6BD-C2C44C7191EC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{5D4BD3CB-C344-4155-B3C1-ECC49F86CED1}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{61DF1122-5C54-47A3-98F9-27CA1B50CA9D}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{130590EE-DDCB-43DB-A020-385B521DA018}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="99"/>
+    <tableColumn id="9" xr3:uid="{06B903F7-5E22-476D-A116-655599D2C518}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="98"/>
+    <tableColumn id="10" xr3:uid="{CED96D55-8B0D-492D-B0EC-F3E56EFB2649}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="97"/>
+    <tableColumn id="11" xr3:uid="{346823E9-F305-4F11-941F-1C42A8AB0C99}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="96"/>
+    <tableColumn id="12" xr3:uid="{7B421AA8-C9DB-4E35-A456-DF0F56050B79}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}" name="Table009__Page_6" displayName="Table009__Page_6" ref="A1:I16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:I16" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5980B244-73E4-43AF-B863-305E8B039C33}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{549208EE-7E07-4F0F-ACFD-9606CC8F6B50}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{086F7B88-A201-47FD-B9A0-0C976108E144}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{CC912184-CE02-4DC9-8815-71C4295C86DF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{8F3F2202-7C07-4D43-B483-871C9E242208}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{6D2190D6-B434-4BB9-95B1-A29148C453AF}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{A33DE0AF-7DA7-4623-87E7-DBA2BF4E404A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="63"/>
-    <tableColumn id="8" xr3:uid="{CD689B59-BA44-4F67-9FF9-E08337BE66FD}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{744F224A-BA1E-4758-B291-8D5C8D341610}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}" name="Table008__Page_5" displayName="Table008__Page_5" ref="A18:L20" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A18:L20" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{01D3C90B-BA67-46B4-BD1D-5C53486CAE57}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{166854EB-0B50-4420-BB3F-7A5A2C9FB7F7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{638857E5-1EB4-4FBE-9FFE-2951F2F4ABD0}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{F4EFE2EF-AC84-40F8-BE68-0B6B520F8EA8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{38D026D2-A47E-46EA-BA10-AF890A55BF2B}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{025C6DA2-37A6-491F-904E-DDE12948D35B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{AC28B573-67B7-4468-A6A2-F648D17079B6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="88"/>
+    <tableColumn id="8" xr3:uid="{F6F06554-210B-472F-95F2-8E89D931E4C1}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="87"/>
+    <tableColumn id="9" xr3:uid="{F0A8F323-36C1-4290-980B-8F6F5DC6A41E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="86"/>
+    <tableColumn id="10" xr3:uid="{25D60007-5007-4174-85F5-572E3C29FE33}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="85"/>
+    <tableColumn id="11" xr3:uid="{2071EB9B-B14E-4EF0-9B86-0D5FDA96828D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="84"/>
+    <tableColumn id="12" xr3:uid="{1660C180-EE6B-48E8-9880-55F02CC623C4}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5062,1306 +5547,1435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05C9E0-A64E-40AC-B9F4-C919ED5906CC}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="51.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.08984375" customWidth="1"/>
-    <col min="10" max="10" width="32.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="37.08984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="33.6328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.08984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.36328125" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.08984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="18" t="s">
         <v>546</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="18" t="s">
         <v>553</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="18" t="s">
         <v>562</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="18" t="s">
         <v>563</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="18" t="s">
         <v>552</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="18" t="s">
         <v>564</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="19" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>514</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>447200000</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <f>I2/1.12</f>
         <v>31249999.999999996</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <f>D2*90%</f>
         <v>28124999.999999996</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <f>D2*70%</f>
         <v>21874999.999999996</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="7">
         <v>228</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="15">
         <v>35000000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>547</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>388500000</v>
       </c>
-      <c r="D3" s="7">
-        <f t="shared" ref="D3:D39" si="0">I3/1.12</f>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D42" si="0">I3/1.12</f>
         <v>29464285.714285709</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <f t="shared" ref="E3:E29" si="1">D3*90%</f>
         <v>26517857.142857138</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <f t="shared" ref="F3:F29" si="2">D3*70%</f>
         <v>20624999.999999996</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>227</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="15">
         <v>32999999.999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>515</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>311500000</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <f t="shared" si="0"/>
         <v>20758928.571428567</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <f t="shared" si="1"/>
         <v>18683035.714285713</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <f t="shared" si="2"/>
         <v>14531249.999999996</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>222</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="15">
         <v>23249999.999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>516</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>329050000</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>22053571.428571429</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <f t="shared" si="1"/>
         <v>19848214.285714287</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <f t="shared" si="2"/>
         <v>15437500</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>223</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="15">
         <v>24700000.000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>496</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>405000000</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>31249999.999999996</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <f t="shared" si="1"/>
         <v>28124999.999999996</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <f t="shared" si="2"/>
         <v>21874999.999999996</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>244</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="15">
         <v>35000000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>497</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>442000000</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <f t="shared" si="0"/>
         <v>33928571.428571425</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <f t="shared" si="1"/>
         <v>30535714.285714284</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <f t="shared" si="2"/>
         <v>23749999.999999996</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>245</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="15">
         <v>38000000</v>
       </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>303000000</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <f t="shared" si="0"/>
         <v>20535714.285714284</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <f t="shared" si="1"/>
         <v>18482142.857142854</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <f t="shared" si="2"/>
         <v>14374999.999999998</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>240</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="15">
         <v>23000000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
         <v>518</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>263000000</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <f t="shared" si="0"/>
         <v>17857142.857142854</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <f t="shared" si="1"/>
         <v>16071428.571428569</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <f t="shared" si="2"/>
         <v>12499999.999999998</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>241</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="15">
         <v>20000000</v>
       </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>519</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>217000000</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <f t="shared" si="0"/>
         <v>11607142.857142856</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <f t="shared" si="1"/>
         <v>10446428.571428571</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <f t="shared" si="2"/>
         <v>8124999.9999999991</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>242</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="15">
         <v>13000000</v>
       </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>188300000</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <f t="shared" si="0"/>
         <v>11339285.714285715</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <f t="shared" si="1"/>
         <v>10205357.142857144</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <f t="shared" si="2"/>
         <v>7937500</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>202</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="15">
         <v>12700000.000000002</v>
       </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>524</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>222850000</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <f t="shared" si="0"/>
         <v>14285714.285714284</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <f t="shared" si="1"/>
         <v>12857142.857142856</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <f t="shared" si="2"/>
         <v>9999999.9999999981</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>204</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="15">
         <v>16000000</v>
       </c>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
         <v>498</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>210700000</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <f t="shared" si="0"/>
         <v>13124999.999999998</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <f t="shared" si="1"/>
         <v>11812499.999999998</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <f t="shared" si="2"/>
         <v>9187499.9999999981</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>205</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="15">
         <v>14700000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>277200000</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <f t="shared" si="0"/>
         <v>18660714.285714284</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <f t="shared" si="1"/>
         <v>16794642.857142854</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <f t="shared" si="2"/>
         <v>13062499.999999998</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>213</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="15">
         <v>20900000</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
         <v>528</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <v>291300000</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <f t="shared" si="0"/>
         <v>19642857.142857142</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <f t="shared" si="1"/>
         <v>17678571.428571429</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <f t="shared" si="2"/>
         <v>13749999.999999998</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>214</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="15">
         <v>22000000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>525</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="5">
         <v>262500000</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <f t="shared" si="0"/>
         <v>16339285.714285713</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <f t="shared" si="1"/>
         <v>14705357.142857142</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="5">
         <f t="shared" si="2"/>
         <v>11437499.999999998</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>209</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="15">
         <v>18300000</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="12" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>285200000</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <f t="shared" si="0"/>
         <v>18303571.428571429</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <f t="shared" si="1"/>
         <v>16473214.285714287</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <f t="shared" si="2"/>
         <v>12812500</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>220</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="15">
         <v>20500000.000000004</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="12" t="s">
         <v>580</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <v>214000000</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <f t="shared" si="0"/>
         <v>18750000</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <f t="shared" si="1"/>
         <v>16875000</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="5">
         <f t="shared" si="2"/>
         <v>13125000</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>221</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="15">
         <v>21000000.000000004</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="12" t="s">
         <v>555</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <v>251000000</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <f t="shared" si="0"/>
         <v>18750000</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <f t="shared" ref="E19" si="3">D19*90%</f>
         <v>16875000</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <f t="shared" ref="F19" si="4">D19*70%</f>
         <v>13125000</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>221</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="15">
         <v>21000000.000000004</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="12" t="s">
         <v>500</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <v>251000000</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="5">
         <f t="shared" si="0"/>
         <v>18750000</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <f t="shared" si="1"/>
         <v>16875000</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="5">
         <f t="shared" si="2"/>
         <v>13125000</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>243</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="15">
         <v>21000000.000000004</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="12" t="s">
         <v>501</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <v>251000000</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <f t="shared" si="0"/>
         <v>18750000</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <f t="shared" si="1"/>
         <v>16875000</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="5">
         <f t="shared" si="2"/>
         <v>13125000</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>250</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="15">
         <v>21000000.000000004</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="12" t="s">
         <v>502</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="5">
         <v>307500000</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="5">
         <f t="shared" si="0"/>
         <v>22321428.571428567</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <f t="shared" si="1"/>
         <v>20089285.714285713</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="5">
         <f t="shared" si="2"/>
         <v>15624999.999999996</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>235</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="15">
         <v>24999999.999999996</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="12" t="s">
         <v>503</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>353000000</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
         <f t="shared" si="0"/>
         <v>25892857.142857142</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <f t="shared" si="1"/>
         <v>23303571.428571429</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="5">
         <f t="shared" si="2"/>
         <v>18124999.999999996</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>246</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="4" t="s">
         <v>576</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="15">
         <v>29000000</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="12" t="s">
         <v>504</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="5">
         <v>363000000</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <f t="shared" si="0"/>
         <v>26785714.285714284</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <f t="shared" si="1"/>
         <v>24107142.857142854</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="5">
         <f t="shared" si="2"/>
         <v>18749999.999999996</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>247</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="15">
         <v>30000000</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="12" t="s">
         <v>588</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <v>363000000</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <f t="shared" ref="D25" si="5">I25/1.12</f>
         <v>25892857.142857142</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <f t="shared" si="1"/>
         <v>23303571.428571429</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="5">
         <f t="shared" si="2"/>
         <v>18124999.999999996</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>253</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I25" s="15">
         <v>29000000</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="12" t="s">
         <v>505</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="5">
         <v>413000000</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <f t="shared" si="0"/>
         <v>30357142.857142854</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="5">
         <f t="shared" si="1"/>
         <v>27321428.571428571</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="5">
         <f t="shared" si="2"/>
         <v>21249999.999999996</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>248</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="15">
         <v>34000000</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="12" t="s">
         <v>586</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="5">
         <v>318000000</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <f t="shared" si="0"/>
         <v>23214285.714285713</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="5">
         <f t="shared" ref="E27:E28" si="6">D27*90%</f>
         <v>20892857.142857142</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="5">
         <f t="shared" ref="F27:F28" si="7">D27*70%</f>
         <v>16249999.999999998</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>252</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="4" t="s">
         <v>576</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I27" s="15">
         <v>26000000</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="12" t="s">
         <v>587</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="5">
         <v>363000000</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="5">
         <f t="shared" si="0"/>
         <v>25892857.142857142</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="5">
         <f t="shared" si="6"/>
         <v>23303571.428571429</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="5">
         <f t="shared" si="7"/>
         <v>18124999.999999996</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>253</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="15">
         <v>29000000</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="12" t="s">
         <v>557</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>415000000</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="5">
         <f t="shared" si="0"/>
         <v>33035714.285714284</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="5">
         <f t="shared" si="1"/>
         <v>29732142.857142854</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="5">
         <f t="shared" si="2"/>
         <v>23124999.999999996</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>251</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="15">
         <v>37000000</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="12" t="s">
         <v>582</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <v>415000000</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="5">
         <f t="shared" si="0"/>
         <v>33035714.285714284</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="5">
         <f t="shared" ref="E30" si="8">D30*90%</f>
         <v>29732142.857142854</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="5">
         <f t="shared" ref="F30" si="9">D30*70%</f>
         <v>23124999.999999996</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>251</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="15">
         <v>37000000</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="5">
         <v>443000000</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="5">
         <f t="shared" si="0"/>
         <v>33035714.285714284</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="5">
         <f t="shared" ref="E31" si="10">D31*90%</f>
         <v>29732142.857142854</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="5">
         <f t="shared" ref="F31" si="11">D31*70%</f>
         <v>23124999.999999996</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>249</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="15">
         <v>37000000</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="12" t="s">
         <v>506</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="5">
         <v>443000000</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="5">
         <f t="shared" si="0"/>
         <v>33035714.285714284</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="5">
         <f>D32*90%</f>
         <v>29732142.857142854</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="5">
         <f>D32*70%</f>
         <v>23124999.999999996</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>249</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="15">
         <v>37000000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="12" t="s">
         <v>529</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="5">
         <v>155700000</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="5">
         <f t="shared" si="0"/>
         <v>10892857.142857142</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="5">
         <f>D33*90%</f>
         <v>9803571.4285714272</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="5">
         <f>D33*70%</f>
         <v>7624999.9999999991</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>201</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="I33" s="12">
+      <c r="I33" s="15">
         <v>12200000</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="12" t="s">
         <v>520</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="5">
         <v>172600000</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="5">
         <f t="shared" si="0"/>
         <v>7142857.1428571418</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="5">
         <f>D34*90%</f>
         <v>6428571.4285714282</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="5">
         <f>D34*70%</f>
         <v>4999999.9999999991</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <v>230</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="I34" s="12">
+      <c r="I34" s="15">
         <v>8000000</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="12" t="s">
         <v>521</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="5">
         <v>176000000</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="5">
         <f t="shared" si="0"/>
         <v>12053571.428571427</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="5">
         <f>D35*90%</f>
         <v>10848214.285714285</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="5">
         <f>D35*70%</f>
         <v>8437499.9999999981</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <v>238</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="I35" s="12">
+      <c r="I35" s="15">
         <v>13500000</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="12" t="s">
         <v>526</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="5">
         <v>168000000</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="5">
         <f t="shared" si="0"/>
         <v>11160714.285714284</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="5">
         <f>D36*90%</f>
         <v>10044642.857142856</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="5">
         <f>D36*70%</f>
         <v>7812499.9999999981</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>237</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="15">
         <v>12499999.999999998</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="12" t="s">
         <v>560</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="5">
         <v>188300000</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="5">
         <f t="shared" si="0"/>
         <v>11339285.714285715</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="5">
         <f t="shared" ref="E37:E38" si="12">D37*90%</f>
         <v>10205357.142857144</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="5">
         <f t="shared" ref="F37:F38" si="13">D37*70%</f>
         <v>7937500</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <v>202</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="15">
         <v>12700000.000000002</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="12" t="s">
         <v>561</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="5">
         <v>443000000</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="5">
         <f t="shared" si="0"/>
         <v>33035714.285714284</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="5">
         <f t="shared" si="12"/>
         <v>29732142.857142854</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="5">
         <f t="shared" si="13"/>
         <v>23124999.999999996</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <v>249</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H38" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="I38" s="12">
+      <c r="I38" s="15">
         <v>37000000</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="13" t="s">
         <v>522</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="5">
         <v>345650000</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="5">
         <f t="shared" si="0"/>
         <v>22857142.857142854</v>
       </c>
-      <c r="E39" s="7">
-        <f t="shared" ref="E39" si="14">D39*90%</f>
+      <c r="E39" s="5">
+        <f t="shared" ref="E39:E42" si="14">D39*90%</f>
         <v>20571428.571428571</v>
       </c>
-      <c r="F39" s="7">
-        <f t="shared" ref="F39" si="15">D39*70%</f>
+      <c r="F39" s="5">
+        <f t="shared" ref="F39:F42" si="15">D39*70%</f>
         <v>15999999.999999996</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <v>233</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H39" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I39" s="12">
+      <c r="I39" s="15">
         <v>25600000</v>
       </c>
     </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="C40" s="11">
+        <v>328000000</v>
+      </c>
+      <c r="D40" s="11">
+        <f t="shared" si="0"/>
+        <v>17857142.857142854</v>
+      </c>
+      <c r="E40" s="11">
+        <f t="shared" si="14"/>
+        <v>16071428.571428569</v>
+      </c>
+      <c r="F40" s="11">
+        <f t="shared" si="15"/>
+        <v>12499999.999999998</v>
+      </c>
+      <c r="G40" s="24">
+        <v>254</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="I40" s="15">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="C41" s="11">
+        <v>348000000</v>
+      </c>
+      <c r="D41" s="11">
+        <f t="shared" si="0"/>
+        <v>17857142.857142854</v>
+      </c>
+      <c r="E41" s="11">
+        <f t="shared" si="14"/>
+        <v>16071428.571428569</v>
+      </c>
+      <c r="F41" s="11">
+        <f t="shared" si="15"/>
+        <v>12499999.999999998</v>
+      </c>
+      <c r="G41" s="24">
+        <v>256</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="I41" s="16">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="14" t="s">
+        <v>591</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>595</v>
+      </c>
+      <c r="C42" s="11">
+        <v>358000000</v>
+      </c>
+      <c r="D42" s="11">
+        <f t="shared" si="0"/>
+        <v>22321428.571428571</v>
+      </c>
+      <c r="E42" s="11">
+        <f t="shared" si="14"/>
+        <v>20089285.714285713</v>
+      </c>
+      <c r="F42" s="11">
+        <f t="shared" si="15"/>
+        <v>15624999.999999998</v>
+      </c>
+      <c r="G42" s="24">
+        <v>255</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="I42" s="16">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="20" t="s">
+        <v>592</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>596</v>
+      </c>
+      <c r="C43" s="22">
+        <v>378000000</v>
+      </c>
+      <c r="D43" s="11">
+        <f t="shared" ref="D43" si="16">I43/1.12</f>
+        <v>22321428.571428571</v>
+      </c>
+      <c r="E43" s="11">
+        <f t="shared" ref="E43" si="17">D43*90%</f>
+        <v>20089285.714285713</v>
+      </c>
+      <c r="F43" s="11">
+        <f t="shared" ref="F43" si="18">D43*70%</f>
+        <v>15624999.999999998</v>
+      </c>
+      <c r="G43" s="25">
+        <v>257</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="I43" s="23">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D48" s="9"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A31:A38 A2:A29">
+  <conditionalFormatting sqref="A31:A38 A2:A29 A40:A43">
     <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31:A39 A2:A29">
+  <conditionalFormatting sqref="A2:A29 A31:A43">
     <cfRule type="duplicateValues" dxfId="2" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -7356,55 +7970,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <f>VLOOKUP(B2,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>447200000</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <f>VLOOKUP(B2,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>31249.999999999996</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <f>D2*90%</f>
         <v>28124.999999999996</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <f>D2*70%</f>
         <v>21874.999999999996</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="7">
         <v>228</v>
       </c>
       <c r="H2" t="s">
@@ -7412,29 +8026,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <f>VLOOKUP(B3,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>388500000</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <f>VLOOKUP(B3,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>29464.28571428571</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <f t="shared" ref="E3:E34" si="0">D3*90%</f>
         <v>26517.857142857141</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <f t="shared" ref="F3:F34" si="1">D3*70%</f>
         <v>20624.999999999996</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>227</v>
       </c>
       <c r="H3" t="s">
@@ -7442,29 +8056,29 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <f>VLOOKUP(B4,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>311500000</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <f>VLOOKUP(B4,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>20758.928571428569</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>18683.035714285714</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <f t="shared" si="1"/>
         <v>14531.249999999996</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>222</v>
       </c>
       <c r="H4" t="s">
@@ -7472,29 +8086,29 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <f>VLOOKUP(B5,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>329050000</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <f>VLOOKUP(B5,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>22053.571428571428</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
         <v>19848.214285714286</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <f t="shared" si="1"/>
         <v>15437.499999999998</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>223</v>
       </c>
       <c r="H5" t="s">
@@ -7502,29 +8116,29 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <f>VLOOKUP(B6,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>405000000</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <f>VLOOKUP(B6,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>31249.999999999996</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>28124.999999999996</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <f t="shared" si="1"/>
         <v>21874.999999999996</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>244</v>
       </c>
       <c r="H6" t="s">
@@ -7532,29 +8146,29 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <f>VLOOKUP(B7,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>442000000</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <f>VLOOKUP(B7,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33928.571428571428</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>30535.714285714286</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <f t="shared" si="1"/>
         <v>23749.999999999996</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>245</v>
       </c>
       <c r="H7" t="s">
@@ -7562,29 +8176,29 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <f>VLOOKUP(B8,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>303000000</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <f>VLOOKUP(B8,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>20535.714285714283</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>18482.142857142855</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <f t="shared" si="1"/>
         <v>14374.999999999996</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>240</v>
       </c>
       <c r="H8" t="s">
@@ -7592,29 +8206,29 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <f>VLOOKUP(B9,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>263000000</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <f>VLOOKUP(B9,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>17857.142857142855</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>16071.428571428571</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <f t="shared" si="1"/>
         <v>12499.999999999998</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>241</v>
       </c>
       <c r="H9" t="s">
@@ -7622,29 +8236,29 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <f>VLOOKUP(B10,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>217000000</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <f>VLOOKUP(B10,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>11607.142857142857</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
         <v>10446.428571428571</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <f t="shared" si="1"/>
         <v>8124.9999999999991</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>242</v>
       </c>
       <c r="H10" t="s">
@@ -7652,29 +8266,29 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <f>VLOOKUP(B11,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>188300000</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <f>VLOOKUP(B11,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>11339.285714285714</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
         <v>10205.357142857143</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <f t="shared" si="1"/>
         <v>7937.4999999999991</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>202</v>
       </c>
       <c r="H11" t="s">
@@ -7682,29 +8296,29 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <f>VLOOKUP(B12,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>222850000</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <f>VLOOKUP(B12,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>14285.714285714284</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <f t="shared" si="0"/>
         <v>12857.142857142857</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <f t="shared" si="1"/>
         <v>9999.9999999999982</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>204</v>
       </c>
       <c r="H12" t="s">
@@ -7712,29 +8326,29 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <f>VLOOKUP(B13,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>210700000</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <f>VLOOKUP(B13,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>13124.999999999998</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <f t="shared" si="0"/>
         <v>11812.499999999998</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <f t="shared" si="1"/>
         <v>9187.4999999999982</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>205</v>
       </c>
       <c r="H13" t="s">
@@ -7742,29 +8356,29 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <f>VLOOKUP(B14,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>277200000</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <f>VLOOKUP(B14,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18660.714285714283</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <f t="shared" si="0"/>
         <v>16794.642857142855</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <f t="shared" si="1"/>
         <v>13062.499999999996</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>213</v>
       </c>
       <c r="H14" t="s">
@@ -7772,29 +8386,29 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <f>VLOOKUP(B15,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>291300000</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <f>VLOOKUP(B15,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>19642.857142857141</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <f t="shared" si="0"/>
         <v>17678.571428571428</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <f t="shared" si="1"/>
         <v>13749.999999999998</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>214</v>
       </c>
       <c r="H15" t="s">
@@ -7802,29 +8416,29 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="5">
         <f>VLOOKUP(B16,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>262500000</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <f>VLOOKUP(B16,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>16339.285714285712</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <f t="shared" si="0"/>
         <v>14705.357142857141</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="5">
         <f t="shared" si="1"/>
         <v>11437.499999999998</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>209</v>
       </c>
       <c r="H16" t="s">
@@ -7832,29 +8446,29 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <f>VLOOKUP(B17,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>285200000</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <f>VLOOKUP(B17,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18303.571428571428</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <f t="shared" si="0"/>
         <v>16473.214285714286</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <f t="shared" si="1"/>
         <v>12812.499999999998</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>220</v>
       </c>
       <c r="H17" t="s">
@@ -7862,29 +8476,29 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <f>VLOOKUP(B18,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>214000000</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <f>VLOOKUP(B18,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18750</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <f t="shared" si="0"/>
         <v>16875</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="5">
         <f t="shared" si="1"/>
         <v>13125</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>221</v>
       </c>
       <c r="H18" t="s">
@@ -7892,29 +8506,29 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <f>VLOOKUP(B19,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>251000000</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <f>VLOOKUP(B19,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18750</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <f t="shared" si="0"/>
         <v>16875</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <f t="shared" si="1"/>
         <v>13125</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>243</v>
       </c>
       <c r="H19" t="s">
@@ -7922,29 +8536,29 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <f>VLOOKUP(B20,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>251000000</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="5">
         <f>VLOOKUP(B20,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>18750</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <f t="shared" si="0"/>
         <v>16875</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="5">
         <f t="shared" si="1"/>
         <v>13125</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>250</v>
       </c>
       <c r="H20" t="s">
@@ -7952,29 +8566,29 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <f>VLOOKUP(B21,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>307500000</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <f>VLOOKUP(B21,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>22321.428571428569</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <f t="shared" si="0"/>
         <v>20089.285714285714</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="5">
         <f t="shared" si="1"/>
         <v>15624.999999999996</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>235</v>
       </c>
       <c r="H21" t="s">
@@ -7982,29 +8596,29 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="5">
         <f>VLOOKUP(B22,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>353000000</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="5">
         <f>VLOOKUP(B22,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>25892.857142857141</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <f t="shared" si="0"/>
         <v>23303.571428571428</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="5">
         <f t="shared" si="1"/>
         <v>18124.999999999996</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>246</v>
       </c>
       <c r="H22" t="s">
@@ -8012,29 +8626,29 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <f>VLOOKUP(B23,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>363000000</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
         <f>VLOOKUP(B23,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>26785.714285714283</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <f t="shared" si="0"/>
         <v>24107.142857142855</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="5">
         <f t="shared" si="1"/>
         <v>18749.999999999996</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>247</v>
       </c>
       <c r="H23" t="s">
@@ -8042,29 +8656,29 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="5">
         <f>VLOOKUP(B24,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>413000000</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <f>VLOOKUP(B24,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>30357.142857142855</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <f t="shared" si="0"/>
         <v>27321.428571428569</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="5">
         <f t="shared" si="1"/>
         <v>21249.999999999996</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>248</v>
       </c>
       <c r="H24" t="s">
@@ -8072,29 +8686,29 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <f>VLOOKUP(B25,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>415000000</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <f>VLOOKUP(B25,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33035.714285714283</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <f t="shared" si="0"/>
         <v>29732.142857142855</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="5">
         <f t="shared" si="1"/>
         <v>23124.999999999996</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>251</v>
       </c>
       <c r="H25" t="s">
@@ -8102,29 +8716,29 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="5">
         <f>VLOOKUP(B26,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>443000000</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <f>VLOOKUP(B26,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33035.714285714283</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="5">
         <f t="shared" si="0"/>
         <v>29732.142857142855</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="5">
         <f t="shared" si="1"/>
         <v>23124.999999999996</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>249</v>
       </c>
       <c r="H26" t="s">
@@ -8132,29 +8746,29 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="5">
         <f>VLOOKUP(B27,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>443000000</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <f>VLOOKUP(B27,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33035.714285714283</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="5">
         <f t="shared" si="0"/>
         <v>29732.142857142855</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="5">
         <f t="shared" si="1"/>
         <v>23124.999999999996</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>249</v>
       </c>
       <c r="H27" t="s">
@@ -8162,29 +8776,29 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="5">
         <f>VLOOKUP(B28,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>155700000</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="5">
         <f>VLOOKUP(B28,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>10892.857142857141</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="5">
         <f t="shared" si="0"/>
         <v>9803.5714285714275</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="5">
         <f t="shared" si="1"/>
         <v>7624.9999999999982</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>201</v>
       </c>
       <c r="H28" t="s">
@@ -8192,29 +8806,29 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <f>VLOOKUP(B29,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>172600000</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="5">
         <f>VLOOKUP(B29,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>7142.8571428571422</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="5">
         <f t="shared" si="0"/>
         <v>6428.5714285714284</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="5">
         <f t="shared" si="1"/>
         <v>4999.9999999999991</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>230</v>
       </c>
       <c r="H29" t="s">
@@ -8222,29 +8836,29 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <f>VLOOKUP(B30,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>176000000</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="5">
         <f>VLOOKUP(B30,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>12053.571428571428</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="5">
         <f t="shared" si="0"/>
         <v>10848.214285714284</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="5">
         <f t="shared" si="1"/>
         <v>8437.4999999999982</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>238</v>
       </c>
       <c r="H30" t="s">
@@ -8252,29 +8866,29 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="5">
         <f>VLOOKUP(B31,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>168000000</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="5">
         <f>VLOOKUP(B31,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>11160.714285714284</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="5">
         <f t="shared" si="0"/>
         <v>10044.642857142857</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="5">
         <f t="shared" si="1"/>
         <v>7812.4999999999982</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>237</v>
       </c>
       <c r="H31" t="s">
@@ -8282,29 +8896,29 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="5">
         <f>VLOOKUP(B32,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>188300000</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="5">
         <f>VLOOKUP(B32,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>11339.285714285714</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="5">
         <f t="shared" si="0"/>
         <v>10205.357142857143</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="5">
         <f t="shared" si="1"/>
         <v>7937.4999999999991</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>202</v>
       </c>
       <c r="H32" t="s">
@@ -8312,29 +8926,29 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="5">
         <f>VLOOKUP(B33,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>443000000</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="5">
         <f>VLOOKUP(B33,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>33035.714285714283</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="5">
         <f t="shared" si="0"/>
         <v>29732.142857142855</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="5">
         <f t="shared" si="1"/>
         <v>23124.999999999996</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>249</v>
       </c>
       <c r="H33" t="s">
@@ -8342,29 +8956,29 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="5">
         <f>VLOOKUP(B34,[1]pricelist!$B$3:$C$53,2,0)</f>
         <v>345650000</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="5">
         <f>VLOOKUP(B34,[1]pricelist!$B$3:$H$53,7,0)</f>
         <v>22857.142857142855</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="5">
         <f t="shared" si="0"/>
         <v>20571.428571428569</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="5">
         <f t="shared" si="1"/>
         <v>15999.999999999998</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <v>233</v>
       </c>
       <c r="H34" t="s">

</xml_diff>

<commit_message>
UPDATE: Updated Mitra EV vechicle code
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01E09BF-8E46-444D-A9D9-9201054E1B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9164552-B3A7-4C22-A0F9-4EBD03ED6B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="593">
   <si>
     <t>Column1</t>
   </si>
@@ -2339,18 +2339,6 @@
     <t>E260R EV 50KW333LV1YID (4X2) A/T</t>
   </si>
   <si>
-    <t>350VB E1C (4X2) A/T</t>
-  </si>
-  <si>
-    <t>350V E1C (4X2) A/T</t>
-  </si>
-  <si>
-    <t>350VB E2C (4X2) A/T</t>
-  </si>
-  <si>
-    <t>350V E2C (4X2) A/T</t>
-  </si>
-  <si>
     <t>Mitra EV BV 300</t>
   </si>
   <si>
@@ -2361,12 +2349,6 @@
   </si>
   <si>
     <t>Mitra EV MB 400</t>
-  </si>
-  <si>
-    <t>MITRA EV BV</t>
-  </si>
-  <si>
-    <t>MITRA EV MB</t>
   </si>
 </sst>
 </file>
@@ -2558,7 +2540,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2575,22 +2557,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2644,6 +2623,402 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -2919,13 +3294,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2935,6 +3303,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2967,402 +3342,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4921,18 +4900,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I43" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I43" totalsRowShown="0" headerRowDxfId="148" headerRowBorderDxfId="147" tableBorderDxfId="146" totalsRowBorderDxfId="145">
   <autoFilter ref="A1:I43" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0E6335F2-6B6A-436C-92FA-B48E61551308}" name="Merek/Type" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{5A4965DA-398A-4134-90BD-9CE4D8355880}" name="Tipe" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{010303D1-E0A2-4DE6-8E87-64ACC3102E09}" name="Harga OTR Awal" dataDxfId="10" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{91C798B0-7964-436A-84A5-7687993F376F}" name="Dealer Margin" dataDxfId="9" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{CD936623-36F3-4BAA-A615-AF79A61C51E8}" name="Dealer Margin 9 %" dataDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{A36173E8-D9B2-4F38-A572-F5D32CDADEB8}" name="Dealer Margin 7 %" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{7A11B7F5-7683-492A-A8B5-D96984323DDD}" name="Code Unit" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{AF243BB3-2044-4D1E-9F0D-A1EC0D2C15CF}" name="Merk/Type" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{9E0E2E6A-108F-4ACE-959D-9EB0F753BD73}" name="Full Margin" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{0E6335F2-6B6A-436C-92FA-B48E61551308}" name="Merek/Type" dataDxfId="144"/>
+    <tableColumn id="2" xr3:uid="{5A4965DA-398A-4134-90BD-9CE4D8355880}" name="Tipe" dataDxfId="143"/>
+    <tableColumn id="3" xr3:uid="{010303D1-E0A2-4DE6-8E87-64ACC3102E09}" name="Harga OTR Awal" dataDxfId="142" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{91C798B0-7964-436A-84A5-7687993F376F}" name="Dealer Margin" dataDxfId="141" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{CD936623-36F3-4BAA-A615-AF79A61C51E8}" name="Dealer Margin 9 %" dataDxfId="140" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{A36173E8-D9B2-4F38-A572-F5D32CDADEB8}" name="Dealer Margin 7 %" dataDxfId="139" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{7A11B7F5-7683-492A-A8B5-D96984323DDD}" name="Code Unit" dataDxfId="138"/>
+    <tableColumn id="8" xr3:uid="{AF243BB3-2044-4D1E-9F0D-A1EC0D2C15CF}" name="Merk/Type" dataDxfId="137"/>
+    <tableColumn id="9" xr3:uid="{9E0E2E6A-108F-4ACE-959D-9EB0F753BD73}" name="Full Margin" dataDxfId="136"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4942,15 +4921,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}" name="Table009__Page_6" displayName="Table009__Page_6" ref="A1:I16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I16" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5980B244-73E4-43AF-B863-305E8B039C33}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{549208EE-7E07-4F0F-ACFD-9606CC8F6B50}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{086F7B88-A201-47FD-B9A0-0C976108E144}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{CC912184-CE02-4DC9-8815-71C4295C86DF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{8F3F2202-7C07-4D43-B483-871C9E242208}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="78"/>
-    <tableColumn id="6" xr3:uid="{6D2190D6-B434-4BB9-95B1-A29148C453AF}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="77"/>
-    <tableColumn id="7" xr3:uid="{A33DE0AF-7DA7-4623-87E7-DBA2BF4E404A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="76"/>
-    <tableColumn id="8" xr3:uid="{CD689B59-BA44-4F67-9FF9-E08337BE66FD}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="75"/>
-    <tableColumn id="9" xr3:uid="{744F224A-BA1E-4758-B291-8D5C8D341610}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{5980B244-73E4-43AF-B863-305E8B039C33}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{549208EE-7E07-4F0F-ACFD-9606CC8F6B50}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{086F7B88-A201-47FD-B9A0-0C976108E144}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{CC912184-CE02-4DC9-8815-71C4295C86DF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{8F3F2202-7C07-4D43-B483-871C9E242208}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{6D2190D6-B434-4BB9-95B1-A29148C453AF}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{A33DE0AF-7DA7-4623-87E7-DBA2BF4E404A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{CD689B59-BA44-4F67-9FF9-E08337BE66FD}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{744F224A-BA1E-4758-B291-8D5C8D341610}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4960,15 +4939,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}" name="Table010__Page_6" displayName="Table010__Page_6" ref="A18:I20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:I20" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D02866AC-7C8C-4041-B0D6-297717EA2BCA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{F9BA0334-AC0F-4599-91DD-1D3B53530BA2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{2E40CB08-FF90-4211-A5F6-3255AA5CEAED}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{951E49DE-3DB8-41C0-8F36-6E5A1649659D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{D7FC7D23-AA29-4FAE-8DF4-B23A11020D8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{85DA6C7C-BC56-4316-BB56-3D2CA86DF4B0}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{47F39228-8CCC-4319-9964-568280350AF4}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="67"/>
-    <tableColumn id="8" xr3:uid="{781188CD-5AC0-41B9-8575-2EACD4BA90A4}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="66"/>
-    <tableColumn id="9" xr3:uid="{A2DFBEC8-960F-4613-A8B8-821CF42818AC}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{D02866AC-7C8C-4041-B0D6-297717EA2BCA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{F9BA0334-AC0F-4599-91DD-1D3B53530BA2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{2E40CB08-FF90-4211-A5F6-3255AA5CEAED}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{951E49DE-3DB8-41C0-8F36-6E5A1649659D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{D7FC7D23-AA29-4FAE-8DF4-B23A11020D8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{85DA6C7C-BC56-4316-BB56-3D2CA86DF4B0}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{47F39228-8CCC-4319-9964-568280350AF4}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{781188CD-5AC0-41B9-8575-2EACD4BA90A4}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{A2DFBEC8-960F-4613-A8B8-821CF42818AC}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4978,9 +4957,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}" name="Table011__Page_7" displayName="Table011__Page_7" ref="A1:C15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C15" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{384F6B08-E7B1-4ECD-BC7E-1F8C8FC9CD11}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{BD116665-54B3-487B-82AD-7E260403FB1A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{A0C72322-3C63-446F-A7B0-E45538411191}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{384F6B08-E7B1-4ECD-BC7E-1F8C8FC9CD11}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{BD116665-54B3-487B-82AD-7E260403FB1A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{A0C72322-3C63-446F-A7B0-E45538411191}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4990,9 +4969,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}" name="Table012__Page_7" displayName="Table012__Page_7" ref="A17:C19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A17:C19" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{92B56AD9-FE6F-4702-B777-811CB1B6E64F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{C37743D7-7886-43A1-BB26-C0F3914426C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{DFF6BFBF-623A-4318-86AF-C5448FC821A5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{92B56AD9-FE6F-4702-B777-811CB1B6E64F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{C37743D7-7886-43A1-BB26-C0F3914426C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{DFF6BFBF-623A-4318-86AF-C5448FC821A5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5002,11 +4981,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}" name="Table013__Page_8" displayName="Table013__Page_8" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E16" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{811DEB23-A3B8-4E1E-AF98-CBD4FE9515C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{D1233A63-9D37-45F3-9DC7-52977AC06ADC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{400191B1-4CF8-4D78-82E7-FED7CD6730E6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{3D829CC4-4292-4CD0-80B8-3490D4014AC9}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{9BC50CF1-EF44-42B4-9129-E887F74428C9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{811DEB23-A3B8-4E1E-AF98-CBD4FE9515C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{D1233A63-9D37-45F3-9DC7-52977AC06ADC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{400191B1-4CF8-4D78-82E7-FED7CD6730E6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{3D829CC4-4292-4CD0-80B8-3490D4014AC9}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{9BC50CF1-EF44-42B4-9129-E887F74428C9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5016,11 +4995,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}" name="Table014__Page_8" displayName="Table014__Page_8" ref="A18:E21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:E21" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{98A6121C-2EC1-48CA-8A40-28DAFD66423E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{6B521FB3-E639-4556-B8C5-473A63201BC1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{3D07F9E9-4DA3-41C6-98A7-BC28F0C8BFB5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{89F1E0D5-9B1D-4170-BB1D-3FBA7855FC27}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{68E29A0D-4E20-4E2A-A030-157EF3C69E97}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{98A6121C-2EC1-48CA-8A40-28DAFD66423E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{6B521FB3-E639-4556-B8C5-473A63201BC1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{3D07F9E9-4DA3-41C6-98A7-BC28F0C8BFB5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{89F1E0D5-9B1D-4170-BB1D-3FBA7855FC27}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{68E29A0D-4E20-4E2A-A030-157EF3C69E97}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5030,12 +5009,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}" name="Table015__Page_9" displayName="Table015__Page_9" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F16" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B9D47F1B-922B-4B02-855C-93AF62167342}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{9915D8BD-1C99-4D36-BE7E-9EBEAD6D7B12}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{D353D58B-6A1D-4079-A9EC-77376B67A375}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{ACF53426-7425-4D38-9673-B3197A3F9292}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{673A9374-D6DA-46D7-AAD2-6F2220F4ED8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{37C428F9-0692-44D1-B8CF-2CBC7901020B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{B9D47F1B-922B-4B02-855C-93AF62167342}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{9915D8BD-1C99-4D36-BE7E-9EBEAD6D7B12}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{D353D58B-6A1D-4079-A9EC-77376B67A375}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{ACF53426-7425-4D38-9673-B3197A3F9292}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{673A9374-D6DA-46D7-AAD2-6F2220F4ED8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{37C428F9-0692-44D1-B8CF-2CBC7901020B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5045,12 +5024,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}" name="Table016__Page_9" displayName="Table016__Page_9" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:F20" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{48EBD4D1-26EB-449F-8D09-DF1A8D9D96A3}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{671AE648-452F-44F1-9A65-8468F7B19950}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{C3287937-E8A8-4D80-A27C-D2A5C0E44D68}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{49CAB777-0355-40CC-9F2D-C41408ED9E98}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{A19C49CB-F2CF-4D60-B082-761FE4F0ABC5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{801427E9-2562-451E-AE45-ACF6DAAAFFFB}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{48EBD4D1-26EB-449F-8D09-DF1A8D9D96A3}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{671AE648-452F-44F1-9A65-8468F7B19950}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{C3287937-E8A8-4D80-A27C-D2A5C0E44D68}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{49CAB777-0355-40CC-9F2D-C41408ED9E98}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{A19C49CB-F2CF-4D60-B082-761FE4F0ABC5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{801427E9-2562-451E-AE45-ACF6DAAAFFFB}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5060,11 +5039,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}" name="Table017__Page_10" displayName="Table017__Page_10" ref="A1:E15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E15" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{626476ED-551C-48ED-A0F5-9CB680097EF0}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{9215A7DD-9718-48E5-BA20-B6B9989DD0D2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{AE2AC56F-3587-4342-A60B-0B4A30905DD3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{F7BE237D-2C3F-4C27-92EF-2601ABCBA887}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{7950C4F9-8FA4-4C6E-B03A-A0235ECC51FF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{626476ED-551C-48ED-A0F5-9CB680097EF0}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{9215A7DD-9718-48E5-BA20-B6B9989DD0D2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{AE2AC56F-3587-4342-A60B-0B4A30905DD3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{F7BE237D-2C3F-4C27-92EF-2601ABCBA887}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{7950C4F9-8FA4-4C6E-B03A-A0235ECC51FF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5074,11 +5053,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}" name="Table018__Page_10" displayName="Table018__Page_10" ref="A17:E19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A17:E19" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{210B1486-2DC9-4D94-98AC-6BEB874B7545}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{BB67F395-3AAE-4514-BCCE-DE32693EB37D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{230B22CA-5CA3-4E2D-92CC-C75BC5831FF2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{42788CA6-A70D-442A-9072-79E0D19F0B28}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{E37C1038-7442-4E7D-BB43-162AD6FA4195}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{210B1486-2DC9-4D94-98AC-6BEB874B7545}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{BB67F395-3AAE-4514-BCCE-DE32693EB37D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{230B22CA-5CA3-4E2D-92CC-C75BC5831FF2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{42788CA6-A70D-442A-9072-79E0D19F0B28}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{E37C1038-7442-4E7D-BB43-162AD6FA4195}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5088,13 +5067,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}" name="Table001__Page_2" displayName="Table001__Page_2" ref="A1:G16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G16" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A26CE965-72B2-472B-B9FF-D68F7847F3C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="148"/>
-    <tableColumn id="2" xr3:uid="{375BF78E-5806-424A-B7BD-C63C40843BE9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="147"/>
-    <tableColumn id="3" xr3:uid="{CD1FFC74-B097-42B5-B1FA-08D3BD4531B9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="146"/>
-    <tableColumn id="4" xr3:uid="{EA6F5C08-47B3-4BE3-8F9B-3167F2B34338}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="145"/>
-    <tableColumn id="5" xr3:uid="{67D1B145-6151-4A54-9C79-A6B0381CDA09}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="144"/>
-    <tableColumn id="6" xr3:uid="{E8D8899E-ED32-4A2F-B13D-18F4C289A59B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="143"/>
-    <tableColumn id="7" xr3:uid="{CD1BCBB0-10DE-4DDA-903D-C14D16829749}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="142"/>
+    <tableColumn id="1" xr3:uid="{A26CE965-72B2-472B-B9FF-D68F7847F3C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{375BF78E-5806-424A-B7BD-C63C40843BE9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{CD1FFC74-B097-42B5-B1FA-08D3BD4531B9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="133"/>
+    <tableColumn id="4" xr3:uid="{EA6F5C08-47B3-4BE3-8F9B-3167F2B34338}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="132"/>
+    <tableColumn id="5" xr3:uid="{67D1B145-6151-4A54-9C79-A6B0381CDA09}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="131"/>
+    <tableColumn id="6" xr3:uid="{E8D8899E-ED32-4A2F-B13D-18F4C289A59B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="130"/>
+    <tableColumn id="7" xr3:uid="{CD1BCBB0-10DE-4DDA-903D-C14D16829749}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5104,11 +5083,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}" name="Table019__Page_11" displayName="Table019__Page_11" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E16" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{60EAA1C9-E43C-458C-A33C-365CF023541D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{BF4ECEAF-8998-4833-A444-7DD2840947AB}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{A77E13C5-CB25-43C0-9678-51A378FA64FC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{46713ABC-AA6E-45DD-9BBE-03C863D6B1D1}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{85365AB6-280F-40C4-AB42-3455547D61F1}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{60EAA1C9-E43C-458C-A33C-365CF023541D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{BF4ECEAF-8998-4833-A444-7DD2840947AB}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{A77E13C5-CB25-43C0-9678-51A378FA64FC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{46713ABC-AA6E-45DD-9BBE-03C863D6B1D1}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{85365AB6-280F-40C4-AB42-3455547D61F1}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5118,11 +5097,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0B4290D5-7CEE-4DDC-B997-690EEF6D9589}" name="Table020__Page_11" displayName="Table020__Page_11" ref="A18:E20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:E20" xr:uid="{0B4290D5-7CEE-4DDC-B997-690EEF6D9589}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{344C3D84-8C5A-4C60-ADD3-4EE73F83858B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{3470DF86-5A38-429A-95CF-F5FF5E59449C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{BC1BD851-46F6-4634-95EE-ED117E75EBB6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{FF5D3D34-BBDB-4113-8340-C737255ED1BD}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{F05FA152-C9D6-4773-B0A5-5B18B60C7102}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{344C3D84-8C5A-4C60-ADD3-4EE73F83858B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{3470DF86-5A38-429A-95CF-F5FF5E59449C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{BC1BD851-46F6-4634-95EE-ED117E75EBB6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{FF5D3D34-BBDB-4113-8340-C737255ED1BD}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F05FA152-C9D6-4773-B0A5-5B18B60C7102}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5132,13 +5111,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}" name="Table002__Page_2" displayName="Table002__Page_2" ref="A19:G21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A19:G21" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8A3681DA-5FE9-4564-BCAB-75CCDF2C3A51}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{44D6563C-A88C-4FEE-9427-B5252DF8FA5D}" uniqueName="2" name="Column6" queryTableFieldId="2" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{2514D758-49E4-4E3E-A628-2B2D894F398E}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{062470EA-CB73-435C-8DF3-28DE262C8D69}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="138"/>
-    <tableColumn id="5" xr3:uid="{CDE500EE-B268-43D9-A30D-9E6CC1608CD0}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{699F51E2-9A1B-4953-91BE-8D6434D76B20}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{C62D0670-E212-49FF-BA61-22C41F21B60E}" uniqueName="7" name="Column62" queryTableFieldId="7" dataDxfId="135"/>
+    <tableColumn id="1" xr3:uid="{8A3681DA-5FE9-4564-BCAB-75CCDF2C3A51}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="128"/>
+    <tableColumn id="2" xr3:uid="{44D6563C-A88C-4FEE-9427-B5252DF8FA5D}" uniqueName="2" name="Column6" queryTableFieldId="2" dataDxfId="127"/>
+    <tableColumn id="3" xr3:uid="{2514D758-49E4-4E3E-A628-2B2D894F398E}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="126"/>
+    <tableColumn id="4" xr3:uid="{062470EA-CB73-435C-8DF3-28DE262C8D69}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="125"/>
+    <tableColumn id="5" xr3:uid="{CDE500EE-B268-43D9-A30D-9E6CC1608CD0}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="124"/>
+    <tableColumn id="6" xr3:uid="{699F51E2-9A1B-4953-91BE-8D6434D76B20}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="123"/>
+    <tableColumn id="7" xr3:uid="{C62D0670-E212-49FF-BA61-22C41F21B60E}" uniqueName="7" name="Column62" queryTableFieldId="7" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5148,14 +5127,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}" name="Table003__Page_3" displayName="Table003__Page_3" ref="A1:H16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H16" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5E78ED26-3040-4033-A95F-3AC09118D17C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="134"/>
-    <tableColumn id="2" xr3:uid="{52F60F93-88D4-4F60-A15A-4B2113E53BE2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="133"/>
-    <tableColumn id="3" xr3:uid="{2A66B2A9-165C-4995-937F-8E0D8B01B3D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="132"/>
-    <tableColumn id="4" xr3:uid="{937ED0C3-8277-4EC6-BFD2-C6699696538D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="131"/>
-    <tableColumn id="5" xr3:uid="{37EAAABA-4FEF-4D28-B237-360AD0A7194A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="130"/>
-    <tableColumn id="6" xr3:uid="{6E7D50A0-6329-4797-9F9A-628D251C7CA5}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="129"/>
-    <tableColumn id="7" xr3:uid="{F8F31C01-9522-488B-915F-110987168D09}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="128"/>
-    <tableColumn id="8" xr3:uid="{FFD35FDD-AAE7-4F54-8AF3-197380BC0AEB}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="127"/>
+    <tableColumn id="1" xr3:uid="{5E78ED26-3040-4033-A95F-3AC09118D17C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{52F60F93-88D4-4F60-A15A-4B2113E53BE2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{2A66B2A9-165C-4995-937F-8E0D8B01B3D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{937ED0C3-8277-4EC6-BFD2-C6699696538D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{37EAAABA-4FEF-4D28-B237-360AD0A7194A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="117"/>
+    <tableColumn id="6" xr3:uid="{6E7D50A0-6329-4797-9F9A-628D251C7CA5}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{F8F31C01-9522-488B-915F-110987168D09}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="115"/>
+    <tableColumn id="8" xr3:uid="{FFD35FDD-AAE7-4F54-8AF3-197380BC0AEB}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5165,14 +5144,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}" name="Table004__Page_3" displayName="Table004__Page_3" ref="A18:H20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:H20" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A8A6FCCE-AE43-4EDA-82DC-831809E03401}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{0231594E-DA9E-47DE-A01C-22488210A4CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="125"/>
-    <tableColumn id="3" xr3:uid="{7A06306A-69AF-482D-910F-86D0EF88F740}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="124"/>
-    <tableColumn id="4" xr3:uid="{E96F3603-E9D2-4710-BDE5-6FE3E6A378D8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="123"/>
-    <tableColumn id="5" xr3:uid="{37151140-CC9F-4EBB-B58D-F87E1081314A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="122"/>
-    <tableColumn id="6" xr3:uid="{F0AAEEC2-014D-412A-B58D-24C71FEC9A66}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="121"/>
-    <tableColumn id="7" xr3:uid="{A4B4F3F0-B14D-498F-B185-AA3E2BAE729A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="120"/>
-    <tableColumn id="8" xr3:uid="{0C517BB9-44A4-4BBA-AA88-B86BB679F208}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="119"/>
+    <tableColumn id="1" xr3:uid="{A8A6FCCE-AE43-4EDA-82DC-831809E03401}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{0231594E-DA9E-47DE-A01C-22488210A4CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{7A06306A-69AF-482D-910F-86D0EF88F740}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{E96F3603-E9D2-4710-BDE5-6FE3E6A378D8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="110"/>
+    <tableColumn id="5" xr3:uid="{37151140-CC9F-4EBB-B58D-F87E1081314A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="109"/>
+    <tableColumn id="6" xr3:uid="{F0AAEEC2-014D-412A-B58D-24C71FEC9A66}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="108"/>
+    <tableColumn id="7" xr3:uid="{A4B4F3F0-B14D-498F-B185-AA3E2BAE729A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="107"/>
+    <tableColumn id="8" xr3:uid="{0C517BB9-44A4-4BBA-AA88-B86BB679F208}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5182,12 +5161,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}" name="Table005__Page_4" displayName="Table005__Page_4" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F16" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AB42FEA9-5A85-4A69-B46D-444C53C4B4EF}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{0D7919B1-FB5E-4192-8675-3D57B39D9AB0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{94F12F3D-88BF-4BEB-85E7-FF6313F6B88E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{2B04EEA3-DC55-4C69-860F-9571D35E352D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{461C5084-182B-40CC-B479-24798E48D0F4}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{258F7EB6-7345-43CA-BF8A-5E088D06FF8F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{AB42FEA9-5A85-4A69-B46D-444C53C4B4EF}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{0D7919B1-FB5E-4192-8675-3D57B39D9AB0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{94F12F3D-88BF-4BEB-85E7-FF6313F6B88E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{2B04EEA3-DC55-4C69-860F-9571D35E352D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{461C5084-182B-40CC-B479-24798E48D0F4}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{258F7EB6-7345-43CA-BF8A-5E088D06FF8F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5197,12 +5176,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}" name="Table006__Page_4" displayName="Table006__Page_4" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:F20" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{55987721-40E8-4E11-9B6F-67EE503D78F4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{15260D47-39CC-4501-9656-F8DBE6AD3AB1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{06C8B30C-3DD3-49E6-8BE6-C8A9D39F2FC4}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="110"/>
-    <tableColumn id="4" xr3:uid="{40A070F6-4BDB-49A7-9394-4D63F3A9E318}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="109"/>
-    <tableColumn id="5" xr3:uid="{C5E0BAEF-796C-4C71-ACA7-889E63543C2D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="108"/>
-    <tableColumn id="6" xr3:uid="{1BA75280-A961-41F1-B113-5935891BA00A}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="107"/>
+    <tableColumn id="1" xr3:uid="{55987721-40E8-4E11-9B6F-67EE503D78F4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{15260D47-39CC-4501-9656-F8DBE6AD3AB1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{06C8B30C-3DD3-49E6-8BE6-C8A9D39F2FC4}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{40A070F6-4BDB-49A7-9394-4D63F3A9E318}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{C5E0BAEF-796C-4C71-ACA7-889E63543C2D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{1BA75280-A961-41F1-B113-5935891BA00A}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5212,18 +5191,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}" name="Table007__Page_5" displayName="Table007__Page_5" ref="A1:L16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:L16" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9561388E-64AE-4A76-863E-A0B2091E2F9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{151810A9-7DD3-4FD0-91D6-6608DF85A8CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{94D629BF-F745-493D-8F74-FA7EEFDEAA84}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{AE87299A-170F-4661-BD08-B108394E2F7C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{708CB468-5E3F-4D0C-B6BD-C2C44C7191EC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{5D4BD3CB-C344-4155-B3C1-ECC49F86CED1}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{61DF1122-5C54-47A3-98F9-27CA1B50CA9D}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{130590EE-DDCB-43DB-A020-385B521DA018}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="99"/>
-    <tableColumn id="9" xr3:uid="{06B903F7-5E22-476D-A116-655599D2C518}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="98"/>
-    <tableColumn id="10" xr3:uid="{CED96D55-8B0D-492D-B0EC-F3E56EFB2649}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="97"/>
-    <tableColumn id="11" xr3:uid="{346823E9-F305-4F11-941F-1C42A8AB0C99}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="96"/>
-    <tableColumn id="12" xr3:uid="{7B421AA8-C9DB-4E35-A456-DF0F56050B79}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{9561388E-64AE-4A76-863E-A0B2091E2F9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{151810A9-7DD3-4FD0-91D6-6608DF85A8CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{94D629BF-F745-493D-8F74-FA7EEFDEAA84}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{AE87299A-170F-4661-BD08-B108394E2F7C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{708CB468-5E3F-4D0C-B6BD-C2C44C7191EC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{5D4BD3CB-C344-4155-B3C1-ECC49F86CED1}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{61DF1122-5C54-47A3-98F9-27CA1B50CA9D}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="87"/>
+    <tableColumn id="8" xr3:uid="{130590EE-DDCB-43DB-A020-385B521DA018}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="86"/>
+    <tableColumn id="9" xr3:uid="{06B903F7-5E22-476D-A116-655599D2C518}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="85"/>
+    <tableColumn id="10" xr3:uid="{CED96D55-8B0D-492D-B0EC-F3E56EFB2649}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="84"/>
+    <tableColumn id="11" xr3:uid="{346823E9-F305-4F11-941F-1C42A8AB0C99}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="83"/>
+    <tableColumn id="12" xr3:uid="{7B421AA8-C9DB-4E35-A456-DF0F56050B79}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5233,18 +5212,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}" name="Table008__Page_5" displayName="Table008__Page_5" ref="A18:L20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:L20" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{01D3C90B-BA67-46B4-BD1D-5C53486CAE57}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{166854EB-0B50-4420-BB3F-7A5A2C9FB7F7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{638857E5-1EB4-4FBE-9FFE-2951F2F4ABD0}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{F4EFE2EF-AC84-40F8-BE68-0B6B520F8EA8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{38D026D2-A47E-46EA-BA10-AF890A55BF2B}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="90"/>
-    <tableColumn id="6" xr3:uid="{025C6DA2-37A6-491F-904E-DDE12948D35B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="89"/>
-    <tableColumn id="7" xr3:uid="{AC28B573-67B7-4468-A6A2-F648D17079B6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="88"/>
-    <tableColumn id="8" xr3:uid="{F6F06554-210B-472F-95F2-8E89D931E4C1}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="87"/>
-    <tableColumn id="9" xr3:uid="{F0A8F323-36C1-4290-980B-8F6F5DC6A41E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="86"/>
-    <tableColumn id="10" xr3:uid="{25D60007-5007-4174-85F5-572E3C29FE33}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="85"/>
-    <tableColumn id="11" xr3:uid="{2071EB9B-B14E-4EF0-9B86-0D5FDA96828D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="84"/>
-    <tableColumn id="12" xr3:uid="{1660C180-EE6B-48E8-9880-55F02CC623C4}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{01D3C90B-BA67-46B4-BD1D-5C53486CAE57}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{166854EB-0B50-4420-BB3F-7A5A2C9FB7F7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{638857E5-1EB4-4FBE-9FFE-2951F2F4ABD0}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{F4EFE2EF-AC84-40F8-BE68-0B6B520F8EA8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{38D026D2-A47E-46EA-BA10-AF890A55BF2B}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{025C6DA2-37A6-491F-904E-DDE12948D35B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{AC28B573-67B7-4468-A6A2-F648D17079B6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{F6F06554-210B-472F-95F2-8E89D931E4C1}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="74"/>
+    <tableColumn id="9" xr3:uid="{F0A8F323-36C1-4290-980B-8F6F5DC6A41E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="73"/>
+    <tableColumn id="10" xr3:uid="{25D60007-5007-4174-85F5-572E3C29FE33}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="72"/>
+    <tableColumn id="11" xr3:uid="{2071EB9B-B14E-4EF0-9B86-0D5FDA96828D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="71"/>
+    <tableColumn id="12" xr3:uid="{1660C180-EE6B-48E8-9880-55F02CC623C4}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5550,8 +5529,8 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5589,36 +5568,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>551</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>553</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>562</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>563</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>552</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="16" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>514</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -5645,12 +5624,12 @@
       <c r="H2" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="13">
         <v>35000000</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>547</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5677,12 +5656,12 @@
       <c r="H3" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="13">
         <v>32999999.999999996</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>515</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -5709,12 +5688,12 @@
       <c r="H4" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <v>23249999.999999996</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>516</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -5741,12 +5720,12 @@
       <c r="H5" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="13">
         <v>24700000.000000004</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>496</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5773,12 +5752,12 @@
       <c r="H6" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="13">
         <v>35000000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>497</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -5805,12 +5784,12 @@
       <c r="H7" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="13">
         <v>38000000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>517</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -5837,12 +5816,12 @@
       <c r="H8" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="13">
         <v>23000000</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>518</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5869,12 +5848,12 @@
       <c r="H9" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="13">
         <v>20000000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>519</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -5901,12 +5880,12 @@
       <c r="H10" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="13">
         <v>13000000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>523</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -5933,12 +5912,12 @@
       <c r="H11" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="13">
         <v>12700000.000000002</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>524</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5965,12 +5944,12 @@
       <c r="H12" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="13">
         <v>16000000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>498</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -5997,12 +5976,12 @@
       <c r="H13" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="13">
         <v>14700000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>527</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -6029,12 +6008,12 @@
       <c r="H14" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="13">
         <v>20900000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>528</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -6061,12 +6040,12 @@
       <c r="H15" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="13">
         <v>22000000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>525</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -6093,12 +6072,12 @@
       <c r="H16" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="13">
         <v>18300000</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>499</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -6125,12 +6104,12 @@
       <c r="H17" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="13">
         <v>20500000.000000004</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>580</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -6157,12 +6136,12 @@
       <c r="H18" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="13">
         <v>21000000.000000004</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>555</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -6189,12 +6168,12 @@
       <c r="H19" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="13">
         <v>21000000.000000004</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>500</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -6221,12 +6200,12 @@
       <c r="H20" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="13">
         <v>21000000.000000004</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>501</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -6253,12 +6232,12 @@
       <c r="H21" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="13">
         <v>21000000.000000004</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>502</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -6285,12 +6264,12 @@
       <c r="H22" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="13">
         <v>24999999.999999996</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>503</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -6317,12 +6296,12 @@
       <c r="H23" s="4" t="s">
         <v>576</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I23" s="13">
         <v>29000000</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>504</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -6349,12 +6328,12 @@
       <c r="H24" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I24" s="13">
         <v>30000000</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>588</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -6381,12 +6360,12 @@
       <c r="H25" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="13">
         <v>29000000</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>505</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -6413,12 +6392,12 @@
       <c r="H26" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="13">
         <v>34000000</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>586</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -6445,12 +6424,12 @@
       <c r="H27" s="4" t="s">
         <v>576</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="13">
         <v>26000000</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="11" t="s">
         <v>587</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -6477,12 +6456,12 @@
       <c r="H28" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="I28" s="15">
+      <c r="I28" s="13">
         <v>29000000</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>557</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -6509,12 +6488,12 @@
       <c r="H29" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="I29" s="15">
+      <c r="I29" s="13">
         <v>37000000</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>582</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -6541,12 +6520,12 @@
       <c r="H30" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I30" s="13">
         <v>37000000</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>558</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -6573,12 +6552,12 @@
       <c r="H31" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="I31" s="15">
+      <c r="I31" s="13">
         <v>37000000</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>506</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -6605,12 +6584,12 @@
       <c r="H32" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="I32" s="15">
+      <c r="I32" s="13">
         <v>37000000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>529</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -6637,12 +6616,12 @@
       <c r="H33" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="I33" s="15">
+      <c r="I33" s="13">
         <v>12200000</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="11" t="s">
         <v>520</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -6669,12 +6648,12 @@
       <c r="H34" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="I34" s="15">
+      <c r="I34" s="13">
         <v>8000000</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>521</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -6701,12 +6680,12 @@
       <c r="H35" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="I35" s="15">
+      <c r="I35" s="13">
         <v>13500000</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="11" t="s">
         <v>526</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -6733,12 +6712,12 @@
       <c r="H36" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="I36" s="15">
+      <c r="I36" s="13">
         <v>12499999.999999998</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="11" t="s">
         <v>560</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -6765,12 +6744,12 @@
       <c r="H37" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="I37" s="15">
+      <c r="I37" s="13">
         <v>12700000.000000002</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="11" t="s">
         <v>561</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -6797,12 +6776,12 @@
       <c r="H38" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="I38" s="15">
+      <c r="I38" s="13">
         <v>37000000</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="12" t="s">
         <v>522</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -6829,135 +6808,135 @@
       <c r="H39" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="I39" s="15">
+      <c r="I39" s="13">
         <v>25600000</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="11" t="s">
         <v>589</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>593</v>
-      </c>
-      <c r="C40" s="11">
+      <c r="B40" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="C40" s="10">
         <v>328000000</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="10">
         <f t="shared" si="0"/>
         <v>17857142.857142854</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E40" s="10">
         <f t="shared" si="14"/>
         <v>16071428.571428569</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F40" s="10">
         <f t="shared" si="15"/>
         <v>12499999.999999998</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G40" s="21">
         <v>254</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="I40" s="15">
+        <v>589</v>
+      </c>
+      <c r="I40" s="13">
         <v>20000000</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="11" t="s">
         <v>590</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>594</v>
-      </c>
-      <c r="C41" s="11">
+      <c r="B41" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C41" s="10">
         <v>348000000</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="10">
         <f t="shared" si="0"/>
         <v>17857142.857142854</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E41" s="10">
         <f t="shared" si="14"/>
         <v>16071428.571428569</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F41" s="10">
         <f t="shared" si="15"/>
         <v>12499999.999999998</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="21">
         <v>256</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="I41" s="16">
+        <v>590</v>
+      </c>
+      <c r="I41" s="13">
         <v>20000000</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="11" t="s">
         <v>591</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>595</v>
-      </c>
-      <c r="C42" s="11">
+      <c r="B42" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C42" s="10">
         <v>358000000</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="10">
         <f t="shared" si="0"/>
         <v>22321428.571428571</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E42" s="10">
         <f t="shared" si="14"/>
         <v>20089285.714285713</v>
       </c>
-      <c r="F42" s="11">
+      <c r="F42" s="10">
         <f t="shared" si="15"/>
         <v>15624999.999999998</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G42" s="21">
         <v>255</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="I42" s="16">
+        <v>591</v>
+      </c>
+      <c r="I42" s="13">
         <v>25000000</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="17" t="s">
         <v>592</v>
       </c>
-      <c r="B43" s="21" t="s">
-        <v>596</v>
-      </c>
-      <c r="C43" s="22">
+      <c r="B43" s="18" t="s">
+        <v>592</v>
+      </c>
+      <c r="C43" s="19">
         <v>378000000</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="10">
         <f t="shared" ref="D43" si="16">I43/1.12</f>
         <v>22321428.571428571</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E43" s="10">
         <f t="shared" ref="E43" si="17">D43*90%</f>
         <v>20089285.714285713</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="10">
         <f t="shared" ref="F43" si="18">D43*70%</f>
         <v>15624999.999999998</v>
       </c>
-      <c r="G43" s="25">
+      <c r="G43" s="22">
         <v>257</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="I43" s="23">
+      <c r="H43" s="18" t="s">
+        <v>592</v>
+      </c>
+      <c r="I43" s="20">
         <v>25000000</v>
       </c>
     </row>
@@ -6965,11 +6944,11 @@
       <c r="D48" s="9"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A29 A31:A43">
+    <cfRule type="duplicateValues" dxfId="3" priority="10"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A31:A38 A2:A29 A40:A43">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A29 A31:A43">
-    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
UPDATE: Meta data November 2025
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E23BC3-2BDC-45F2-B4B8-99BF0B875FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD6C0A-3216-4268-BA87-FA4CE27D95DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="605">
   <si>
     <t>Column1</t>
   </si>
@@ -2361,6 +2361,30 @@
   </si>
   <si>
     <t>MITRA EV MB 400</t>
+  </si>
+  <si>
+    <t>DARION EV LV1</t>
+  </si>
+  <si>
+    <t>520M E1D (4X2) A/T</t>
+  </si>
+  <si>
+    <t>DARION EV LV2</t>
+  </si>
+  <si>
+    <t>520M E2D (4X2) A/T</t>
+  </si>
+  <si>
+    <t>DARION PHEV LV1</t>
+  </si>
+  <si>
+    <t>520M P2D (4X2) A/T</t>
+  </si>
+  <si>
+    <t>DARION PHEV LV2</t>
+  </si>
+  <si>
+    <t>520M P3D (4X2) A/T</t>
   </si>
 </sst>
 </file>
@@ -2552,7 +2576,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2588,6 +2612,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -4932,8 +4962,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I43" totalsRowShown="0" headerRowDxfId="150" headerRowBorderDxfId="149" tableBorderDxfId="148" totalsRowBorderDxfId="147">
-  <autoFilter ref="A1:I43" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I47" totalsRowShown="0" headerRowDxfId="150" headerRowBorderDxfId="149" tableBorderDxfId="148" totalsRowBorderDxfId="147">
+  <autoFilter ref="A1:I47" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0E6335F2-6B6A-436C-92FA-B48E61551308}" name="Merek/Type" dataDxfId="146"/>
     <tableColumn id="2" xr3:uid="{5A4965DA-398A-4134-90BD-9CE4D8355880}" name="Tipe" dataDxfId="145"/>
@@ -5562,7 +5592,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40:H43"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6951,15 +6981,15 @@
         <v>378000000</v>
       </c>
       <c r="D43" s="10">
-        <f t="shared" ref="D43" si="16">I43/1.12</f>
+        <f t="shared" ref="D43:D47" si="16">I43/1.12</f>
         <v>22321428.571428571</v>
       </c>
       <c r="E43" s="10">
-        <f t="shared" ref="E43" si="17">D43*90%</f>
+        <f t="shared" ref="E43:E47" si="17">D43*90%</f>
         <v>20089285.714285713</v>
       </c>
       <c r="F43" s="10">
-        <f t="shared" ref="F43" si="18">D43*70%</f>
+        <f t="shared" ref="F43:F47" si="18">D43*70%</f>
         <v>15624999.999999998</v>
       </c>
       <c r="G43" s="22">
@@ -6970,6 +7000,134 @@
       </c>
       <c r="I43" s="20">
         <v>25000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="23" t="s">
+        <v>597</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>598</v>
+      </c>
+      <c r="C44" s="10">
+        <v>399000000</v>
+      </c>
+      <c r="D44" s="10">
+        <f t="shared" si="16"/>
+        <v>28214285.714285713</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" si="17"/>
+        <v>25392857.142857142</v>
+      </c>
+      <c r="F44" s="10">
+        <f t="shared" si="18"/>
+        <v>19749999.999999996</v>
+      </c>
+      <c r="G44" s="21">
+        <v>258</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="I44" s="25">
+        <v>31600000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="23" t="s">
+        <v>599</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>600</v>
+      </c>
+      <c r="C45" s="10">
+        <v>459000000</v>
+      </c>
+      <c r="D45" s="10">
+        <f t="shared" si="16"/>
+        <v>32499999.999999996</v>
+      </c>
+      <c r="E45" s="10">
+        <f t="shared" si="17"/>
+        <v>29249999.999999996</v>
+      </c>
+      <c r="F45" s="10">
+        <f t="shared" si="18"/>
+        <v>22749999.999999996</v>
+      </c>
+      <c r="G45" s="21">
+        <v>259</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="I45" s="25">
+        <v>36400000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="23" t="s">
+        <v>601</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="C46" s="10">
+        <v>449000000</v>
+      </c>
+      <c r="D46" s="10">
+        <f t="shared" si="16"/>
+        <v>29196428.571428567</v>
+      </c>
+      <c r="E46" s="10">
+        <f t="shared" si="17"/>
+        <v>26276785.714285713</v>
+      </c>
+      <c r="F46" s="10">
+        <f t="shared" si="18"/>
+        <v>20437499.999999996</v>
+      </c>
+      <c r="G46" s="21">
+        <v>260</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="I46" s="25">
+        <v>32700000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="26" t="s">
+        <v>603</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>604</v>
+      </c>
+      <c r="C47" s="19">
+        <v>499000000</v>
+      </c>
+      <c r="D47" s="19">
+        <f t="shared" si="16"/>
+        <v>32499999.999999996</v>
+      </c>
+      <c r="E47" s="19">
+        <f t="shared" si="17"/>
+        <v>29249999.999999996</v>
+      </c>
+      <c r="F47" s="19">
+        <f t="shared" si="18"/>
+        <v>22749999.999999996</v>
+      </c>
+      <c r="G47" s="22">
+        <v>261</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>603</v>
+      </c>
+      <c r="I47" s="28">
+        <v>36400000</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -6983,10 +7141,8 @@
     <cfRule type="duplicateValues" dxfId="4" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:H43">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40:H43">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -9004,10 +9160,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A33">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A34">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UPDATE: Pricelist December 2025
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6E663F-34C0-4FEC-8D5A-11C276771AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2B87BF-BC2C-4C56-8D3E-BF360BDEE8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -2366,9 +2366,6 @@
     <t>DARION EV LV1</t>
   </si>
   <si>
-    <t>520M E1D (4X2) A/T</t>
-  </si>
-  <si>
     <t>DARION EV LV2</t>
   </si>
   <si>
@@ -2397,6 +2394,9 @@
   </si>
   <si>
     <t>350VB E2C (4X2) A/T</t>
+  </si>
+  <si>
+    <t>520M E1C (4X2) A/T</t>
   </si>
 </sst>
 </file>
@@ -2630,27 +2630,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DA2601EE-1999-4BF8-AF5E-538A4398209C}"/>
     <cellStyle name="Normal 2 2" xfId="3" xr:uid="{8C240942-BC33-4996-847D-14CFBB46F4A3}"/>
   </cellStyles>
-  <dxfs count="155">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="153">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5007,18 +4987,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I51" totalsRowShown="0" headerRowDxfId="154" headerRowBorderDxfId="153" tableBorderDxfId="152" totalsRowBorderDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I51" totalsRowShown="0" headerRowDxfId="152" headerRowBorderDxfId="151" tableBorderDxfId="150" totalsRowBorderDxfId="149">
   <autoFilter ref="A1:I51" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0E6335F2-6B6A-436C-92FA-B48E61551308}" name="Merek/Type" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{5A4965DA-398A-4134-90BD-9CE4D8355880}" name="Tipe" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{010303D1-E0A2-4DE6-8E87-64ACC3102E09}" name="Harga OTR Awal" dataDxfId="148" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{91C798B0-7964-436A-84A5-7687993F376F}" name="Dealer Margin" dataDxfId="147" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{CD936623-36F3-4BAA-A615-AF79A61C51E8}" name="Dealer Margin 9 %" dataDxfId="146" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{A36173E8-D9B2-4F38-A572-F5D32CDADEB8}" name="Dealer Margin 7 %" dataDxfId="145" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{7A11B7F5-7683-492A-A8B5-D96984323DDD}" name="Code Unit" dataDxfId="144"/>
-    <tableColumn id="8" xr3:uid="{AF243BB3-2044-4D1E-9F0D-A1EC0D2C15CF}" name="Merk/Type" dataDxfId="143"/>
-    <tableColumn id="9" xr3:uid="{9E0E2E6A-108F-4ACE-959D-9EB0F753BD73}" name="Full Margin" dataDxfId="142"/>
+    <tableColumn id="1" xr3:uid="{0E6335F2-6B6A-436C-92FA-B48E61551308}" name="Merek/Type" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{5A4965DA-398A-4134-90BD-9CE4D8355880}" name="Tipe" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{010303D1-E0A2-4DE6-8E87-64ACC3102E09}" name="Harga OTR Awal" dataDxfId="146" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{91C798B0-7964-436A-84A5-7687993F376F}" name="Dealer Margin" dataDxfId="145" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{CD936623-36F3-4BAA-A615-AF79A61C51E8}" name="Dealer Margin 9 %" dataDxfId="144" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{A36173E8-D9B2-4F38-A572-F5D32CDADEB8}" name="Dealer Margin 7 %" dataDxfId="143" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{7A11B7F5-7683-492A-A8B5-D96984323DDD}" name="Code Unit" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{AF243BB3-2044-4D1E-9F0D-A1EC0D2C15CF}" name="Merk/Type" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{9E0E2E6A-108F-4ACE-959D-9EB0F753BD73}" name="Full Margin" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5028,15 +5008,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}" name="Table009__Page_6" displayName="Table009__Page_6" ref="A1:I16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I16" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5980B244-73E4-43AF-B863-305E8B039C33}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{549208EE-7E07-4F0F-ACFD-9606CC8F6B50}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{086F7B88-A201-47FD-B9A0-0C976108E144}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{CC912184-CE02-4DC9-8815-71C4295C86DF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{8F3F2202-7C07-4D43-B483-871C9E242208}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{6D2190D6-B434-4BB9-95B1-A29148C453AF}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{A33DE0AF-7DA7-4623-87E7-DBA2BF4E404A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{CD689B59-BA44-4F67-9FF9-E08337BE66FD}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{744F224A-BA1E-4758-B291-8D5C8D341610}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{5980B244-73E4-43AF-B863-305E8B039C33}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{549208EE-7E07-4F0F-ACFD-9606CC8F6B50}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{086F7B88-A201-47FD-B9A0-0C976108E144}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{CC912184-CE02-4DC9-8815-71C4295C86DF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{8F3F2202-7C07-4D43-B483-871C9E242208}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{6D2190D6-B434-4BB9-95B1-A29148C453AF}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{A33DE0AF-7DA7-4623-87E7-DBA2BF4E404A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{CD689B59-BA44-4F67-9FF9-E08337BE66FD}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{744F224A-BA1E-4758-B291-8D5C8D341610}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5046,15 +5026,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}" name="Table010__Page_6" displayName="Table010__Page_6" ref="A18:I20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:I20" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D02866AC-7C8C-4041-B0D6-297717EA2BCA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{F9BA0334-AC0F-4599-91DD-1D3B53530BA2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{2E40CB08-FF90-4211-A5F6-3255AA5CEAED}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{951E49DE-3DB8-41C0-8F36-6E5A1649659D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{D7FC7D23-AA29-4FAE-8DF4-B23A11020D8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{85DA6C7C-BC56-4316-BB56-3D2CA86DF4B0}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{47F39228-8CCC-4319-9964-568280350AF4}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{781188CD-5AC0-41B9-8575-2EACD4BA90A4}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{A2DFBEC8-960F-4613-A8B8-821CF42818AC}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{D02866AC-7C8C-4041-B0D6-297717EA2BCA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{F9BA0334-AC0F-4599-91DD-1D3B53530BA2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{2E40CB08-FF90-4211-A5F6-3255AA5CEAED}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{951E49DE-3DB8-41C0-8F36-6E5A1649659D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{D7FC7D23-AA29-4FAE-8DF4-B23A11020D8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{85DA6C7C-BC56-4316-BB56-3D2CA86DF4B0}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{47F39228-8CCC-4319-9964-568280350AF4}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{781188CD-5AC0-41B9-8575-2EACD4BA90A4}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{A2DFBEC8-960F-4613-A8B8-821CF42818AC}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5064,9 +5044,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}" name="Table011__Page_7" displayName="Table011__Page_7" ref="A1:C15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C15" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{384F6B08-E7B1-4ECD-BC7E-1F8C8FC9CD11}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{BD116665-54B3-487B-82AD-7E260403FB1A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{A0C72322-3C63-446F-A7B0-E45538411191}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{384F6B08-E7B1-4ECD-BC7E-1F8C8FC9CD11}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{BD116665-54B3-487B-82AD-7E260403FB1A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{A0C72322-3C63-446F-A7B0-E45538411191}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5076,9 +5056,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}" name="Table012__Page_7" displayName="Table012__Page_7" ref="A17:C19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A17:C19" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{92B56AD9-FE6F-4702-B777-811CB1B6E64F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{C37743D7-7886-43A1-BB26-C0F3914426C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{DFF6BFBF-623A-4318-86AF-C5448FC821A5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{92B56AD9-FE6F-4702-B777-811CB1B6E64F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{C37743D7-7886-43A1-BB26-C0F3914426C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{DFF6BFBF-623A-4318-86AF-C5448FC821A5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5088,11 +5068,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}" name="Table013__Page_8" displayName="Table013__Page_8" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E16" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{811DEB23-A3B8-4E1E-AF98-CBD4FE9515C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{D1233A63-9D37-45F3-9DC7-52977AC06ADC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{400191B1-4CF8-4D78-82E7-FED7CD6730E6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{3D829CC4-4292-4CD0-80B8-3490D4014AC9}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{9BC50CF1-EF44-42B4-9129-E887F74428C9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{811DEB23-A3B8-4E1E-AF98-CBD4FE9515C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{D1233A63-9D37-45F3-9DC7-52977AC06ADC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{400191B1-4CF8-4D78-82E7-FED7CD6730E6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{3D829CC4-4292-4CD0-80B8-3490D4014AC9}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{9BC50CF1-EF44-42B4-9129-E887F74428C9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5102,11 +5082,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}" name="Table014__Page_8" displayName="Table014__Page_8" ref="A18:E21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:E21" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{98A6121C-2EC1-48CA-8A40-28DAFD66423E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{6B521FB3-E639-4556-B8C5-473A63201BC1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{3D07F9E9-4DA3-41C6-98A7-BC28F0C8BFB5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{89F1E0D5-9B1D-4170-BB1D-3FBA7855FC27}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{68E29A0D-4E20-4E2A-A030-157EF3C69E97}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{98A6121C-2EC1-48CA-8A40-28DAFD66423E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{6B521FB3-E639-4556-B8C5-473A63201BC1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{3D07F9E9-4DA3-41C6-98A7-BC28F0C8BFB5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{89F1E0D5-9B1D-4170-BB1D-3FBA7855FC27}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{68E29A0D-4E20-4E2A-A030-157EF3C69E97}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5116,12 +5096,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}" name="Table015__Page_9" displayName="Table015__Page_9" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F16" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B9D47F1B-922B-4B02-855C-93AF62167342}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{9915D8BD-1C99-4D36-BE7E-9EBEAD6D7B12}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{D353D58B-6A1D-4079-A9EC-77376B67A375}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{ACF53426-7425-4D38-9673-B3197A3F9292}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{673A9374-D6DA-46D7-AAD2-6F2220F4ED8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{37C428F9-0692-44D1-B8CF-2CBC7901020B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{B9D47F1B-922B-4B02-855C-93AF62167342}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{9915D8BD-1C99-4D36-BE7E-9EBEAD6D7B12}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{D353D58B-6A1D-4079-A9EC-77376B67A375}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{ACF53426-7425-4D38-9673-B3197A3F9292}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{673A9374-D6DA-46D7-AAD2-6F2220F4ED8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{37C428F9-0692-44D1-B8CF-2CBC7901020B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5131,12 +5111,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}" name="Table016__Page_9" displayName="Table016__Page_9" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:F20" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{48EBD4D1-26EB-449F-8D09-DF1A8D9D96A3}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{671AE648-452F-44F1-9A65-8468F7B19950}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{C3287937-E8A8-4D80-A27C-D2A5C0E44D68}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{49CAB777-0355-40CC-9F2D-C41408ED9E98}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{A19C49CB-F2CF-4D60-B082-761FE4F0ABC5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{801427E9-2562-451E-AE45-ACF6DAAAFFFB}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{48EBD4D1-26EB-449F-8D09-DF1A8D9D96A3}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{671AE648-452F-44F1-9A65-8468F7B19950}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{C3287937-E8A8-4D80-A27C-D2A5C0E44D68}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{49CAB777-0355-40CC-9F2D-C41408ED9E98}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{A19C49CB-F2CF-4D60-B082-761FE4F0ABC5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{801427E9-2562-451E-AE45-ACF6DAAAFFFB}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5146,11 +5126,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}" name="Table017__Page_10" displayName="Table017__Page_10" ref="A1:E15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E15" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{626476ED-551C-48ED-A0F5-9CB680097EF0}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{9215A7DD-9718-48E5-BA20-B6B9989DD0D2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{AE2AC56F-3587-4342-A60B-0B4A30905DD3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{F7BE237D-2C3F-4C27-92EF-2601ABCBA887}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{7950C4F9-8FA4-4C6E-B03A-A0235ECC51FF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{626476ED-551C-48ED-A0F5-9CB680097EF0}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{9215A7DD-9718-48E5-BA20-B6B9989DD0D2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{AE2AC56F-3587-4342-A60B-0B4A30905DD3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{F7BE237D-2C3F-4C27-92EF-2601ABCBA887}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{7950C4F9-8FA4-4C6E-B03A-A0235ECC51FF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5160,11 +5140,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}" name="Table018__Page_10" displayName="Table018__Page_10" ref="A17:E19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A17:E19" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{210B1486-2DC9-4D94-98AC-6BEB874B7545}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{BB67F395-3AAE-4514-BCCE-DE32693EB37D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{230B22CA-5CA3-4E2D-92CC-C75BC5831FF2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{42788CA6-A70D-442A-9072-79E0D19F0B28}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{E37C1038-7442-4E7D-BB43-162AD6FA4195}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{210B1486-2DC9-4D94-98AC-6BEB874B7545}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{BB67F395-3AAE-4514-BCCE-DE32693EB37D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{230B22CA-5CA3-4E2D-92CC-C75BC5831FF2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{42788CA6-A70D-442A-9072-79E0D19F0B28}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{E37C1038-7442-4E7D-BB43-162AD6FA4195}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5174,13 +5154,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}" name="Table001__Page_2" displayName="Table001__Page_2" ref="A1:G16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G16" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A26CE965-72B2-472B-B9FF-D68F7847F3C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{375BF78E-5806-424A-B7BD-C63C40843BE9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{CD1FFC74-B097-42B5-B1FA-08D3BD4531B9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{EA6F5C08-47B3-4BE3-8F9B-3167F2B34338}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="138"/>
-    <tableColumn id="5" xr3:uid="{67D1B145-6151-4A54-9C79-A6B0381CDA09}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{E8D8899E-ED32-4A2F-B13D-18F4C289A59B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{CD1BCBB0-10DE-4DDA-903D-C14D16829749}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="135"/>
+    <tableColumn id="1" xr3:uid="{A26CE965-72B2-472B-B9FF-D68F7847F3C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="139"/>
+    <tableColumn id="2" xr3:uid="{375BF78E-5806-424A-B7BD-C63C40843BE9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="138"/>
+    <tableColumn id="3" xr3:uid="{CD1FFC74-B097-42B5-B1FA-08D3BD4531B9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="137"/>
+    <tableColumn id="4" xr3:uid="{EA6F5C08-47B3-4BE3-8F9B-3167F2B34338}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="136"/>
+    <tableColumn id="5" xr3:uid="{67D1B145-6151-4A54-9C79-A6B0381CDA09}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="135"/>
+    <tableColumn id="6" xr3:uid="{E8D8899E-ED32-4A2F-B13D-18F4C289A59B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="134"/>
+    <tableColumn id="7" xr3:uid="{CD1BCBB0-10DE-4DDA-903D-C14D16829749}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="133"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5190,11 +5170,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}" name="Table019__Page_11" displayName="Table019__Page_11" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E16" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{60EAA1C9-E43C-458C-A33C-365CF023541D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{BF4ECEAF-8998-4833-A444-7DD2840947AB}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{A77E13C5-CB25-43C0-9678-51A378FA64FC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{46713ABC-AA6E-45DD-9BBE-03C863D6B1D1}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{85365AB6-280F-40C4-AB42-3455547D61F1}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{60EAA1C9-E43C-458C-A33C-365CF023541D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{BF4ECEAF-8998-4833-A444-7DD2840947AB}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{A77E13C5-CB25-43C0-9678-51A378FA64FC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{46713ABC-AA6E-45DD-9BBE-03C863D6B1D1}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{85365AB6-280F-40C4-AB42-3455547D61F1}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5204,11 +5184,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0B4290D5-7CEE-4DDC-B997-690EEF6D9589}" name="Table020__Page_11" displayName="Table020__Page_11" ref="A18:E20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:E20" xr:uid="{0B4290D5-7CEE-4DDC-B997-690EEF6D9589}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{344C3D84-8C5A-4C60-ADD3-4EE73F83858B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{3470DF86-5A38-429A-95CF-F5FF5E59449C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{BC1BD851-46F6-4634-95EE-ED117E75EBB6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{FF5D3D34-BBDB-4113-8340-C737255ED1BD}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{F05FA152-C9D6-4773-B0A5-5B18B60C7102}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{344C3D84-8C5A-4C60-ADD3-4EE73F83858B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{3470DF86-5A38-429A-95CF-F5FF5E59449C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{BC1BD851-46F6-4634-95EE-ED117E75EBB6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{FF5D3D34-BBDB-4113-8340-C737255ED1BD}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{F05FA152-C9D6-4773-B0A5-5B18B60C7102}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5218,13 +5198,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}" name="Table002__Page_2" displayName="Table002__Page_2" ref="A19:G21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A19:G21" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8A3681DA-5FE9-4564-BCAB-75CCDF2C3A51}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="134"/>
-    <tableColumn id="2" xr3:uid="{44D6563C-A88C-4FEE-9427-B5252DF8FA5D}" uniqueName="2" name="Column6" queryTableFieldId="2" dataDxfId="133"/>
-    <tableColumn id="3" xr3:uid="{2514D758-49E4-4E3E-A628-2B2D894F398E}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="132"/>
-    <tableColumn id="4" xr3:uid="{062470EA-CB73-435C-8DF3-28DE262C8D69}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="131"/>
-    <tableColumn id="5" xr3:uid="{CDE500EE-B268-43D9-A30D-9E6CC1608CD0}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="130"/>
-    <tableColumn id="6" xr3:uid="{699F51E2-9A1B-4953-91BE-8D6434D76B20}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="129"/>
-    <tableColumn id="7" xr3:uid="{C62D0670-E212-49FF-BA61-22C41F21B60E}" uniqueName="7" name="Column62" queryTableFieldId="7" dataDxfId="128"/>
+    <tableColumn id="1" xr3:uid="{8A3681DA-5FE9-4564-BCAB-75CCDF2C3A51}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="132"/>
+    <tableColumn id="2" xr3:uid="{44D6563C-A88C-4FEE-9427-B5252DF8FA5D}" uniqueName="2" name="Column6" queryTableFieldId="2" dataDxfId="131"/>
+    <tableColumn id="3" xr3:uid="{2514D758-49E4-4E3E-A628-2B2D894F398E}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{062470EA-CB73-435C-8DF3-28DE262C8D69}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="129"/>
+    <tableColumn id="5" xr3:uid="{CDE500EE-B268-43D9-A30D-9E6CC1608CD0}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="128"/>
+    <tableColumn id="6" xr3:uid="{699F51E2-9A1B-4953-91BE-8D6434D76B20}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="127"/>
+    <tableColumn id="7" xr3:uid="{C62D0670-E212-49FF-BA61-22C41F21B60E}" uniqueName="7" name="Column62" queryTableFieldId="7" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5234,14 +5214,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}" name="Table003__Page_3" displayName="Table003__Page_3" ref="A1:H16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H16" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5E78ED26-3040-4033-A95F-3AC09118D17C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="127"/>
-    <tableColumn id="2" xr3:uid="{52F60F93-88D4-4F60-A15A-4B2113E53BE2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="126"/>
-    <tableColumn id="3" xr3:uid="{2A66B2A9-165C-4995-937F-8E0D8B01B3D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="125"/>
-    <tableColumn id="4" xr3:uid="{937ED0C3-8277-4EC6-BFD2-C6699696538D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="124"/>
-    <tableColumn id="5" xr3:uid="{37EAAABA-4FEF-4D28-B237-360AD0A7194A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="123"/>
-    <tableColumn id="6" xr3:uid="{6E7D50A0-6329-4797-9F9A-628D251C7CA5}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="122"/>
-    <tableColumn id="7" xr3:uid="{F8F31C01-9522-488B-915F-110987168D09}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="121"/>
-    <tableColumn id="8" xr3:uid="{FFD35FDD-AAE7-4F54-8AF3-197380BC0AEB}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{5E78ED26-3040-4033-A95F-3AC09118D17C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{52F60F93-88D4-4F60-A15A-4B2113E53BE2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{2A66B2A9-165C-4995-937F-8E0D8B01B3D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="123"/>
+    <tableColumn id="4" xr3:uid="{937ED0C3-8277-4EC6-BFD2-C6699696538D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="122"/>
+    <tableColumn id="5" xr3:uid="{37EAAABA-4FEF-4D28-B237-360AD0A7194A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="121"/>
+    <tableColumn id="6" xr3:uid="{6E7D50A0-6329-4797-9F9A-628D251C7CA5}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="120"/>
+    <tableColumn id="7" xr3:uid="{F8F31C01-9522-488B-915F-110987168D09}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="119"/>
+    <tableColumn id="8" xr3:uid="{FFD35FDD-AAE7-4F54-8AF3-197380BC0AEB}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5251,14 +5231,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}" name="Table004__Page_3" displayName="Table004__Page_3" ref="A18:H20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:H20" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A8A6FCCE-AE43-4EDA-82DC-831809E03401}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{0231594E-DA9E-47DE-A01C-22488210A4CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{7A06306A-69AF-482D-910F-86D0EF88F740}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="117"/>
-    <tableColumn id="4" xr3:uid="{E96F3603-E9D2-4710-BDE5-6FE3E6A378D8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="116"/>
-    <tableColumn id="5" xr3:uid="{37151140-CC9F-4EBB-B58D-F87E1081314A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="115"/>
-    <tableColumn id="6" xr3:uid="{F0AAEEC2-014D-412A-B58D-24C71FEC9A66}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="114"/>
-    <tableColumn id="7" xr3:uid="{A4B4F3F0-B14D-498F-B185-AA3E2BAE729A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="113"/>
-    <tableColumn id="8" xr3:uid="{0C517BB9-44A4-4BBA-AA88-B86BB679F208}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{A8A6FCCE-AE43-4EDA-82DC-831809E03401}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{0231594E-DA9E-47DE-A01C-22488210A4CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{7A06306A-69AF-482D-910F-86D0EF88F740}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{E96F3603-E9D2-4710-BDE5-6FE3E6A378D8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="114"/>
+    <tableColumn id="5" xr3:uid="{37151140-CC9F-4EBB-B58D-F87E1081314A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="113"/>
+    <tableColumn id="6" xr3:uid="{F0AAEEC2-014D-412A-B58D-24C71FEC9A66}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="112"/>
+    <tableColumn id="7" xr3:uid="{A4B4F3F0-B14D-498F-B185-AA3E2BAE729A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="111"/>
+    <tableColumn id="8" xr3:uid="{0C517BB9-44A4-4BBA-AA88-B86BB679F208}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5268,12 +5248,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}" name="Table005__Page_4" displayName="Table005__Page_4" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F16" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AB42FEA9-5A85-4A69-B46D-444C53C4B4EF}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{0D7919B1-FB5E-4192-8675-3D57B39D9AB0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{94F12F3D-88BF-4BEB-85E7-FF6313F6B88E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{2B04EEA3-DC55-4C69-860F-9571D35E352D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="108"/>
-    <tableColumn id="5" xr3:uid="{461C5084-182B-40CC-B479-24798E48D0F4}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="107"/>
-    <tableColumn id="6" xr3:uid="{258F7EB6-7345-43CA-BF8A-5E088D06FF8F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="106"/>
+    <tableColumn id="1" xr3:uid="{AB42FEA9-5A85-4A69-B46D-444C53C4B4EF}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{0D7919B1-FB5E-4192-8675-3D57B39D9AB0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="108"/>
+    <tableColumn id="3" xr3:uid="{94F12F3D-88BF-4BEB-85E7-FF6313F6B88E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="107"/>
+    <tableColumn id="4" xr3:uid="{2B04EEA3-DC55-4C69-860F-9571D35E352D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="106"/>
+    <tableColumn id="5" xr3:uid="{461C5084-182B-40CC-B479-24798E48D0F4}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="105"/>
+    <tableColumn id="6" xr3:uid="{258F7EB6-7345-43CA-BF8A-5E088D06FF8F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5283,12 +5263,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}" name="Table006__Page_4" displayName="Table006__Page_4" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:F20" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{55987721-40E8-4E11-9B6F-67EE503D78F4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{15260D47-39CC-4501-9656-F8DBE6AD3AB1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{06C8B30C-3DD3-49E6-8BE6-C8A9D39F2FC4}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{40A070F6-4BDB-49A7-9394-4D63F3A9E318}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{C5E0BAEF-796C-4C71-ACA7-889E63543C2D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{1BA75280-A961-41F1-B113-5935891BA00A}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="100"/>
+    <tableColumn id="1" xr3:uid="{55987721-40E8-4E11-9B6F-67EE503D78F4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{15260D47-39CC-4501-9656-F8DBE6AD3AB1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="102"/>
+    <tableColumn id="3" xr3:uid="{06C8B30C-3DD3-49E6-8BE6-C8A9D39F2FC4}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{40A070F6-4BDB-49A7-9394-4D63F3A9E318}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="100"/>
+    <tableColumn id="5" xr3:uid="{C5E0BAEF-796C-4C71-ACA7-889E63543C2D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{1BA75280-A961-41F1-B113-5935891BA00A}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5298,18 +5278,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}" name="Table007__Page_5" displayName="Table007__Page_5" ref="A1:L16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:L16" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9561388E-64AE-4A76-863E-A0B2091E2F9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{151810A9-7DD3-4FD0-91D6-6608DF85A8CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{94D629BF-F745-493D-8F74-FA7EEFDEAA84}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{AE87299A-170F-4661-BD08-B108394E2F7C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{708CB468-5E3F-4D0C-B6BD-C2C44C7191EC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{5D4BD3CB-C344-4155-B3C1-ECC49F86CED1}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{61DF1122-5C54-47A3-98F9-27CA1B50CA9D}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{130590EE-DDCB-43DB-A020-385B521DA018}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="92"/>
-    <tableColumn id="9" xr3:uid="{06B903F7-5E22-476D-A116-655599D2C518}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{CED96D55-8B0D-492D-B0EC-F3E56EFB2649}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="90"/>
-    <tableColumn id="11" xr3:uid="{346823E9-F305-4F11-941F-1C42A8AB0C99}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="89"/>
-    <tableColumn id="12" xr3:uid="{7B421AA8-C9DB-4E35-A456-DF0F56050B79}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{9561388E-64AE-4A76-863E-A0B2091E2F9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{151810A9-7DD3-4FD0-91D6-6608DF85A8CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="96"/>
+    <tableColumn id="3" xr3:uid="{94D629BF-F745-493D-8F74-FA7EEFDEAA84}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{AE87299A-170F-4661-BD08-B108394E2F7C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{708CB468-5E3F-4D0C-B6BD-C2C44C7191EC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="93"/>
+    <tableColumn id="6" xr3:uid="{5D4BD3CB-C344-4155-B3C1-ECC49F86CED1}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="92"/>
+    <tableColumn id="7" xr3:uid="{61DF1122-5C54-47A3-98F9-27CA1B50CA9D}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="91"/>
+    <tableColumn id="8" xr3:uid="{130590EE-DDCB-43DB-A020-385B521DA018}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="90"/>
+    <tableColumn id="9" xr3:uid="{06B903F7-5E22-476D-A116-655599D2C518}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="89"/>
+    <tableColumn id="10" xr3:uid="{CED96D55-8B0D-492D-B0EC-F3E56EFB2649}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="88"/>
+    <tableColumn id="11" xr3:uid="{346823E9-F305-4F11-941F-1C42A8AB0C99}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="87"/>
+    <tableColumn id="12" xr3:uid="{7B421AA8-C9DB-4E35-A456-DF0F56050B79}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5319,18 +5299,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}" name="Table008__Page_5" displayName="Table008__Page_5" ref="A18:L20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:L20" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{01D3C90B-BA67-46B4-BD1D-5C53486CAE57}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{166854EB-0B50-4420-BB3F-7A5A2C9FB7F7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{638857E5-1EB4-4FBE-9FFE-2951F2F4ABD0}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{F4EFE2EF-AC84-40F8-BE68-0B6B520F8EA8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{38D026D2-A47E-46EA-BA10-AF890A55BF2B}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="83"/>
-    <tableColumn id="6" xr3:uid="{025C6DA2-37A6-491F-904E-DDE12948D35B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{AC28B573-67B7-4468-A6A2-F648D17079B6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="81"/>
-    <tableColumn id="8" xr3:uid="{F6F06554-210B-472F-95F2-8E89D931E4C1}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{F0A8F323-36C1-4290-980B-8F6F5DC6A41E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="79"/>
-    <tableColumn id="10" xr3:uid="{25D60007-5007-4174-85F5-572E3C29FE33}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="78"/>
-    <tableColumn id="11" xr3:uid="{2071EB9B-B14E-4EF0-9B86-0D5FDA96828D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="77"/>
-    <tableColumn id="12" xr3:uid="{1660C180-EE6B-48E8-9880-55F02CC623C4}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{01D3C90B-BA67-46B4-BD1D-5C53486CAE57}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{166854EB-0B50-4420-BB3F-7A5A2C9FB7F7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{638857E5-1EB4-4FBE-9FFE-2951F2F4ABD0}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{F4EFE2EF-AC84-40F8-BE68-0B6B520F8EA8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{38D026D2-A47E-46EA-BA10-AF890A55BF2B}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="81"/>
+    <tableColumn id="6" xr3:uid="{025C6DA2-37A6-491F-904E-DDE12948D35B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{AC28B573-67B7-4468-A6A2-F648D17079B6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="79"/>
+    <tableColumn id="8" xr3:uid="{F6F06554-210B-472F-95F2-8E89D931E4C1}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="78"/>
+    <tableColumn id="9" xr3:uid="{F0A8F323-36C1-4290-980B-8F6F5DC6A41E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="77"/>
+    <tableColumn id="10" xr3:uid="{25D60007-5007-4174-85F5-572E3C29FE33}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="76"/>
+    <tableColumn id="11" xr3:uid="{2071EB9B-B14E-4EF0-9B86-0D5FDA96828D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="75"/>
+    <tableColumn id="12" xr3:uid="{1660C180-EE6B-48E8-9880-55F02CC623C4}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5636,8 +5616,8 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48:B51"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7049,7 +7029,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>597</v>
@@ -7081,10 +7061,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C45" s="9">
         <v>459000000</v>
@@ -7105,7 +7085,7 @@
         <v>259</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I45" s="12">
         <v>36400000</v>
@@ -7113,10 +7093,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C46" s="9">
         <v>449000000</v>
@@ -7137,7 +7117,7 @@
         <v>260</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I46" s="12">
         <v>32700000</v>
@@ -7145,10 +7125,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C47" s="18">
         <v>499000000</v>
@@ -7169,7 +7149,7 @@
         <v>261</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I47" s="19">
         <v>36400000</v>
@@ -7177,7 +7157,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>589</v>
@@ -7209,7 +7189,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>590</v>
@@ -7241,7 +7221,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>591</v>
@@ -7273,7 +7253,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>592</v>
@@ -7305,10 +7285,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A29 A31:A43">
-    <cfRule type="duplicateValues" dxfId="9" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A38 A2:A29 A40:A43">
-    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:H43">
     <cfRule type="duplicateValues" dxfId="5" priority="5"/>

</xml_diff>

<commit_message>
UPDATE: update RS and pricelist
</commit_message>
<xml_diff>
--- a/gp-app-1.0/Pricelist Car.xlsx
+++ b/gp-app-1.0/Pricelist Car.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\gp-app\gp-app-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0717B9-F5D3-42FC-B298-8BA4FE2D27B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8626274-3E33-48DC-967C-B4755BBB7B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="861" xr2:uid="{C4C7316A-D95F-426A-ADF9-AD32FA680374}"/>
   </bookViews>
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="614">
   <si>
     <t>Column1</t>
   </si>
@@ -2403,6 +2403,15 @@
   </si>
   <si>
     <t>Formo MB 1.2MT 5 Seat</t>
+  </si>
+  <si>
+    <t>NEW ALVEZ CE MT 310S I1F1 (4X2) M/T</t>
+  </si>
+  <si>
+    <t>New Alvez 1.5 CE 4X2 CVT</t>
+  </si>
+  <si>
+    <t>Cortez (NEW CORTEZ CE LUX+CVT) LT +CVT</t>
   </si>
 </sst>
 </file>
@@ -2594,7 +2603,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2629,7 +2638,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2727,6 +2745,402 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -3002,13 +3416,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -3018,6 +3425,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -3050,402 +3464,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5004,18 +5022,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I52" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
-  <autoFilter ref="A1:I52" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}" name="Table20" displayName="Table20" ref="A1:I54" totalsRowShown="0" headerRowDxfId="153" headerRowBorderDxfId="152" tableBorderDxfId="151" totalsRowBorderDxfId="150">
+  <autoFilter ref="A1:I54" xr:uid="{DF067A72-54A6-48F4-972D-2DE4603D61A4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I54">
+    <sortCondition ref="H1:H54"/>
+  </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0E6335F2-6B6A-436C-92FA-B48E61551308}" name="Merek/Type" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{5A4965DA-398A-4134-90BD-9CE4D8355880}" name="Tipe" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{010303D1-E0A2-4DE6-8E87-64ACC3102E09}" name="Harga OTR Awal" dataDxfId="15" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{91C798B0-7964-436A-84A5-7687993F376F}" name="Dealer Margin" dataDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{CD936623-36F3-4BAA-A615-AF79A61C51E8}" name="Dealer Margin 9 %" dataDxfId="13" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{A36173E8-D9B2-4F38-A572-F5D32CDADEB8}" name="Dealer Margin 7 %" dataDxfId="12" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{7A11B7F5-7683-492A-A8B5-D96984323DDD}" name="Code Unit" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{AF243BB3-2044-4D1E-9F0D-A1EC0D2C15CF}" name="Merk/Type" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{9E0E2E6A-108F-4ACE-959D-9EB0F753BD73}" name="Full Margin" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{0E6335F2-6B6A-436C-92FA-B48E61551308}" name="Merek/Type" dataDxfId="149"/>
+    <tableColumn id="2" xr3:uid="{5A4965DA-398A-4134-90BD-9CE4D8355880}" name="Tipe" dataDxfId="148"/>
+    <tableColumn id="3" xr3:uid="{010303D1-E0A2-4DE6-8E87-64ACC3102E09}" name="Harga OTR Awal" dataDxfId="147" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{91C798B0-7964-436A-84A5-7687993F376F}" name="Dealer Margin" dataDxfId="146" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{CD936623-36F3-4BAA-A615-AF79A61C51E8}" name="Dealer Margin 9 %" dataDxfId="145" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{A36173E8-D9B2-4F38-A572-F5D32CDADEB8}" name="Dealer Margin 7 %" dataDxfId="144" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{7A11B7F5-7683-492A-A8B5-D96984323DDD}" name="Code Unit" dataDxfId="143"/>
+    <tableColumn id="8" xr3:uid="{AF243BB3-2044-4D1E-9F0D-A1EC0D2C15CF}" name="Merk/Type" dataDxfId="142"/>
+    <tableColumn id="9" xr3:uid="{9E0E2E6A-108F-4ACE-959D-9EB0F753BD73}" name="Full Margin" dataDxfId="141"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5025,15 +5046,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}" name="Table009__Page_6" displayName="Table009__Page_6" ref="A1:I16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I16" xr:uid="{630D8221-A5B4-4162-BEFC-7BB63825B861}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5980B244-73E4-43AF-B863-305E8B039C33}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{549208EE-7E07-4F0F-ACFD-9606CC8F6B50}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{086F7B88-A201-47FD-B9A0-0C976108E144}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{CC912184-CE02-4DC9-8815-71C4295C86DF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{8F3F2202-7C07-4D43-B483-871C9E242208}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="83"/>
-    <tableColumn id="6" xr3:uid="{6D2190D6-B434-4BB9-95B1-A29148C453AF}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{A33DE0AF-7DA7-4623-87E7-DBA2BF4E404A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="81"/>
-    <tableColumn id="8" xr3:uid="{CD689B59-BA44-4F67-9FF9-E08337BE66FD}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{744F224A-BA1E-4758-B291-8D5C8D341610}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{5980B244-73E4-43AF-B863-305E8B039C33}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{549208EE-7E07-4F0F-ACFD-9606CC8F6B50}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{086F7B88-A201-47FD-B9A0-0C976108E144}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{CC912184-CE02-4DC9-8815-71C4295C86DF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{8F3F2202-7C07-4D43-B483-871C9E242208}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="70"/>
+    <tableColumn id="6" xr3:uid="{6D2190D6-B434-4BB9-95B1-A29148C453AF}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="69"/>
+    <tableColumn id="7" xr3:uid="{A33DE0AF-7DA7-4623-87E7-DBA2BF4E404A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="68"/>
+    <tableColumn id="8" xr3:uid="{CD689B59-BA44-4F67-9FF9-E08337BE66FD}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="67"/>
+    <tableColumn id="9" xr3:uid="{744F224A-BA1E-4758-B291-8D5C8D341610}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5043,15 +5064,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}" name="Table010__Page_6" displayName="Table010__Page_6" ref="A18:I20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:I20" xr:uid="{116BBD7B-F856-4C44-8F1F-EA66756E3A0B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D02866AC-7C8C-4041-B0D6-297717EA2BCA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{F9BA0334-AC0F-4599-91DD-1D3B53530BA2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{2E40CB08-FF90-4211-A5F6-3255AA5CEAED}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{951E49DE-3DB8-41C0-8F36-6E5A1649659D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{D7FC7D23-AA29-4FAE-8DF4-B23A11020D8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{85DA6C7C-BC56-4316-BB56-3D2CA86DF4B0}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{47F39228-8CCC-4319-9964-568280350AF4}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{781188CD-5AC0-41B9-8575-2EACD4BA90A4}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{A2DFBEC8-960F-4613-A8B8-821CF42818AC}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{D02866AC-7C8C-4041-B0D6-297717EA2BCA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{F9BA0334-AC0F-4599-91DD-1D3B53530BA2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{2E40CB08-FF90-4211-A5F6-3255AA5CEAED}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{951E49DE-3DB8-41C0-8F36-6E5A1649659D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{D7FC7D23-AA29-4FAE-8DF4-B23A11020D8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{85DA6C7C-BC56-4316-BB56-3D2CA86DF4B0}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{47F39228-8CCC-4319-9964-568280350AF4}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{781188CD-5AC0-41B9-8575-2EACD4BA90A4}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{A2DFBEC8-960F-4613-A8B8-821CF42818AC}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5061,9 +5082,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}" name="Table011__Page_7" displayName="Table011__Page_7" ref="A1:C15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C15" xr:uid="{D5A80464-2F5E-4F81-BC09-642A89962C82}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{384F6B08-E7B1-4ECD-BC7E-1F8C8FC9CD11}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{BD116665-54B3-487B-82AD-7E260403FB1A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{A0C72322-3C63-446F-A7B0-E45538411191}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{384F6B08-E7B1-4ECD-BC7E-1F8C8FC9CD11}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{BD116665-54B3-487B-82AD-7E260403FB1A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{A0C72322-3C63-446F-A7B0-E45538411191}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5073,9 +5094,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}" name="Table012__Page_7" displayName="Table012__Page_7" ref="A17:C19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A17:C19" xr:uid="{BF5A7D5F-42BD-4927-9517-2459449E72C6}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{92B56AD9-FE6F-4702-B777-811CB1B6E64F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{C37743D7-7886-43A1-BB26-C0F3914426C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{DFF6BFBF-623A-4318-86AF-C5448FC821A5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{92B56AD9-FE6F-4702-B777-811CB1B6E64F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{C37743D7-7886-43A1-BB26-C0F3914426C9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{DFF6BFBF-623A-4318-86AF-C5448FC821A5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5085,11 +5106,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}" name="Table013__Page_8" displayName="Table013__Page_8" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E16" xr:uid="{4DAA9679-BE71-4F3A-B608-132984AF6DF1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{811DEB23-A3B8-4E1E-AF98-CBD4FE9515C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{D1233A63-9D37-45F3-9DC7-52977AC06ADC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{400191B1-4CF8-4D78-82E7-FED7CD6730E6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{3D829CC4-4292-4CD0-80B8-3490D4014AC9}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{9BC50CF1-EF44-42B4-9129-E887F74428C9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{811DEB23-A3B8-4E1E-AF98-CBD4FE9515C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{D1233A63-9D37-45F3-9DC7-52977AC06ADC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{400191B1-4CF8-4D78-82E7-FED7CD6730E6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{3D829CC4-4292-4CD0-80B8-3490D4014AC9}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{9BC50CF1-EF44-42B4-9129-E887F74428C9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5099,11 +5120,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}" name="Table014__Page_8" displayName="Table014__Page_8" ref="A18:E21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:E21" xr:uid="{9D3195A8-F1BD-4429-B95A-60FCF241B775}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{98A6121C-2EC1-48CA-8A40-28DAFD66423E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{6B521FB3-E639-4556-B8C5-473A63201BC1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{3D07F9E9-4DA3-41C6-98A7-BC28F0C8BFB5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{89F1E0D5-9B1D-4170-BB1D-3FBA7855FC27}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{68E29A0D-4E20-4E2A-A030-157EF3C69E97}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{98A6121C-2EC1-48CA-8A40-28DAFD66423E}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{6B521FB3-E639-4556-B8C5-473A63201BC1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{3D07F9E9-4DA3-41C6-98A7-BC28F0C8BFB5}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{89F1E0D5-9B1D-4170-BB1D-3FBA7855FC27}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{68E29A0D-4E20-4E2A-A030-157EF3C69E97}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5113,12 +5134,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}" name="Table015__Page_9" displayName="Table015__Page_9" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F16" xr:uid="{F2B12C92-B774-477F-98C9-509526BBDEE5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B9D47F1B-922B-4B02-855C-93AF62167342}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{9915D8BD-1C99-4D36-BE7E-9EBEAD6D7B12}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{D353D58B-6A1D-4079-A9EC-77376B67A375}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{ACF53426-7425-4D38-9673-B3197A3F9292}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{673A9374-D6DA-46D7-AAD2-6F2220F4ED8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{37C428F9-0692-44D1-B8CF-2CBC7901020B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{B9D47F1B-922B-4B02-855C-93AF62167342}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{9915D8BD-1C99-4D36-BE7E-9EBEAD6D7B12}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{D353D58B-6A1D-4079-A9EC-77376B67A375}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{ACF53426-7425-4D38-9673-B3197A3F9292}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{673A9374-D6DA-46D7-AAD2-6F2220F4ED8C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{37C428F9-0692-44D1-B8CF-2CBC7901020B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5128,12 +5149,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}" name="Table016__Page_9" displayName="Table016__Page_9" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:F20" xr:uid="{3C596C1A-3A31-47DF-B534-2A3593167FFF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{48EBD4D1-26EB-449F-8D09-DF1A8D9D96A3}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{671AE648-452F-44F1-9A65-8468F7B19950}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{C3287937-E8A8-4D80-A27C-D2A5C0E44D68}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{49CAB777-0355-40CC-9F2D-C41408ED9E98}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{A19C49CB-F2CF-4D60-B082-761FE4F0ABC5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{801427E9-2562-451E-AE45-ACF6DAAAFFFB}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{48EBD4D1-26EB-449F-8D09-DF1A8D9D96A3}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{671AE648-452F-44F1-9A65-8468F7B19950}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{C3287937-E8A8-4D80-A27C-D2A5C0E44D68}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{49CAB777-0355-40CC-9F2D-C41408ED9E98}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{A19C49CB-F2CF-4D60-B082-761FE4F0ABC5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{801427E9-2562-451E-AE45-ACF6DAAAFFFB}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5143,11 +5164,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}" name="Table017__Page_10" displayName="Table017__Page_10" ref="A1:E15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E15" xr:uid="{510F87AB-8378-4FE2-9EBF-7361BA7DB6B8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{626476ED-551C-48ED-A0F5-9CB680097EF0}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{9215A7DD-9718-48E5-BA20-B6B9989DD0D2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{AE2AC56F-3587-4342-A60B-0B4A30905DD3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{F7BE237D-2C3F-4C27-92EF-2601ABCBA887}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{7950C4F9-8FA4-4C6E-B03A-A0235ECC51FF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{626476ED-551C-48ED-A0F5-9CB680097EF0}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{9215A7DD-9718-48E5-BA20-B6B9989DD0D2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{AE2AC56F-3587-4342-A60B-0B4A30905DD3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{F7BE237D-2C3F-4C27-92EF-2601ABCBA887}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{7950C4F9-8FA4-4C6E-B03A-A0235ECC51FF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5157,11 +5178,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}" name="Table018__Page_10" displayName="Table018__Page_10" ref="A17:E19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A17:E19" xr:uid="{14CF879A-74C7-4F0C-8E76-F1430C9579CD}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{210B1486-2DC9-4D94-98AC-6BEB874B7545}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{BB67F395-3AAE-4514-BCCE-DE32693EB37D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{230B22CA-5CA3-4E2D-92CC-C75BC5831FF2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{42788CA6-A70D-442A-9072-79E0D19F0B28}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{E37C1038-7442-4E7D-BB43-162AD6FA4195}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{210B1486-2DC9-4D94-98AC-6BEB874B7545}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{BB67F395-3AAE-4514-BCCE-DE32693EB37D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{230B22CA-5CA3-4E2D-92CC-C75BC5831FF2}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{42788CA6-A70D-442A-9072-79E0D19F0B28}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{E37C1038-7442-4E7D-BB43-162AD6FA4195}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5171,13 +5192,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}" name="Table001__Page_2" displayName="Table001__Page_2" ref="A1:G16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G16" xr:uid="{8D8C9D73-217D-4974-B35A-0740746DA27F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A26CE965-72B2-472B-B9FF-D68F7847F3C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="153"/>
-    <tableColumn id="2" xr3:uid="{375BF78E-5806-424A-B7BD-C63C40843BE9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="152"/>
-    <tableColumn id="3" xr3:uid="{CD1FFC74-B097-42B5-B1FA-08D3BD4531B9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="151"/>
-    <tableColumn id="4" xr3:uid="{EA6F5C08-47B3-4BE3-8F9B-3167F2B34338}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="150"/>
-    <tableColumn id="5" xr3:uid="{67D1B145-6151-4A54-9C79-A6B0381CDA09}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="149"/>
-    <tableColumn id="6" xr3:uid="{E8D8899E-ED32-4A2F-B13D-18F4C289A59B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="148"/>
-    <tableColumn id="7" xr3:uid="{CD1BCBB0-10DE-4DDA-903D-C14D16829749}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="147"/>
+    <tableColumn id="1" xr3:uid="{A26CE965-72B2-472B-B9FF-D68F7847F3C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="140"/>
+    <tableColumn id="2" xr3:uid="{375BF78E-5806-424A-B7BD-C63C40843BE9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="139"/>
+    <tableColumn id="3" xr3:uid="{CD1FFC74-B097-42B5-B1FA-08D3BD4531B9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{EA6F5C08-47B3-4BE3-8F9B-3167F2B34338}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="137"/>
+    <tableColumn id="5" xr3:uid="{67D1B145-6151-4A54-9C79-A6B0381CDA09}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="136"/>
+    <tableColumn id="6" xr3:uid="{E8D8899E-ED32-4A2F-B13D-18F4C289A59B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="135"/>
+    <tableColumn id="7" xr3:uid="{CD1BCBB0-10DE-4DDA-903D-C14D16829749}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5187,11 +5208,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}" name="Table019__Page_11" displayName="Table019__Page_11" ref="A1:E16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E16" xr:uid="{A8D65B7F-C1B3-4E37-BFF7-03252131F371}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{60EAA1C9-E43C-458C-A33C-365CF023541D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{BF4ECEAF-8998-4833-A444-7DD2840947AB}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{A77E13C5-CB25-43C0-9678-51A378FA64FC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{46713ABC-AA6E-45DD-9BBE-03C863D6B1D1}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{85365AB6-280F-40C4-AB42-3455547D61F1}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{60EAA1C9-E43C-458C-A33C-365CF023541D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{BF4ECEAF-8998-4833-A444-7DD2840947AB}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{A77E13C5-CB25-43C0-9678-51A378FA64FC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{46713ABC-AA6E-45DD-9BBE-03C863D6B1D1}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{85365AB6-280F-40C4-AB42-3455547D61F1}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5201,11 +5222,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0B4290D5-7CEE-4DDC-B997-690EEF6D9589}" name="Table020__Page_11" displayName="Table020__Page_11" ref="A18:E20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:E20" xr:uid="{0B4290D5-7CEE-4DDC-B997-690EEF6D9589}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{344C3D84-8C5A-4C60-ADD3-4EE73F83858B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{3470DF86-5A38-429A-95CF-F5FF5E59449C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{BC1BD851-46F6-4634-95EE-ED117E75EBB6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{FF5D3D34-BBDB-4113-8340-C737255ED1BD}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{F05FA152-C9D6-4773-B0A5-5B18B60C7102}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{344C3D84-8C5A-4C60-ADD3-4EE73F83858B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{3470DF86-5A38-429A-95CF-F5FF5E59449C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{BC1BD851-46F6-4634-95EE-ED117E75EBB6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{FF5D3D34-BBDB-4113-8340-C737255ED1BD}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{F05FA152-C9D6-4773-B0A5-5B18B60C7102}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5215,13 +5236,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}" name="Table002__Page_2" displayName="Table002__Page_2" ref="A19:G21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A19:G21" xr:uid="{D4474760-F3B7-4070-AE77-2962D090A5AB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8A3681DA-5FE9-4564-BCAB-75CCDF2C3A51}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="146"/>
-    <tableColumn id="2" xr3:uid="{44D6563C-A88C-4FEE-9427-B5252DF8FA5D}" uniqueName="2" name="Column6" queryTableFieldId="2" dataDxfId="145"/>
-    <tableColumn id="3" xr3:uid="{2514D758-49E4-4E3E-A628-2B2D894F398E}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="144"/>
-    <tableColumn id="4" xr3:uid="{062470EA-CB73-435C-8DF3-28DE262C8D69}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="143"/>
-    <tableColumn id="5" xr3:uid="{CDE500EE-B268-43D9-A30D-9E6CC1608CD0}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="142"/>
-    <tableColumn id="6" xr3:uid="{699F51E2-9A1B-4953-91BE-8D6434D76B20}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="141"/>
-    <tableColumn id="7" xr3:uid="{C62D0670-E212-49FF-BA61-22C41F21B60E}" uniqueName="7" name="Column62" queryTableFieldId="7" dataDxfId="140"/>
+    <tableColumn id="1" xr3:uid="{8A3681DA-5FE9-4564-BCAB-75CCDF2C3A51}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="133"/>
+    <tableColumn id="2" xr3:uid="{44D6563C-A88C-4FEE-9427-B5252DF8FA5D}" uniqueName="2" name="Column6" queryTableFieldId="2" dataDxfId="132"/>
+    <tableColumn id="3" xr3:uid="{2514D758-49E4-4E3E-A628-2B2D894F398E}" uniqueName="3" name="Column2" queryTableFieldId="3" dataDxfId="131"/>
+    <tableColumn id="4" xr3:uid="{062470EA-CB73-435C-8DF3-28DE262C8D69}" uniqueName="4" name="Column3" queryTableFieldId="4" dataDxfId="130"/>
+    <tableColumn id="5" xr3:uid="{CDE500EE-B268-43D9-A30D-9E6CC1608CD0}" uniqueName="5" name="Column4" queryTableFieldId="5" dataDxfId="129"/>
+    <tableColumn id="6" xr3:uid="{699F51E2-9A1B-4953-91BE-8D6434D76B20}" uniqueName="6" name="Column5" queryTableFieldId="6" dataDxfId="128"/>
+    <tableColumn id="7" xr3:uid="{C62D0670-E212-49FF-BA61-22C41F21B60E}" uniqueName="7" name="Column62" queryTableFieldId="7" dataDxfId="127"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5231,14 +5252,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}" name="Table003__Page_3" displayName="Table003__Page_3" ref="A1:H16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H16" xr:uid="{EE92A61D-8549-4453-B707-7BA76D39611E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5E78ED26-3040-4033-A95F-3AC09118D17C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="139"/>
-    <tableColumn id="2" xr3:uid="{52F60F93-88D4-4F60-A15A-4B2113E53BE2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="138"/>
-    <tableColumn id="3" xr3:uid="{2A66B2A9-165C-4995-937F-8E0D8B01B3D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="137"/>
-    <tableColumn id="4" xr3:uid="{937ED0C3-8277-4EC6-BFD2-C6699696538D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="136"/>
-    <tableColumn id="5" xr3:uid="{37EAAABA-4FEF-4D28-B237-360AD0A7194A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="135"/>
-    <tableColumn id="6" xr3:uid="{6E7D50A0-6329-4797-9F9A-628D251C7CA5}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="134"/>
-    <tableColumn id="7" xr3:uid="{F8F31C01-9522-488B-915F-110987168D09}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="133"/>
-    <tableColumn id="8" xr3:uid="{FFD35FDD-AAE7-4F54-8AF3-197380BC0AEB}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="132"/>
+    <tableColumn id="1" xr3:uid="{5E78ED26-3040-4033-A95F-3AC09118D17C}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{52F60F93-88D4-4F60-A15A-4B2113E53BE2}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{2A66B2A9-165C-4995-937F-8E0D8B01B3D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{937ED0C3-8277-4EC6-BFD2-C6699696538D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{37EAAABA-4FEF-4D28-B237-360AD0A7194A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="122"/>
+    <tableColumn id="6" xr3:uid="{6E7D50A0-6329-4797-9F9A-628D251C7CA5}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="121"/>
+    <tableColumn id="7" xr3:uid="{F8F31C01-9522-488B-915F-110987168D09}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="120"/>
+    <tableColumn id="8" xr3:uid="{FFD35FDD-AAE7-4F54-8AF3-197380BC0AEB}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5248,14 +5269,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}" name="Table004__Page_3" displayName="Table004__Page_3" ref="A18:H20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:H20" xr:uid="{1C7E55B7-7D73-418F-9229-407F52A253A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A8A6FCCE-AE43-4EDA-82DC-831809E03401}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="131"/>
-    <tableColumn id="2" xr3:uid="{0231594E-DA9E-47DE-A01C-22488210A4CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="130"/>
-    <tableColumn id="3" xr3:uid="{7A06306A-69AF-482D-910F-86D0EF88F740}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="129"/>
-    <tableColumn id="4" xr3:uid="{E96F3603-E9D2-4710-BDE5-6FE3E6A378D8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="128"/>
-    <tableColumn id="5" xr3:uid="{37151140-CC9F-4EBB-B58D-F87E1081314A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="127"/>
-    <tableColumn id="6" xr3:uid="{F0AAEEC2-014D-412A-B58D-24C71FEC9A66}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="126"/>
-    <tableColumn id="7" xr3:uid="{A4B4F3F0-B14D-498F-B185-AA3E2BAE729A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="125"/>
-    <tableColumn id="8" xr3:uid="{0C517BB9-44A4-4BBA-AA88-B86BB679F208}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{A8A6FCCE-AE43-4EDA-82DC-831809E03401}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="118"/>
+    <tableColumn id="2" xr3:uid="{0231594E-DA9E-47DE-A01C-22488210A4CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="117"/>
+    <tableColumn id="3" xr3:uid="{7A06306A-69AF-482D-910F-86D0EF88F740}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="116"/>
+    <tableColumn id="4" xr3:uid="{E96F3603-E9D2-4710-BDE5-6FE3E6A378D8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="115"/>
+    <tableColumn id="5" xr3:uid="{37151140-CC9F-4EBB-B58D-F87E1081314A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="114"/>
+    <tableColumn id="6" xr3:uid="{F0AAEEC2-014D-412A-B58D-24C71FEC9A66}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="113"/>
+    <tableColumn id="7" xr3:uid="{A4B4F3F0-B14D-498F-B185-AA3E2BAE729A}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="112"/>
+    <tableColumn id="8" xr3:uid="{0C517BB9-44A4-4BBA-AA88-B86BB679F208}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5265,12 +5286,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}" name="Table005__Page_4" displayName="Table005__Page_4" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F16" xr:uid="{2EB30D60-3074-4922-8217-6B97953C0F87}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AB42FEA9-5A85-4A69-B46D-444C53C4B4EF}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{0D7919B1-FB5E-4192-8675-3D57B39D9AB0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{94F12F3D-88BF-4BEB-85E7-FF6313F6B88E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{2B04EEA3-DC55-4C69-860F-9571D35E352D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="120"/>
-    <tableColumn id="5" xr3:uid="{461C5084-182B-40CC-B479-24798E48D0F4}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="119"/>
-    <tableColumn id="6" xr3:uid="{258F7EB6-7345-43CA-BF8A-5E088D06FF8F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{AB42FEA9-5A85-4A69-B46D-444C53C4B4EF}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{0D7919B1-FB5E-4192-8675-3D57B39D9AB0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{94F12F3D-88BF-4BEB-85E7-FF6313F6B88E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="108"/>
+    <tableColumn id="4" xr3:uid="{2B04EEA3-DC55-4C69-860F-9571D35E352D}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="107"/>
+    <tableColumn id="5" xr3:uid="{461C5084-182B-40CC-B479-24798E48D0F4}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="106"/>
+    <tableColumn id="6" xr3:uid="{258F7EB6-7345-43CA-BF8A-5E088D06FF8F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5280,12 +5301,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}" name="Table006__Page_4" displayName="Table006__Page_4" ref="A18:F20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:F20" xr:uid="{BA3E356C-A98F-4646-B7E8-7B0C3904E2A4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{55987721-40E8-4E11-9B6F-67EE503D78F4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="117"/>
-    <tableColumn id="2" xr3:uid="{15260D47-39CC-4501-9656-F8DBE6AD3AB1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="116"/>
-    <tableColumn id="3" xr3:uid="{06C8B30C-3DD3-49E6-8BE6-C8A9D39F2FC4}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="115"/>
-    <tableColumn id="4" xr3:uid="{40A070F6-4BDB-49A7-9394-4D63F3A9E318}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="114"/>
-    <tableColumn id="5" xr3:uid="{C5E0BAEF-796C-4C71-ACA7-889E63543C2D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="113"/>
-    <tableColumn id="6" xr3:uid="{1BA75280-A961-41F1-B113-5935891BA00A}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{55987721-40E8-4E11-9B6F-67EE503D78F4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{15260D47-39CC-4501-9656-F8DBE6AD3AB1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{06C8B30C-3DD3-49E6-8BE6-C8A9D39F2FC4}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{40A070F6-4BDB-49A7-9394-4D63F3A9E318}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{C5E0BAEF-796C-4C71-ACA7-889E63543C2D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{1BA75280-A961-41F1-B113-5935891BA00A}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5295,18 +5316,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}" name="Table007__Page_5" displayName="Table007__Page_5" ref="A1:L16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:L16" xr:uid="{6040FF08-DFFC-4D6C-87C0-7C33D5281777}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9561388E-64AE-4A76-863E-A0B2091E2F9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{151810A9-7DD3-4FD0-91D6-6608DF85A8CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{94D629BF-F745-493D-8F74-FA7EEFDEAA84}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{AE87299A-170F-4661-BD08-B108394E2F7C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="108"/>
-    <tableColumn id="5" xr3:uid="{708CB468-5E3F-4D0C-B6BD-C2C44C7191EC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="107"/>
-    <tableColumn id="6" xr3:uid="{5D4BD3CB-C344-4155-B3C1-ECC49F86CED1}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="106"/>
-    <tableColumn id="7" xr3:uid="{61DF1122-5C54-47A3-98F9-27CA1B50CA9D}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="105"/>
-    <tableColumn id="8" xr3:uid="{130590EE-DDCB-43DB-A020-385B521DA018}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="104"/>
-    <tableColumn id="9" xr3:uid="{06B903F7-5E22-476D-A116-655599D2C518}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="103"/>
-    <tableColumn id="10" xr3:uid="{CED96D55-8B0D-492D-B0EC-F3E56EFB2649}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="102"/>
-    <tableColumn id="11" xr3:uid="{346823E9-F305-4F11-941F-1C42A8AB0C99}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="101"/>
-    <tableColumn id="12" xr3:uid="{7B421AA8-C9DB-4E35-A456-DF0F56050B79}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="100"/>
+    <tableColumn id="1" xr3:uid="{9561388E-64AE-4A76-863E-A0B2091E2F9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="98"/>
+    <tableColumn id="2" xr3:uid="{151810A9-7DD3-4FD0-91D6-6608DF85A8CF}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{94D629BF-F745-493D-8F74-FA7EEFDEAA84}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="96"/>
+    <tableColumn id="4" xr3:uid="{AE87299A-170F-4661-BD08-B108394E2F7C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="95"/>
+    <tableColumn id="5" xr3:uid="{708CB468-5E3F-4D0C-B6BD-C2C44C7191EC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{5D4BD3CB-C344-4155-B3C1-ECC49F86CED1}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="93"/>
+    <tableColumn id="7" xr3:uid="{61DF1122-5C54-47A3-98F9-27CA1B50CA9D}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{130590EE-DDCB-43DB-A020-385B521DA018}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="91"/>
+    <tableColumn id="9" xr3:uid="{06B903F7-5E22-476D-A116-655599D2C518}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="90"/>
+    <tableColumn id="10" xr3:uid="{CED96D55-8B0D-492D-B0EC-F3E56EFB2649}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{346823E9-F305-4F11-941F-1C42A8AB0C99}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{7B421AA8-C9DB-4E35-A456-DF0F56050B79}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5316,18 +5337,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}" name="Table008__Page_5" displayName="Table008__Page_5" ref="A18:L20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A18:L20" xr:uid="{DBF54861-4823-4965-9BF8-BF4D83A85FD1}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{01D3C90B-BA67-46B4-BD1D-5C53486CAE57}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{166854EB-0B50-4420-BB3F-7A5A2C9FB7F7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{638857E5-1EB4-4FBE-9FFE-2951F2F4ABD0}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{F4EFE2EF-AC84-40F8-BE68-0B6B520F8EA8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{38D026D2-A47E-46EA-BA10-AF890A55BF2B}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{025C6DA2-37A6-491F-904E-DDE12948D35B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{AC28B573-67B7-4468-A6A2-F648D17079B6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{F6F06554-210B-472F-95F2-8E89D931E4C1}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="92"/>
-    <tableColumn id="9" xr3:uid="{F0A8F323-36C1-4290-980B-8F6F5DC6A41E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{25D60007-5007-4174-85F5-572E3C29FE33}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="90"/>
-    <tableColumn id="11" xr3:uid="{2071EB9B-B14E-4EF0-9B86-0D5FDA96828D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="89"/>
-    <tableColumn id="12" xr3:uid="{1660C180-EE6B-48E8-9880-55F02CC623C4}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{01D3C90B-BA67-46B4-BD1D-5C53486CAE57}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{166854EB-0B50-4420-BB3F-7A5A2C9FB7F7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{638857E5-1EB4-4FBE-9FFE-2951F2F4ABD0}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{F4EFE2EF-AC84-40F8-BE68-0B6B520F8EA8}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="83"/>
+    <tableColumn id="5" xr3:uid="{38D026D2-A47E-46EA-BA10-AF890A55BF2B}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{025C6DA2-37A6-491F-904E-DDE12948D35B}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="81"/>
+    <tableColumn id="7" xr3:uid="{AC28B573-67B7-4468-A6A2-F648D17079B6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="80"/>
+    <tableColumn id="8" xr3:uid="{F6F06554-210B-472F-95F2-8E89D931E4C1}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="79"/>
+    <tableColumn id="9" xr3:uid="{F0A8F323-36C1-4290-980B-8F6F5DC6A41E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="78"/>
+    <tableColumn id="10" xr3:uid="{25D60007-5007-4174-85F5-572E3C29FE33}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="77"/>
+    <tableColumn id="11" xr3:uid="{2071EB9B-B14E-4EF0-9B86-0D5FDA96828D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="76"/>
+    <tableColumn id="12" xr3:uid="{1660C180-EE6B-48E8-9880-55F02CC623C4}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5630,11 +5651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05C9E0-A64E-40AC-B9F4-C919ED5906CC}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53:XFD53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5702,1474 +5723,1474 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>514</v>
+        <v>580</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>541</v>
+        <v>507</v>
       </c>
       <c r="C2" s="5">
-        <v>447200000</v>
+        <v>214000000</v>
       </c>
       <c r="D2" s="5">
         <f>I2/1.12</f>
-        <v>31249999.999999996</v>
+        <v>18750000</v>
       </c>
       <c r="E2" s="5">
         <f>D2*90%</f>
-        <v>28124999.999999996</v>
+        <v>16875000</v>
       </c>
       <c r="F2" s="5">
         <f>D2*70%</f>
-        <v>21874999.999999996</v>
-      </c>
-      <c r="G2" s="7">
-        <v>228</v>
+        <v>13125000</v>
+      </c>
+      <c r="G2" s="3">
+        <v>221</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>565</v>
+        <v>574</v>
       </c>
       <c r="I2" s="12">
-        <v>35000000</v>
+        <v>21000000.000000004</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>548</v>
+        <v>507</v>
       </c>
       <c r="C3" s="5">
-        <v>388500000</v>
+        <v>251000000</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D42" si="0">I3/1.12</f>
-        <v>29464285.714285709</v>
+        <f>I3/1.12</f>
+        <v>18750000</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E29" si="1">D3*90%</f>
-        <v>26517857.142857138</v>
+        <f>D3*90%</f>
+        <v>16875000</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F29" si="2">D3*70%</f>
-        <v>20624999.999999996</v>
-      </c>
-      <c r="G3" s="7">
-        <v>227</v>
+        <f>D3*70%</f>
+        <v>13125000</v>
+      </c>
+      <c r="G3" s="3">
+        <v>221</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>565</v>
+        <v>574</v>
       </c>
       <c r="I3" s="12">
-        <v>32999999.999999996</v>
+        <v>21000000.000000004</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>542</v>
+        <v>556</v>
       </c>
       <c r="C4" s="5">
-        <v>311500000</v>
+        <v>251000000</v>
       </c>
       <c r="D4" s="5">
-        <f t="shared" si="0"/>
-        <v>20758928.571428567</v>
+        <f>I4/1.12</f>
+        <v>18750000</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="1"/>
-        <v>18683035.714285713</v>
+        <f>D4*90%</f>
+        <v>16875000</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" si="2"/>
-        <v>14531249.999999996</v>
-      </c>
-      <c r="G4" s="7">
-        <v>222</v>
+        <f>D4*70%</f>
+        <v>13125000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>243</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>565</v>
+        <v>574</v>
       </c>
       <c r="I4" s="12">
-        <v>23249999.999999996</v>
+        <v>21000000.000000004</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>543</v>
+        <v>508</v>
       </c>
       <c r="C5" s="5">
-        <v>329050000</v>
+        <v>251000000</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" si="0"/>
-        <v>22053571.428571429</v>
+        <f>I5/1.12</f>
+        <v>18750000</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="1"/>
-        <v>19848214.285714287</v>
+        <f>D5*90%</f>
+        <v>16875000</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" si="2"/>
-        <v>15437500</v>
-      </c>
-      <c r="G5" s="7">
-        <v>223</v>
+        <f>D5*70%</f>
+        <v>13125000</v>
+      </c>
+      <c r="G5" s="3">
+        <v>250</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="I5" s="12">
-        <v>24700000.000000004</v>
+        <v>21000000.000000004</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>530</v>
+        <v>509</v>
       </c>
       <c r="C6" s="5">
-        <v>405000000</v>
+        <v>307500000</v>
       </c>
       <c r="D6" s="5">
-        <f t="shared" si="0"/>
-        <v>31249999.999999996</v>
+        <f>I6/1.12</f>
+        <v>22321428.571428567</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="1"/>
-        <v>28124999.999999996</v>
+        <f>D6*90%</f>
+        <v>20089285.714285713</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="2"/>
-        <v>21874999.999999996</v>
-      </c>
-      <c r="G6" s="7">
-        <v>244</v>
+        <f>D6*70%</f>
+        <v>15624999.999999996</v>
+      </c>
+      <c r="G6" s="3">
+        <v>235</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="I6" s="12">
-        <v>35000000</v>
+        <v>24999999.999999996</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>497</v>
+        <v>515</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>531</v>
+        <v>542</v>
       </c>
       <c r="C7" s="5">
-        <v>442000000</v>
+        <v>311500000</v>
       </c>
       <c r="D7" s="5">
-        <f t="shared" si="0"/>
-        <v>33928571.428571425</v>
+        <f>I7/1.12</f>
+        <v>20758928.571428567</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="1"/>
-        <v>30535714.285714284</v>
+        <f>D7*90%</f>
+        <v>18683035.714285713</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="2"/>
-        <v>23749999.999999996</v>
+        <f>D7*70%</f>
+        <v>14531249.999999996</v>
       </c>
       <c r="G7" s="7">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>565</v>
       </c>
       <c r="I7" s="12">
-        <v>38000000</v>
+        <v>23249999.999999996</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="C8" s="5">
-        <v>303000000</v>
+        <v>329050000</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" si="0"/>
-        <v>20535714.285714284</v>
+        <f>I8/1.12</f>
+        <v>22053571.428571429</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="1"/>
-        <v>18482142.857142854</v>
+        <f>D8*90%</f>
+        <v>19848214.285714287</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="2"/>
-        <v>14374999.999999998</v>
-      </c>
-      <c r="G8" s="3">
-        <v>240</v>
+        <f>D8*70%</f>
+        <v>15437500</v>
+      </c>
+      <c r="G8" s="7">
+        <v>223</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I8" s="12">
-        <v>23000000</v>
+        <v>24700000.000000004</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>518</v>
+        <v>547</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
       <c r="C9" s="5">
-        <v>263000000</v>
+        <v>388500000</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" si="0"/>
-        <v>17857142.857142854</v>
+        <f>I9/1.12</f>
+        <v>29464285.714285709</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
-        <v>16071428.571428569</v>
+        <f>D9*90%</f>
+        <v>26517857.142857138</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="2"/>
-        <v>12499999.999999998</v>
-      </c>
-      <c r="G9" s="3">
-        <v>241</v>
+        <f>D9*70%</f>
+        <v>20624999.999999996</v>
+      </c>
+      <c r="G9" s="7">
+        <v>227</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I9" s="12">
-        <v>20000000</v>
+        <v>32999999.999999996</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
       <c r="C10" s="5">
-        <v>217000000</v>
+        <v>447200000</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" si="0"/>
-        <v>11607142.857142856</v>
+        <f>I10/1.12</f>
+        <v>31249999.999999996</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>10446428.571428571</v>
+        <f>D10*90%</f>
+        <v>28124999.999999996</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="2"/>
-        <v>8124999.9999999991</v>
-      </c>
-      <c r="G10" s="3">
-        <v>242</v>
+        <f>D10*70%</f>
+        <v>21874999.999999996</v>
+      </c>
+      <c r="G10" s="7">
+        <v>228</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I10" s="12">
-        <v>13000000</v>
+        <v>35000000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>523</v>
+        <v>496</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="C11" s="5">
-        <v>188300000</v>
+        <v>405000000</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="0"/>
-        <v>11339285.714285715</v>
+        <f>I11/1.12</f>
+        <v>31249999.999999996</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
-        <v>10205357.142857144</v>
+        <f>D11*90%</f>
+        <v>28124999.999999996</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="2"/>
-        <v>7937500</v>
-      </c>
-      <c r="G11" s="3">
-        <v>202</v>
+        <f>D11*70%</f>
+        <v>21874999.999999996</v>
+      </c>
+      <c r="G11" s="7">
+        <v>244</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="I11" s="12">
-        <v>12700000.000000002</v>
+        <v>35000000</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C12" s="5">
-        <v>222850000</v>
+        <v>442000000</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>14285714.285714284</v>
+        <f>I12/1.12</f>
+        <v>33928571.428571425</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>12857142.857142856</v>
+        <f>D12*90%</f>
+        <v>30535714.285714284</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="2"/>
-        <v>9999999.9999999981</v>
-      </c>
-      <c r="G12" s="3">
-        <v>204</v>
+        <f>D12*70%</f>
+        <v>23749999.999999996</v>
+      </c>
+      <c r="G12" s="7">
+        <v>245</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="I12" s="12">
-        <v>16000000</v>
+        <v>38000000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>498</v>
+        <v>517</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="C13" s="5">
-        <v>210700000</v>
+        <v>303000000</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="0"/>
-        <v>13124999.999999998</v>
+        <f>I13/1.12</f>
+        <v>20535714.285714284</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>11812499.999999998</v>
+        <f>D13*90%</f>
+        <v>18482142.857142854</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="2"/>
-        <v>9187499.9999999981</v>
+        <f>D13*70%</f>
+        <v>14374999.999999998</v>
       </c>
       <c r="G13" s="3">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="I13" s="12">
-        <v>14700000</v>
+        <v>23000000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>490</v>
+        <v>533</v>
       </c>
       <c r="C14" s="5">
-        <v>277200000</v>
+        <v>263000000</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" si="0"/>
-        <v>18660714.285714284</v>
+        <f>I14/1.12</f>
+        <v>17857142.857142854</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="1"/>
-        <v>16794642.857142854</v>
+        <f>D14*90%</f>
+        <v>16071428.571428569</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="2"/>
-        <v>13062499.999999998</v>
+        <f>D14*70%</f>
+        <v>12499999.999999998</v>
       </c>
       <c r="G14" s="3">
-        <v>213</v>
+        <v>241</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I14" s="12">
-        <v>20900000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>491</v>
+        <v>534</v>
       </c>
       <c r="C15" s="5">
-        <v>291300000</v>
+        <v>217000000</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="0"/>
-        <v>19642857.142857142</v>
+        <f>I15/1.12</f>
+        <v>11607142.857142856</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
-        <v>17678571.428571429</v>
+        <f>D15*90%</f>
+        <v>10446428.571428571</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="2"/>
-        <v>13749999.999999998</v>
+        <f>D15*70%</f>
+        <v>8124999.9999999991</v>
       </c>
       <c r="G15" s="3">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I15" s="12">
-        <v>22000000</v>
+        <v>13000000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>544</v>
+      <c r="A16" s="22" t="s">
+        <v>611</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>612</v>
       </c>
       <c r="C16" s="5">
-        <v>262500000</v>
+        <v>263000000</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="0"/>
-        <v>16339285.714285713</v>
+        <f>I16/1.12</f>
+        <v>17857142.857142854</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="1"/>
-        <v>14705357.142857142</v>
+        <f>D16*90%</f>
+        <v>16071428.571428569</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="2"/>
-        <v>11437499.999999998</v>
+        <f>D16*70%</f>
+        <v>12499999.999999998</v>
       </c>
       <c r="G16" s="3">
-        <v>209</v>
+        <v>262</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I16" s="12">
-        <v>18300000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>538</v>
+        <v>549</v>
       </c>
       <c r="C17" s="5">
-        <v>285200000</v>
+        <v>353000000</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="0"/>
-        <v>18303571.428571429</v>
+        <f>I17/1.12</f>
+        <v>25892857.142857142</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="1"/>
-        <v>16473214.285714287</v>
+        <f>D17*90%</f>
+        <v>23303571.428571429</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="2"/>
-        <v>12812500</v>
+        <f>D17*70%</f>
+        <v>18124999.999999996</v>
       </c>
       <c r="G17" s="3">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>567</v>
+        <v>576</v>
       </c>
       <c r="I17" s="12">
-        <v>20500000.000000004</v>
+        <v>29000000</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>507</v>
+        <v>583</v>
       </c>
       <c r="C18" s="5">
-        <v>214000000</v>
+        <v>318000000</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="0"/>
-        <v>18750000</v>
+        <f>I18/1.12</f>
+        <v>23214285.714285713</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="1"/>
-        <v>16875000</v>
+        <f>D18*90%</f>
+        <v>20892857.142857142</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="2"/>
-        <v>13125000</v>
+        <f>D18*70%</f>
+        <v>16249999.999999998</v>
       </c>
       <c r="G18" s="3">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="I18" s="12">
-        <v>21000000.000000004</v>
+        <v>26000000</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>555</v>
+        <v>504</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="C19" s="5">
-        <v>251000000</v>
+        <v>363000000</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="0"/>
-        <v>18750000</v>
+        <f>I19/1.12</f>
+        <v>26785714.285714284</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" ref="E19" si="3">D19*90%</f>
-        <v>16875000</v>
+        <f>D19*90%</f>
+        <v>24107142.857142854</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" ref="F19" si="4">D19*70%</f>
-        <v>13125000</v>
+        <f>D19*70%</f>
+        <v>18749999.999999996</v>
       </c>
       <c r="G19" s="3">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="I19" s="12">
-        <v>21000000.000000004</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>500</v>
+        <v>588</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>556</v>
+        <v>584</v>
       </c>
       <c r="C20" s="5">
-        <v>251000000</v>
+        <v>363000000</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="0"/>
-        <v>18750000</v>
+        <f>I20/1.12</f>
+        <v>25892857.142857142</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="1"/>
-        <v>16875000</v>
+        <f>D20*90%</f>
+        <v>23303571.428571429</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" si="2"/>
-        <v>13125000</v>
+        <f>D20*70%</f>
+        <v>18124999.999999996</v>
       </c>
       <c r="G20" s="3">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="I20" s="12">
-        <v>21000000.000000004</v>
+        <v>29000000</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>501</v>
+        <v>587</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>508</v>
+        <v>584</v>
       </c>
       <c r="C21" s="5">
-        <v>251000000</v>
+        <v>363000000</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="0"/>
-        <v>18750000</v>
+        <f>I21/1.12</f>
+        <v>25892857.142857142</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="1"/>
-        <v>16875000</v>
+        <f>D21*90%</f>
+        <v>23303571.428571429</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="2"/>
-        <v>13125000</v>
+        <f>D21*70%</f>
+        <v>18124999.999999996</v>
       </c>
       <c r="G21" s="3">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="I21" s="12">
-        <v>21000000.000000004</v>
+        <v>29000000</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C22" s="5">
-        <v>307500000</v>
+        <v>413000000</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="0"/>
-        <v>22321428.571428567</v>
+        <f>I22/1.12</f>
+        <v>30357142.857142854</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="1"/>
-        <v>20089285.714285713</v>
+        <f>D22*90%</f>
+        <v>27321428.571428571</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="2"/>
-        <v>15624999.999999996</v>
+        <f>D22*70%</f>
+        <v>21249999.999999996</v>
       </c>
       <c r="G22" s="3">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="I22" s="12">
-        <v>24999999.999999996</v>
+        <v>34000000</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>503</v>
+        <v>558</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>549</v>
+        <v>512</v>
       </c>
       <c r="C23" s="5">
-        <v>353000000</v>
+        <v>443000000</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="0"/>
-        <v>25892857.142857142</v>
+        <f>I23/1.12</f>
+        <v>33035714.285714284</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="1"/>
-        <v>23303571.428571429</v>
+        <f>D23*90%</f>
+        <v>29732142.857142854</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="2"/>
-        <v>18124999.999999996</v>
+        <f>D23*70%</f>
+        <v>23124999.999999996</v>
       </c>
       <c r="G23" s="3">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="I23" s="12">
-        <v>29000000</v>
+        <v>37000000</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C24" s="5">
-        <v>363000000</v>
+        <v>443000000</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" si="0"/>
-        <v>26785714.285714284</v>
+        <f>I24/1.12</f>
+        <v>33035714.285714284</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="1"/>
-        <v>24107142.857142854</v>
+        <f>D24*90%</f>
+        <v>29732142.857142854</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="2"/>
-        <v>18749999.999999996</v>
+        <f>D24*70%</f>
+        <v>23124999.999999996</v>
       </c>
       <c r="G24" s="3">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="I24" s="12">
-        <v>30000000</v>
+        <v>37000000</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
-        <v>588</v>
+        <v>561</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>584</v>
+        <v>512</v>
       </c>
       <c r="C25" s="5">
-        <v>363000000</v>
+        <v>443000000</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" ref="D25" si="5">I25/1.12</f>
-        <v>25892857.142857142</v>
+        <f>I25/1.12</f>
+        <v>33035714.285714284</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="1"/>
-        <v>23303571.428571429</v>
+        <f>D25*90%</f>
+        <v>29732142.857142854</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="2"/>
-        <v>18124999.999999996</v>
+        <f>D25*70%</f>
+        <v>23124999.999999996</v>
       </c>
       <c r="G25" s="3">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="I25" s="12">
-        <v>29000000</v>
+        <v>37000000</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>505</v>
+        <v>557</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>511</v>
+        <v>559</v>
       </c>
       <c r="C26" s="5">
-        <v>413000000</v>
+        <v>415000000</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" si="0"/>
-        <v>30357142.857142854</v>
+        <f>I26/1.12</f>
+        <v>33035714.285714284</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="1"/>
-        <v>27321428.571428571</v>
+        <f>D26*90%</f>
+        <v>29732142.857142854</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="2"/>
-        <v>21249999.999999996</v>
+        <f>D26*70%</f>
+        <v>23124999.999999996</v>
       </c>
       <c r="G26" s="3">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="I26" s="12">
-        <v>34000000</v>
+        <v>37000000</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>583</v>
+        <v>559</v>
       </c>
       <c r="C27" s="5">
-        <v>318000000</v>
+        <v>415000000</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="0"/>
-        <v>23214285.714285713</v>
+        <f>I27/1.12</f>
+        <v>33035714.285714284</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" ref="E27:E28" si="6">D27*90%</f>
-        <v>20892857.142857142</v>
+        <f>D27*90%</f>
+        <v>29732142.857142854</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" ref="F27:F28" si="7">D27*70%</f>
-        <v>16249999.999999998</v>
+        <f>D27*70%</f>
+        <v>23124999.999999996</v>
       </c>
       <c r="G27" s="3">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="I27" s="12">
-        <v>26000000</v>
+        <v>37000000</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>587</v>
+        <v>523</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>584</v>
+        <v>535</v>
       </c>
       <c r="C28" s="5">
-        <v>363000000</v>
+        <v>188300000</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="0"/>
-        <v>25892857.142857142</v>
+        <f>I28/1.12</f>
+        <v>11339285.714285715</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="6"/>
-        <v>23303571.428571429</v>
+        <f>D28*90%</f>
+        <v>10205357.142857144</v>
       </c>
       <c r="F28" s="5">
-        <f t="shared" si="7"/>
-        <v>18124999.999999996</v>
+        <f>D28*70%</f>
+        <v>7937500</v>
       </c>
       <c r="G28" s="3">
-        <v>253</v>
+        <v>202</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="I28" s="12">
-        <v>29000000</v>
+        <v>12700000.000000002</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>559</v>
+        <v>535</v>
       </c>
       <c r="C29" s="5">
-        <v>415000000</v>
+        <v>188300000</v>
       </c>
       <c r="D29" s="5">
-        <f t="shared" si="0"/>
-        <v>33035714.285714284</v>
+        <f>I29/1.12</f>
+        <v>11339285.714285715</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="1"/>
-        <v>29732142.857142854</v>
+        <f>D29*90%</f>
+        <v>10205357.142857144</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="2"/>
-        <v>23124999.999999996</v>
+        <f>D29*70%</f>
+        <v>7937500</v>
       </c>
       <c r="G29" s="3">
-        <v>251</v>
+        <v>202</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="I29" s="12">
-        <v>37000000</v>
+        <v>12700000.000000002</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>582</v>
+        <v>524</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>559</v>
+        <v>536</v>
       </c>
       <c r="C30" s="5">
-        <v>415000000</v>
+        <v>222850000</v>
       </c>
       <c r="D30" s="5">
-        <f t="shared" si="0"/>
-        <v>33035714.285714284</v>
+        <f>I30/1.12</f>
+        <v>14285714.285714284</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" ref="E30" si="8">D30*90%</f>
-        <v>29732142.857142854</v>
+        <f>D30*90%</f>
+        <v>12857142.857142856</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" ref="F30" si="9">D30*70%</f>
-        <v>23124999.999999996</v>
+        <f>D30*70%</f>
+        <v>9999999.9999999981</v>
       </c>
       <c r="G30" s="3">
-        <v>251</v>
+        <v>204</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="I30" s="12">
-        <v>37000000</v>
+        <v>16000000</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>558</v>
+        <v>498</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>512</v>
+        <v>537</v>
       </c>
       <c r="C31" s="5">
-        <v>443000000</v>
+        <v>210700000</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" si="0"/>
-        <v>33035714.285714284</v>
+        <f>I31/1.12</f>
+        <v>13124999.999999998</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" ref="E31" si="10">D31*90%</f>
-        <v>29732142.857142854</v>
+        <f>D31*90%</f>
+        <v>11812499.999999998</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" ref="F31" si="11">D31*70%</f>
-        <v>23124999.999999996</v>
+        <f>D31*70%</f>
+        <v>9187499.9999999981</v>
       </c>
       <c r="G31" s="3">
-        <v>249</v>
+        <v>205</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="I31" s="12">
-        <v>37000000</v>
+        <v>14700000</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>506</v>
+        <v>525</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>512</v>
+        <v>544</v>
       </c>
       <c r="C32" s="5">
-        <v>443000000</v>
+        <v>262500000</v>
       </c>
       <c r="D32" s="5">
-        <f t="shared" si="0"/>
-        <v>33035714.285714284</v>
+        <f>I32/1.12</f>
+        <v>16339285.714285713</v>
       </c>
       <c r="E32" s="5">
         <f>D32*90%</f>
-        <v>29732142.857142854</v>
+        <v>14705357.142857142</v>
       </c>
       <c r="F32" s="5">
         <f>D32*70%</f>
-        <v>23124999.999999996</v>
+        <v>11437499.999999998</v>
       </c>
       <c r="G32" s="3">
-        <v>249</v>
+        <v>209</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="I32" s="12">
-        <v>37000000</v>
+        <v>18300000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>539</v>
+        <v>490</v>
       </c>
       <c r="C33" s="5">
-        <v>155700000</v>
+        <v>277200000</v>
       </c>
       <c r="D33" s="5">
-        <f t="shared" si="0"/>
-        <v>10892857.142857142</v>
+        <f>I33/1.12</f>
+        <v>18660714.285714284</v>
       </c>
       <c r="E33" s="5">
         <f>D33*90%</f>
-        <v>9803571.4285714272</v>
+        <v>16794642.857142854</v>
       </c>
       <c r="F33" s="5">
         <f>D33*70%</f>
-        <v>7624999.9999999991</v>
+        <v>13062499.999999998</v>
       </c>
       <c r="G33" s="3">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="I33" s="12">
-        <v>12200000</v>
+        <v>20900000</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>513</v>
+        <v>491</v>
       </c>
       <c r="C34" s="5">
-        <v>172600000</v>
+        <v>291300000</v>
       </c>
       <c r="D34" s="5">
-        <f t="shared" si="0"/>
-        <v>7142857.1428571418</v>
+        <f>I34/1.12</f>
+        <v>19642857.142857142</v>
       </c>
       <c r="E34" s="5">
         <f>D34*90%</f>
-        <v>6428571.4285714282</v>
+        <v>17678571.428571429</v>
       </c>
       <c r="F34" s="5">
         <f>D34*70%</f>
-        <v>4999999.9999999991</v>
+        <v>13749999.999999998</v>
       </c>
       <c r="G34" s="3">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="I34" s="12">
-        <v>8000000</v>
+        <v>22000000</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
-        <v>521</v>
+        <v>499</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C35" s="5">
-        <v>176000000</v>
+        <v>285200000</v>
       </c>
       <c r="D35" s="5">
-        <f t="shared" si="0"/>
-        <v>12053571.428571427</v>
+        <f>I35/1.12</f>
+        <v>18303571.428571429</v>
       </c>
       <c r="E35" s="5">
         <f>D35*90%</f>
-        <v>10848214.285714285</v>
+        <v>16473214.285714287</v>
       </c>
       <c r="F35" s="5">
         <f>D35*70%</f>
-        <v>8437499.9999999981</v>
+        <v>12812500</v>
       </c>
       <c r="G35" s="3">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="I35" s="12">
-        <v>13500000</v>
+        <v>20500000.000000004</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="10" t="s">
-        <v>526</v>
+      <c r="A36" s="11" t="s">
+        <v>522</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="C36" s="5">
-        <v>168000000</v>
+        <v>345650000</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="0"/>
-        <v>11160714.285714284</v>
+        <f>I36/1.12</f>
+        <v>22857142.857142854</v>
       </c>
       <c r="E36" s="5">
         <f>D36*90%</f>
-        <v>10044642.857142856</v>
+        <v>20571428.571428571</v>
       </c>
       <c r="F36" s="5">
         <f>D36*70%</f>
-        <v>7812499.9999999981</v>
+        <v>15999999.999999996</v>
       </c>
       <c r="G36" s="3">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="I36" s="12">
-        <v>12499999.999999998</v>
+        <v>25600000</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="10" t="s">
-        <v>560</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="C37" s="5">
-        <v>188300000</v>
+      <c r="A37" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>613</v>
+      </c>
+      <c r="C37" s="9">
+        <v>307300000</v>
       </c>
       <c r="D37" s="5">
-        <f t="shared" si="0"/>
-        <v>11339285.714285715</v>
+        <f>I37/1.12</f>
+        <v>19999999.999999996</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" ref="E37:E38" si="12">D37*90%</f>
-        <v>10205357.142857144</v>
+        <f>D37*90%</f>
+        <v>17999999.999999996</v>
       </c>
       <c r="F37" s="5">
-        <f t="shared" ref="F37:F38" si="13">D37*70%</f>
-        <v>7937500</v>
-      </c>
-      <c r="G37" s="3">
-        <v>202</v>
+        <f>D37*70%</f>
+        <v>13999999.999999996</v>
+      </c>
+      <c r="G37" s="4">
+        <v>210</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="I37" s="12">
-        <v>12700000.000000002</v>
+        <v>567</v>
+      </c>
+      <c r="I37" s="24">
+        <v>22400000</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
-        <v>561</v>
+        <v>608</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="C38" s="5">
-        <v>443000000</v>
-      </c>
-      <c r="D38" s="5">
-        <f t="shared" si="0"/>
-        <v>33035714.285714284</v>
-      </c>
-      <c r="E38" s="5">
-        <f t="shared" si="12"/>
-        <v>29732142.857142854</v>
-      </c>
-      <c r="F38" s="5">
-        <f t="shared" si="13"/>
-        <v>23124999.999999996</v>
-      </c>
-      <c r="G38" s="3">
-        <v>249</v>
+        <v>597</v>
+      </c>
+      <c r="C38" s="9">
+        <v>399000000</v>
+      </c>
+      <c r="D38" s="9">
+        <f>I38/1.12</f>
+        <v>28214285.714285713</v>
+      </c>
+      <c r="E38" s="9">
+        <f>D38*90%</f>
+        <v>25392857.142857142</v>
+      </c>
+      <c r="F38" s="9">
+        <f>D38*70%</f>
+        <v>19749999.999999996</v>
+      </c>
+      <c r="G38" s="20">
+        <v>258</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>571</v>
+        <v>597</v>
       </c>
       <c r="I38" s="12">
-        <v>37000000</v>
+        <v>31600000</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
-        <v>522</v>
+      <c r="A39" s="10" t="s">
+        <v>599</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>550</v>
-      </c>
-      <c r="C39" s="5">
-        <v>345650000</v>
-      </c>
-      <c r="D39" s="5">
-        <f t="shared" si="0"/>
-        <v>22857142.857142854</v>
-      </c>
-      <c r="E39" s="5">
-        <f t="shared" ref="E39:E42" si="14">D39*90%</f>
-        <v>20571428.571428571</v>
-      </c>
-      <c r="F39" s="5">
-        <f t="shared" ref="F39:F42" si="15">D39*70%</f>
-        <v>15999999.999999996</v>
-      </c>
-      <c r="G39" s="3">
-        <v>233</v>
+        <v>598</v>
+      </c>
+      <c r="C39" s="9">
+        <v>459000000</v>
+      </c>
+      <c r="D39" s="9">
+        <f>I39/1.12</f>
+        <v>32499999.999999996</v>
+      </c>
+      <c r="E39" s="9">
+        <f>D39*90%</f>
+        <v>29249999.999999996</v>
+      </c>
+      <c r="F39" s="9">
+        <f>D39*70%</f>
+        <v>22749999.999999996</v>
+      </c>
+      <c r="G39" s="20">
+        <v>259</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>567</v>
+        <v>598</v>
       </c>
       <c r="I39" s="12">
-        <v>25600000</v>
+        <v>36400000</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
       <c r="C40" s="9">
-        <v>328000000</v>
+        <v>449000000</v>
       </c>
       <c r="D40" s="9">
-        <f t="shared" si="0"/>
-        <v>17857142.857142854</v>
+        <f>I40/1.12</f>
+        <v>29196428.571428567</v>
       </c>
       <c r="E40" s="9">
-        <f t="shared" si="14"/>
-        <v>16071428.571428569</v>
+        <f>D40*90%</f>
+        <v>26276785.714285713</v>
       </c>
       <c r="F40" s="9">
-        <f t="shared" si="15"/>
-        <v>12499999.999999998</v>
+        <f>D40*70%</f>
+        <v>20437499.999999996</v>
       </c>
       <c r="G40" s="20">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
       <c r="I40" s="12">
-        <v>20000000</v>
+        <v>32700000</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
       <c r="C41" s="9">
-        <v>348000000</v>
+        <v>499000000</v>
       </c>
       <c r="D41" s="9">
-        <f t="shared" si="0"/>
-        <v>17857142.857142854</v>
+        <f>I41/1.12</f>
+        <v>32499999.999999996</v>
       </c>
       <c r="E41" s="9">
-        <f t="shared" si="14"/>
-        <v>16071428.571428569</v>
+        <f>D41*90%</f>
+        <v>29249999.999999996</v>
       </c>
       <c r="F41" s="9">
-        <f t="shared" si="15"/>
-        <v>12499999.999999998</v>
+        <f>D41*70%</f>
+        <v>22749999.999999996</v>
       </c>
       <c r="G41" s="20">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="I41" s="12">
-        <v>20000000</v>
+        <v>36400000</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
-        <v>595</v>
+        <v>526</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>591</v>
-      </c>
-      <c r="C42" s="9">
-        <v>358000000</v>
-      </c>
-      <c r="D42" s="9">
-        <f t="shared" si="0"/>
-        <v>22321428.571428571</v>
-      </c>
-      <c r="E42" s="9">
-        <f t="shared" si="14"/>
-        <v>20089285.714285713</v>
-      </c>
-      <c r="F42" s="9">
-        <f t="shared" si="15"/>
-        <v>15624999.999999998</v>
-      </c>
-      <c r="G42" s="20">
-        <v>255</v>
+        <v>545</v>
+      </c>
+      <c r="C42" s="5">
+        <v>168000000</v>
+      </c>
+      <c r="D42" s="5">
+        <f>I42/1.12</f>
+        <v>11160714.285714284</v>
+      </c>
+      <c r="E42" s="5">
+        <f>D42*90%</f>
+        <v>10044642.857142856</v>
+      </c>
+      <c r="F42" s="5">
+        <f>D42*70%</f>
+        <v>7812499.9999999981</v>
+      </c>
+      <c r="G42" s="3">
+        <v>237</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>595</v>
+        <v>579</v>
       </c>
       <c r="I42" s="12">
-        <v>25000000</v>
+        <v>12499999.999999998</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
-        <v>596</v>
+        <v>521</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>592</v>
-      </c>
-      <c r="C43" s="18">
-        <v>378000000</v>
-      </c>
-      <c r="D43" s="9">
-        <f t="shared" ref="D43:D50" si="16">I43/1.12</f>
-        <v>22321428.571428571</v>
-      </c>
-      <c r="E43" s="9">
-        <f t="shared" ref="E43:E50" si="17">D43*90%</f>
-        <v>20089285.714285713</v>
-      </c>
-      <c r="F43" s="9">
-        <f t="shared" ref="F43:F50" si="18">D43*70%</f>
-        <v>15624999.999999998</v>
-      </c>
-      <c r="G43" s="21">
-        <v>257</v>
+        <v>540</v>
+      </c>
+      <c r="C43" s="26">
+        <v>176000000</v>
+      </c>
+      <c r="D43" s="5">
+        <f>I43/1.12</f>
+        <v>12053571.428571427</v>
+      </c>
+      <c r="E43" s="5">
+        <f>D43*90%</f>
+        <v>10848214.285714285</v>
+      </c>
+      <c r="F43" s="5">
+        <f>D43*70%</f>
+        <v>8437499.9999999981</v>
+      </c>
+      <c r="G43" s="27">
+        <v>238</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>596</v>
+        <v>579</v>
       </c>
       <c r="I43" s="19">
-        <v>25000000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>608</v>
+        <v>529</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="C44" s="9">
-        <v>399000000</v>
-      </c>
-      <c r="D44" s="9">
-        <f t="shared" si="16"/>
-        <v>28214285.714285713</v>
-      </c>
-      <c r="E44" s="9">
-        <f t="shared" si="17"/>
-        <v>25392857.142857142</v>
-      </c>
-      <c r="F44" s="9">
-        <f t="shared" si="18"/>
-        <v>19749999.999999996</v>
-      </c>
-      <c r="G44" s="20">
-        <v>258</v>
+        <v>539</v>
+      </c>
+      <c r="C44" s="5">
+        <v>155700000</v>
+      </c>
+      <c r="D44" s="5">
+        <f>I44/1.12</f>
+        <v>10892857.142857142</v>
+      </c>
+      <c r="E44" s="5">
+        <f>D44*90%</f>
+        <v>9803571.4285714272</v>
+      </c>
+      <c r="F44" s="5">
+        <f>D44*70%</f>
+        <v>7624999.9999999991</v>
+      </c>
+      <c r="G44" s="3">
+        <v>201</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>597</v>
+        <v>572</v>
       </c>
       <c r="I44" s="12">
-        <v>31600000</v>
+        <v>12200000</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>598</v>
+        <v>610</v>
       </c>
       <c r="C45" s="9">
-        <v>459000000</v>
+        <v>167800000</v>
       </c>
       <c r="D45" s="9">
-        <f t="shared" si="16"/>
-        <v>32499999.999999996</v>
+        <f>I45/1.12</f>
+        <v>7142857.1428571418</v>
       </c>
       <c r="E45" s="9">
-        <f t="shared" si="17"/>
-        <v>29249999.999999996</v>
+        <f>D45*90%</f>
+        <v>6428571.4285714282</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" si="18"/>
-        <v>22749999.999999996</v>
+        <f>D45*70%</f>
+        <v>4999999.9999999991</v>
       </c>
       <c r="G45" s="20">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="I45" s="12">
-        <v>36400000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>601</v>
+        <v>520</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="C46" s="9">
-        <v>449000000</v>
-      </c>
-      <c r="D46" s="9">
-        <f t="shared" si="16"/>
-        <v>29196428.571428567</v>
-      </c>
-      <c r="E46" s="9">
-        <f t="shared" si="17"/>
-        <v>26276785.714285713</v>
-      </c>
-      <c r="F46" s="9">
-        <f t="shared" si="18"/>
-        <v>20437499.999999996</v>
-      </c>
-      <c r="G46" s="20">
-        <v>260</v>
+        <v>513</v>
+      </c>
+      <c r="C46" s="5">
+        <v>172600000</v>
+      </c>
+      <c r="D46" s="5">
+        <f>I46/1.12</f>
+        <v>7142857.1428571418</v>
+      </c>
+      <c r="E46" s="5">
+        <f>D46*90%</f>
+        <v>6428571.4285714282</v>
+      </c>
+      <c r="F46" s="5">
+        <f>D46*70%</f>
+        <v>4999999.9999999991</v>
+      </c>
+      <c r="G46" s="3">
+        <v>230</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>600</v>
+        <v>572</v>
       </c>
       <c r="I46" s="12">
-        <v>32700000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="C47" s="18">
-        <v>499000000</v>
+        <v>328000000</v>
       </c>
       <c r="D47" s="18">
-        <f t="shared" si="16"/>
-        <v>32499999.999999996</v>
+        <f>I47/1.12</f>
+        <v>17857142.857142854</v>
       </c>
       <c r="E47" s="18">
-        <f t="shared" si="17"/>
-        <v>29249999.999999996</v>
+        <f>D47*90%</f>
+        <v>16071428.571428569</v>
       </c>
       <c r="F47" s="18">
-        <f t="shared" si="18"/>
-        <v>22749999.999999996</v>
+        <f>D47*70%</f>
+        <v>12499999.999999998</v>
       </c>
       <c r="G47" s="21">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="I47" s="19">
-        <v>36400000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -7187,11 +7208,11 @@
         <v>17857142.857142854</v>
       </c>
       <c r="E48" s="9">
-        <f t="shared" si="17"/>
+        <f>D48*90%</f>
         <v>16071428.571428569</v>
       </c>
       <c r="F48" s="9">
-        <f t="shared" si="18"/>
+        <f>D48*70%</f>
         <v>12499999.999999998</v>
       </c>
       <c r="G48" s="20">
@@ -7206,34 +7227,34 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C49" s="9">
-        <v>348000000</v>
+        <v>358000000</v>
       </c>
       <c r="D49" s="9">
-        <f t="shared" si="16"/>
-        <v>17857142.857142854</v>
+        <f>I49/1.12</f>
+        <v>22321428.571428571</v>
       </c>
       <c r="E49" s="9">
-        <f t="shared" si="17"/>
-        <v>16071428.571428569</v>
+        <f>D49*90%</f>
+        <v>20089285.714285713</v>
       </c>
       <c r="F49" s="9">
-        <f t="shared" si="18"/>
-        <v>12499999.999999998</v>
+        <f>D49*70%</f>
+        <v>15624999.999999998</v>
       </c>
       <c r="G49" s="20">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="I49" s="12">
-        <v>20000000</v>
+        <v>25000000</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
@@ -7247,15 +7268,15 @@
         <v>358000000</v>
       </c>
       <c r="D50" s="9">
-        <f t="shared" si="16"/>
+        <f>I50/1.12</f>
         <v>22321428.571428571</v>
       </c>
       <c r="E50" s="9">
-        <f t="shared" si="17"/>
+        <f>D50*90%</f>
         <v>20089285.714285713</v>
       </c>
       <c r="F50" s="9">
-        <f t="shared" si="18"/>
+        <f>D50*70%</f>
         <v>15624999.999999998</v>
       </c>
       <c r="G50" s="20">
@@ -7270,85 +7291,149 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>590</v>
+      </c>
+      <c r="C51" s="18">
+        <v>348000000</v>
+      </c>
+      <c r="D51" s="18">
+        <f>I51/1.12</f>
+        <v>17857142.857142854</v>
+      </c>
+      <c r="E51" s="18">
+        <f>D51*90%</f>
+        <v>16071428.571428569</v>
+      </c>
+      <c r="F51" s="18">
+        <f>D51*70%</f>
+        <v>12499999.999999998</v>
+      </c>
+      <c r="G51" s="21">
+        <v>256</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="I51" s="19">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="16" t="s">
+        <v>606</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C52" s="18">
+        <v>348000000</v>
+      </c>
+      <c r="D52" s="18">
+        <f>I52/1.12</f>
+        <v>17857142.857142854</v>
+      </c>
+      <c r="E52" s="18">
+        <f>D52*90%</f>
+        <v>16071428.571428569</v>
+      </c>
+      <c r="F52" s="18">
+        <f>D52*70%</f>
+        <v>12499999.999999998</v>
+      </c>
+      <c r="G52" s="21">
+        <v>256</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="I52" s="12">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="16" t="s">
+        <v>596</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>592</v>
+      </c>
+      <c r="C53" s="9">
+        <v>378000000</v>
+      </c>
+      <c r="D53" s="9">
+        <f>I53/1.12</f>
+        <v>22321428.571428571</v>
+      </c>
+      <c r="E53" s="9">
+        <f>D53*90%</f>
+        <v>20089285.714285713</v>
+      </c>
+      <c r="F53" s="9">
+        <f>D53*70%</f>
+        <v>15624999.999999998</v>
+      </c>
+      <c r="G53" s="20">
+        <v>257</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="I53" s="12">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B54" s="17" t="s">
         <v>592</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C54" s="18">
         <v>378000000</v>
       </c>
-      <c r="D51" s="18">
-        <f t="shared" ref="D51:D52" si="19">I51/1.12</f>
+      <c r="D54" s="9">
+        <f>I54/1.12</f>
         <v>22321428.571428571</v>
       </c>
-      <c r="E51" s="18">
-        <f t="shared" ref="E51" si="20">D51*90%</f>
+      <c r="E54" s="9">
+        <f>D54*90%</f>
         <v>20089285.714285713</v>
       </c>
-      <c r="F51" s="18">
-        <f t="shared" ref="F51" si="21">D51*70%</f>
+      <c r="F54" s="9">
+        <f>D54*70%</f>
         <v>15624999.999999998</v>
       </c>
-      <c r="G51" s="21">
+      <c r="G54" s="21">
         <v>257</v>
       </c>
-      <c r="H51" s="17" t="s">
+      <c r="H54" s="17" t="s">
         <v>596</v>
       </c>
-      <c r="I51" s="19">
+      <c r="I54" s="19">
         <v>25000000</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="22" t="s">
-        <v>609</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="C52" s="18">
-        <v>167800000</v>
-      </c>
-      <c r="D52" s="18">
-        <f t="shared" ref="D52" si="22">I52/1.12</f>
-        <v>7142857.1428571418</v>
-      </c>
-      <c r="E52" s="18">
-        <f t="shared" ref="E52" si="23">D52*90%</f>
-        <v>6428571.4285714282</v>
-      </c>
-      <c r="F52" s="18">
-        <f t="shared" ref="F52" si="24">D52*70%</f>
-        <v>4999999.9999999991</v>
-      </c>
-      <c r="G52" s="21">
-        <v>229</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="I52" s="12">
-        <v>8000000</v>
-      </c>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2:A29 A31:A43">
-    <cfRule type="duplicateValues" dxfId="8" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A38 A2:A29 A40:A43">
-    <cfRule type="duplicateValues" dxfId="7" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:H43">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48:H51">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>